<commit_message>
Dot color changed to blue
</commit_message>
<xml_diff>
--- a/development/Integrated Mods.xlsx
+++ b/development/Integrated Mods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\S.T.A.L.K.E.R\Anomaly Mods\mods\Back-to-roots-wip\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E334E7-0E4B-4085-B0D6-919B8BF92B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFAF6C2-E122-4392-817D-7FCE2C78577F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14700" windowHeight="15600" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
   </bookViews>
@@ -155,20 +155,27 @@
     <t>map_spots.xml</t>
   </si>
   <si>
-    <t>Soon</t>
-  </si>
-  <si>
     <t>ui_st_zver_map.xml</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -296,9 +303,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -311,14 +318,15 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -657,7 +665,7 @@
   <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,8 +1028,8 @@
       <c r="C21" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>39</v>
+      <c r="D21" s="20" t="s">
+        <v>40</v>
       </c>
       <c r="E21" s="17" t="s">
         <v>17</v>
@@ -1066,7 +1074,7 @@
         <v>29</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>27</v>
@@ -1083,7 +1091,7 @@
         <v>29</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Integrated Return Menu Music
</commit_message>
<xml_diff>
--- a/development/Integrated Mods.xlsx
+++ b/development/Integrated Mods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\S.T.A.L.K.E.R\Anomaly Mods\mods\Back-to-roots-wip\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFAF6C2-E122-4392-817D-7FCE2C78577F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B27275A-3E4E-427A-829D-C910BC7FA1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14700" windowHeight="15600" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="44">
   <si>
     <t>Filename</t>
   </si>
@@ -159,6 +159,15 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Menu Music</t>
+  </si>
+  <si>
+    <t>Mirrowel</t>
+  </si>
+  <si>
+    <t>return_menu_music.script</t>
   </si>
 </sst>
 </file>
@@ -665,7 +674,7 @@
   <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,11 +1113,21 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="18"/>
+      <c r="A26" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
@@ -1514,6 +1533,7 @@
     <hyperlink ref="A23" r:id="rId22" xr:uid="{3F3B0406-D67A-47AA-8FC9-B5287B0EF720}"/>
     <hyperlink ref="A25" r:id="rId23" xr:uid="{94557B4D-1AC3-4BB5-A1A0-85583F61062C}"/>
     <hyperlink ref="A24" r:id="rId24" xr:uid="{08B015F2-443A-4B2E-BE3E-59CDB6D7E12B}"/>
+    <hyperlink ref="A26" r:id="rId25" xr:uid="{8AC3304D-47D0-4E90-A162-34FFE64C55E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Integrated Dynamic Dialogue UI
</commit_message>
<xml_diff>
--- a/development/Integrated Mods.xlsx
+++ b/development/Integrated Mods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\S.T.A.L.K.E.R\Anomaly Mods\mods\Back-to-roots-wip\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E5D698-5033-4111-A8A6-A996521739CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B259D77-EE17-40FF-8DF4-469F41A5B806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21210" windowHeight="15600" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="77">
   <si>
     <t>Filename</t>
   </si>
@@ -246,6 +246,27 @@
   </si>
   <si>
     <t>VERSIONS/</t>
+  </si>
+  <si>
+    <t>Dynamic Dialogue UI</t>
+  </si>
+  <si>
+    <t>TheMrDemonized</t>
+  </si>
+  <si>
+    <t>ui_st_dialog_fov_mcm.xml</t>
+  </si>
+  <si>
+    <t>talk.xml</t>
+  </si>
+  <si>
+    <t>talk_16.xml</t>
+  </si>
+  <si>
+    <t>dialog_fov.script</t>
+  </si>
+  <si>
+    <t>dialog_fov_mcm.script</t>
   </si>
 </sst>
 </file>
@@ -789,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8700934C-DA8F-46A3-9CCC-A5B0203FB02B}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1535,46 +1556,106 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="15"/>
+      <c r="A44" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="14"/>
+      <c r="A45" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="15"/>
+      <c r="A46" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="14"/>
+      <c r="A47" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="15"/>
+      <c r="A48" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="14"/>
+      <c r="A49" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
@@ -1800,43 +1881,49 @@
     <hyperlink ref="A4" r:id="rId3" xr:uid="{6DC9B457-A97D-43C1-B925-29BBAE81D28D}"/>
     <hyperlink ref="A5" r:id="rId4" xr:uid="{0CEEAA07-CCE4-482B-A880-7BF042506AFE}"/>
     <hyperlink ref="A6" r:id="rId5" xr:uid="{3EDA65A1-1DC5-4B24-BB1B-A2B13113E508}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{90A4084C-1C66-481C-8C11-1D8A49E39DCE}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{3C304BA4-FD5F-4CEA-B9E6-6E33A7194879}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{69D90315-5075-44B3-85E5-22F587F37757}"/>
-    <hyperlink ref="A11" r:id="rId9" xr:uid="{CEC2B5C2-1BD9-496E-A9FD-F1191ABC1C68}"/>
-    <hyperlink ref="A13" r:id="rId10" xr:uid="{0B7DBD26-E04E-4D51-A9B2-7825102B3C9C}"/>
-    <hyperlink ref="A10" r:id="rId11" xr:uid="{0853AEA1-3ED0-4522-9249-5ABE3A7CAB1E}"/>
-    <hyperlink ref="A12" r:id="rId12" xr:uid="{3F565B56-28C2-4696-B9FD-6A7374A07144}"/>
-    <hyperlink ref="A14" r:id="rId13" xr:uid="{7417E636-5018-4213-B7A7-56D7326D2B8E}"/>
-    <hyperlink ref="A15" r:id="rId14" xr:uid="{3C431D88-C5CA-4118-AA9B-19370BBDC948}"/>
-    <hyperlink ref="A16" r:id="rId15" xr:uid="{2BBD4D12-9A1D-4E02-BEEE-0EB9C4EDE997}"/>
-    <hyperlink ref="A18" r:id="rId16" xr:uid="{8C20C878-EAD2-4A3A-BCB6-519E8C153083}"/>
-    <hyperlink ref="A20" r:id="rId17" xr:uid="{7EB06454-3C4D-40CF-93E9-D82036CA9954}"/>
-    <hyperlink ref="A22" r:id="rId18" xr:uid="{886211A2-9E3B-4A21-BFD0-0E12AE7EFB2C}"/>
-    <hyperlink ref="A17" r:id="rId19" xr:uid="{B7EE9BAB-ED56-455F-B92A-27FA6759A85B}"/>
-    <hyperlink ref="A19" r:id="rId20" xr:uid="{4B6558AD-89E7-452C-97A2-FE459AACD2D2}"/>
-    <hyperlink ref="A21" r:id="rId21" xr:uid="{D4C60355-B0FB-4A18-9443-9C43834BC7B8}"/>
-    <hyperlink ref="A23" r:id="rId22" xr:uid="{3F3B0406-D67A-47AA-8FC9-B5287B0EF720}"/>
-    <hyperlink ref="A25" r:id="rId23" xr:uid="{94557B4D-1AC3-4BB5-A1A0-85583F61062C}"/>
-    <hyperlink ref="A24" r:id="rId24" xr:uid="{08B015F2-443A-4B2E-BE3E-59CDB6D7E12B}"/>
-    <hyperlink ref="A26" r:id="rId25" xr:uid="{8AC3304D-47D0-4E90-A162-34FFE64C55E4}"/>
-    <hyperlink ref="A27" r:id="rId26" xr:uid="{67434F82-E4BA-4FEA-8F7B-B4A0C40B78E6}"/>
-    <hyperlink ref="A28" r:id="rId27" xr:uid="{6DA97BD3-CC17-403F-B7FF-02F7068EF17B}"/>
-    <hyperlink ref="A29" r:id="rId28" xr:uid="{E7AA11F1-A609-4836-B9BF-13DFAE7D731F}"/>
-    <hyperlink ref="A30" r:id="rId29" xr:uid="{C82EC4B2-2E87-4D62-A803-5967541F5C45}"/>
-    <hyperlink ref="A31" r:id="rId30" xr:uid="{51617730-5764-4AB3-B20B-07520480AAAA}"/>
-    <hyperlink ref="A32" r:id="rId31" xr:uid="{47FFEFD9-016A-4EB2-82E1-F653D4FD39AE}"/>
-    <hyperlink ref="A34" r:id="rId32" xr:uid="{4B409849-CA84-4878-B2FF-A57C7992B888}"/>
-    <hyperlink ref="A36" r:id="rId33" xr:uid="{7FF75CC5-5A26-469D-AB1C-70E19B4316F6}"/>
-    <hyperlink ref="A33" r:id="rId34" xr:uid="{B248F343-0D24-4CEF-96BA-71B832E308C6}"/>
-    <hyperlink ref="A35" r:id="rId35" xr:uid="{D8E230CB-7AEC-4A77-A365-D868FD04D348}"/>
-    <hyperlink ref="A37" r:id="rId36" xr:uid="{BD6D143A-6A15-46A3-A1CC-7CD9D6CA899D}"/>
-    <hyperlink ref="A39" r:id="rId37" xr:uid="{F9C89859-B6BC-4418-9668-A11B86FC207B}"/>
-    <hyperlink ref="A38" r:id="rId38" xr:uid="{AF7A7DA1-2C60-4F6C-9DE0-8D0A22F2F8F4}"/>
-    <hyperlink ref="A40" r:id="rId39" xr:uid="{97547C1D-97C3-4AA8-87D3-E0570D4AA386}"/>
-    <hyperlink ref="A41" r:id="rId40" xr:uid="{90EBA847-6BE3-4A5F-98F9-33A3BFE8AD55}"/>
-    <hyperlink ref="A42" r:id="rId41" xr:uid="{AEB930B8-F348-4B11-9BC6-7E89C9B97A2F}"/>
-    <hyperlink ref="A43" r:id="rId42" xr:uid="{D9DC5DEF-87AC-4F8D-8276-297627A9413C}"/>
+    <hyperlink ref="A14" r:id="rId6" xr:uid="{7417E636-5018-4213-B7A7-56D7326D2B8E}"/>
+    <hyperlink ref="A15" r:id="rId7" xr:uid="{3C431D88-C5CA-4118-AA9B-19370BBDC948}"/>
+    <hyperlink ref="A16" r:id="rId8" xr:uid="{2BBD4D12-9A1D-4E02-BEEE-0EB9C4EDE997}"/>
+    <hyperlink ref="A18" r:id="rId9" xr:uid="{8C20C878-EAD2-4A3A-BCB6-519E8C153083}"/>
+    <hyperlink ref="A20" r:id="rId10" xr:uid="{7EB06454-3C4D-40CF-93E9-D82036CA9954}"/>
+    <hyperlink ref="A22" r:id="rId11" xr:uid="{886211A2-9E3B-4A21-BFD0-0E12AE7EFB2C}"/>
+    <hyperlink ref="A17" r:id="rId12" xr:uid="{B7EE9BAB-ED56-455F-B92A-27FA6759A85B}"/>
+    <hyperlink ref="A19" r:id="rId13" xr:uid="{4B6558AD-89E7-452C-97A2-FE459AACD2D2}"/>
+    <hyperlink ref="A21" r:id="rId14" xr:uid="{D4C60355-B0FB-4A18-9443-9C43834BC7B8}"/>
+    <hyperlink ref="A23" r:id="rId15" xr:uid="{3F3B0406-D67A-47AA-8FC9-B5287B0EF720}"/>
+    <hyperlink ref="A25" r:id="rId16" xr:uid="{94557B4D-1AC3-4BB5-A1A0-85583F61062C}"/>
+    <hyperlink ref="A24" r:id="rId17" xr:uid="{08B015F2-443A-4B2E-BE3E-59CDB6D7E12B}"/>
+    <hyperlink ref="A26" r:id="rId18" xr:uid="{8AC3304D-47D0-4E90-A162-34FFE64C55E4}"/>
+    <hyperlink ref="A27" r:id="rId19" xr:uid="{67434F82-E4BA-4FEA-8F7B-B4A0C40B78E6}"/>
+    <hyperlink ref="A28" r:id="rId20" xr:uid="{6DA97BD3-CC17-403F-B7FF-02F7068EF17B}"/>
+    <hyperlink ref="A29" r:id="rId21" xr:uid="{E7AA11F1-A609-4836-B9BF-13DFAE7D731F}"/>
+    <hyperlink ref="A30" r:id="rId22" xr:uid="{C82EC4B2-2E87-4D62-A803-5967541F5C45}"/>
+    <hyperlink ref="A31" r:id="rId23" xr:uid="{51617730-5764-4AB3-B20B-07520480AAAA}"/>
+    <hyperlink ref="A32" r:id="rId24" xr:uid="{47FFEFD9-016A-4EB2-82E1-F653D4FD39AE}"/>
+    <hyperlink ref="A34" r:id="rId25" xr:uid="{4B409849-CA84-4878-B2FF-A57C7992B888}"/>
+    <hyperlink ref="A36" r:id="rId26" xr:uid="{7FF75CC5-5A26-469D-AB1C-70E19B4316F6}"/>
+    <hyperlink ref="A33" r:id="rId27" xr:uid="{B248F343-0D24-4CEF-96BA-71B832E308C6}"/>
+    <hyperlink ref="A35" r:id="rId28" xr:uid="{D8E230CB-7AEC-4A77-A365-D868FD04D348}"/>
+    <hyperlink ref="A37" r:id="rId29" xr:uid="{BD6D143A-6A15-46A3-A1CC-7CD9D6CA899D}"/>
+    <hyperlink ref="A39" r:id="rId30" xr:uid="{F9C89859-B6BC-4418-9668-A11B86FC207B}"/>
+    <hyperlink ref="A38" r:id="rId31" xr:uid="{AF7A7DA1-2C60-4F6C-9DE0-8D0A22F2F8F4}"/>
+    <hyperlink ref="A40" r:id="rId32" xr:uid="{97547C1D-97C3-4AA8-87D3-E0570D4AA386}"/>
+    <hyperlink ref="A41" r:id="rId33" xr:uid="{90EBA847-6BE3-4A5F-98F9-33A3BFE8AD55}"/>
+    <hyperlink ref="A42" r:id="rId34" xr:uid="{AEB930B8-F348-4B11-9BC6-7E89C9B97A2F}"/>
+    <hyperlink ref="A43" r:id="rId35" xr:uid="{D9DC5DEF-87AC-4F8D-8276-297627A9413C}"/>
+    <hyperlink ref="A44" r:id="rId36" xr:uid="{D33F6994-5A97-46A8-9B3C-5DF835643C25}"/>
+    <hyperlink ref="A8" r:id="rId37" xr:uid="{2D59AB75-03FA-4F2B-96E5-6F2E6F4158C2}"/>
+    <hyperlink ref="A10" r:id="rId38" xr:uid="{49F32376-7630-4C72-84C3-27F16658A30F}"/>
+    <hyperlink ref="A12" r:id="rId39" xr:uid="{F7688210-1E5B-4FBA-89BD-029C6583D26D}"/>
+    <hyperlink ref="A7" r:id="rId40" xr:uid="{F7EC5AEE-79E5-4938-8D0A-7F41572766D4}"/>
+    <hyperlink ref="A9" r:id="rId41" xr:uid="{DAA7C740-B987-4F6D-AAB2-C9DE4B132718}"/>
+    <hyperlink ref="A11" r:id="rId42" xr:uid="{95729464-37DF-40FD-9AA8-37B389C12FD0}"/>
+    <hyperlink ref="A13" r:id="rId43" xr:uid="{A1CB40CF-8E81-410A-B880-E13ED1BEE1C0}"/>
+    <hyperlink ref="A45" r:id="rId44" xr:uid="{514A65D1-F6B9-42FF-9F46-CF61B4BABB73}"/>
+    <hyperlink ref="A46" r:id="rId45" xr:uid="{A64F811F-9AAD-441E-BFD8-BF6A725C9C0B}"/>
+    <hyperlink ref="A47" r:id="rId46" xr:uid="{D425635E-2660-44CA-9C7E-B7FA22046102}"/>
+    <hyperlink ref="A49" r:id="rId47" xr:uid="{C98AC16A-5431-4F8E-A2D1-1D91D98DD1DE}"/>
+    <hyperlink ref="A48" r:id="rId48" xr:uid="{FDC54CF5-7771-49C5-B449-F212EDD30098}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Integrated Utjans Ui Improvements
</commit_message>
<xml_diff>
--- a/development/Integrated Mods.xlsx
+++ b/development/Integrated Mods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\S.T.A.L.K.E.R\Anomaly Mods\mods\Back-to-roots-wip\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B259D77-EE17-40FF-8DF4-469F41A5B806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CF3F7B-75C8-43E7-8C97-9269A1574D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21210" windowHeight="15600" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="93">
   <si>
     <t>Filename</t>
   </si>
@@ -59,6 +59,9 @@
     <t>KalakCZ</t>
   </si>
   <si>
+    <t>configs/ui/textures_descr</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -267,6 +270,51 @@
   </si>
   <si>
     <t>dialog_fov_mcm.script</t>
+  </si>
+  <si>
+    <t>Headlamp anim fix</t>
+  </si>
+  <si>
+    <t>zz_headlamp_animation_fix.script</t>
+  </si>
+  <si>
+    <t>Utjans Item Ui Improvements</t>
+  </si>
+  <si>
+    <t>Utjan</t>
+  </si>
+  <si>
+    <t>configs/plugins/</t>
+  </si>
+  <si>
+    <t>eq_icons_settings.ltx</t>
+  </si>
+  <si>
+    <t>ui_st_item_icon_info.xml</t>
+  </si>
+  <si>
+    <t>ui_dyn_eq_icons.xml</t>
+  </si>
+  <si>
+    <t>ui_utjan_icon_info.xml</t>
+  </si>
+  <si>
+    <t>dynamic_eq_icon.script</t>
+  </si>
+  <si>
+    <t>item_icon_info_mcm.script</t>
+  </si>
+  <si>
+    <t>rax_icon_layers.script</t>
+  </si>
+  <si>
+    <t>z_item_icon_info.script</t>
+  </si>
+  <si>
+    <t>textures/ui/</t>
+  </si>
+  <si>
+    <t>Equipment_icons.dds</t>
   </si>
 </sst>
 </file>
@@ -810,13 +858,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8700934C-DA8F-46A3-9CCC-A5B0203FB02B}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
     <col min="2" max="2" width="34.5703125" style="25" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
@@ -846,13 +894,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>8</v>
-      </c>
       <c r="D2" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>6</v>
@@ -863,13 +911,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>6</v>
@@ -877,865 +925,975 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>14</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>20</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>18</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>28</v>
-      </c>
       <c r="D25" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B26" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B30" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="11" t="s">
-        <v>51</v>
-      </c>
       <c r="D30" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B31" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="14" t="s">
         <v>55</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B32" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="15" t="s">
         <v>55</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C33" s="27" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B44" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="15" t="s">
         <v>72</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="15" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B45" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="14" t="s">
         <v>72</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" s="14" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D49" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C54" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E49" s="14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="19"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="15"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="14"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="15"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="14"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="19"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="15"/>
+      <c r="D54" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="15" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="14"/>
+      <c r="A55" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B55" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="19"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="15"/>
+      <c r="A56" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="15" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="14"/>
+      <c r="A57" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B57" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="19"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="15"/>
+      <c r="A58" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B58" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="15" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="14"/>
+      <c r="A59" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="14" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="19"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="15"/>
+      <c r="A60" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B60" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="15" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
+      <c r="A61" s="13"/>
       <c r="B61" s="20"/>
       <c r="C61" s="10"/>
       <c r="D61" s="3"/>
@@ -1924,6 +2082,17 @@
     <hyperlink ref="A47" r:id="rId46" xr:uid="{D425635E-2660-44CA-9C7E-B7FA22046102}"/>
     <hyperlink ref="A49" r:id="rId47" xr:uid="{C98AC16A-5431-4F8E-A2D1-1D91D98DD1DE}"/>
     <hyperlink ref="A48" r:id="rId48" xr:uid="{FDC54CF5-7771-49C5-B449-F212EDD30098}"/>
+    <hyperlink ref="A50" r:id="rId49" xr:uid="{8601F3BB-9CCE-402B-8AF4-24726719897B}"/>
+    <hyperlink ref="A51" r:id="rId50" xr:uid="{18DE0E86-929C-424F-AC35-C0FA8D68A848}"/>
+    <hyperlink ref="A52" r:id="rId51" xr:uid="{125C8295-5040-4F84-9236-ACD694D73394}"/>
+    <hyperlink ref="A53" r:id="rId52" xr:uid="{FB1FBC3A-90E6-41CD-8267-52EF6423909F}"/>
+    <hyperlink ref="A55" r:id="rId53" xr:uid="{84C8251D-DCDA-4BB0-A8A4-99D756953C8B}"/>
+    <hyperlink ref="A54" r:id="rId54" xr:uid="{1AF8D1BB-D16A-40D2-90AA-0F9CB0A2BDFA}"/>
+    <hyperlink ref="A57" r:id="rId55" xr:uid="{6C228717-AF08-4622-8319-D429FFBE8334}"/>
+    <hyperlink ref="A59" r:id="rId56" xr:uid="{A38A6402-C986-41C5-9EEC-ECC2F20C752A}"/>
+    <hyperlink ref="A56" r:id="rId57" xr:uid="{39ED4D2F-27DF-4B9A-AEEF-0E73600F1BFD}"/>
+    <hyperlink ref="A58" r:id="rId58" xr:uid="{A2E5CB28-9FEB-4358-A570-CB5269A4E6ED}"/>
+    <hyperlink ref="A60" r:id="rId59" xr:uid="{CD3666E4-7555-4823-ACEB-7FB286F67920}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Integrated Hip Sex Mod
</commit_message>
<xml_diff>
--- a/development/Integrated Mods.xlsx
+++ b/development/Integrated Mods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\S.T.A.L.K.E.R\Anomaly Mods\mods\Back-to-roots-wip\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CF3F7B-75C8-43E7-8C97-9269A1574D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05350878-B74E-4A18-9ADF-97BC0B0E97D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="97">
   <si>
     <t>Filename</t>
   </si>
@@ -315,6 +315,18 @@
   </si>
   <si>
     <t>Equipment_icons.dds</t>
+  </si>
+  <si>
+    <t>Gray Hip Outfit</t>
+  </si>
+  <si>
+    <t>textures/act/npc_remeik/</t>
+  </si>
+  <si>
+    <t>act_stalker_nebo_girl.dds</t>
+  </si>
+  <si>
+    <t>DinkyBinky</t>
   </si>
 </sst>
 </file>
@@ -858,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8700934C-DA8F-46A3-9CCC-A5B0203FB02B}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1893,11 +1905,21 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
-      <c r="B61" s="20"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="14"/>
+      <c r="A61" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B61" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="14" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
@@ -2093,6 +2115,7 @@
     <hyperlink ref="A56" r:id="rId57" xr:uid="{39ED4D2F-27DF-4B9A-AEEF-0E73600F1BFD}"/>
     <hyperlink ref="A58" r:id="rId58" xr:uid="{A2E5CB28-9FEB-4358-A570-CB5269A4E6ED}"/>
     <hyperlink ref="A60" r:id="rId59" xr:uid="{CD3666E4-7555-4823-ACEB-7FB286F67920}"/>
+    <hyperlink ref="A61" r:id="rId60" xr:uid="{A572B6C2-66A5-4D87-9090-08B079BF76A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Integrated AI Headlamp fix
</commit_message>
<xml_diff>
--- a/development/Integrated Mods.xlsx
+++ b/development/Integrated Mods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\S.T.A.L.K.E.R\Anomaly Mods\mods\Back-to-roots-wip\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C57C093-35C3-4EAF-A8B1-F169FA0F99B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7516636B-0527-439D-A878-88ED3BFEEE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="109">
   <si>
     <t>Filename</t>
   </si>
@@ -354,6 +354,15 @@
   </si>
   <si>
     <t>zz_ui_workshop_keep_crafting_window_open.script</t>
+  </si>
+  <si>
+    <t>Stealth Fix</t>
+  </si>
+  <si>
+    <t>sr_light.script</t>
+  </si>
+  <si>
+    <t>Tweaki_Breeki</t>
   </si>
 </sst>
 </file>
@@ -897,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8700934C-DA8F-46A3-9CCC-A5B0203FB02B}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,7 +917,7 @@
     <col min="3" max="3" width="36.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" customWidth="1"/>
-    <col min="6" max="6" width="74.28515625" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2068,11 +2077,21 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="20"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="14"/>
+      <c r="A69" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B69" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" s="14" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
@@ -2220,6 +2239,7 @@
     <hyperlink ref="A67" r:id="rId65" xr:uid="{5B018734-69DA-4E66-A6CB-9859F6F46663}"/>
     <hyperlink ref="A66" r:id="rId66" xr:uid="{379263CA-9474-4231-8514-9F7E6B66B20D}"/>
     <hyperlink ref="A68" r:id="rId67" xr:uid="{22CC5744-9D59-4AB0-BE68-FE916F156417}"/>
+    <hyperlink ref="A69" r:id="rId68" xr:uid="{BAB53D87-6B55-49A5-9EBF-F061429D61E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Integrated Headlamp Animation script
</commit_message>
<xml_diff>
--- a/development/Integrated Mods.xlsx
+++ b/development/Integrated Mods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\S.T.A.L.K.E.R\Anomaly Mods\mods\Back-to-roots-wip\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7516636B-0527-439D-A878-88ED3BFEEE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0344BA-C940-4404-AFEA-6FF4101DCAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="109">
   <si>
     <t>Filename</t>
   </si>
@@ -906,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8700934C-DA8F-46A3-9CCC-A5B0203FB02B}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,11 +2094,21 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="19"/>
-      <c r="C70" s="11"/>
-      <c r="D70" s="9"/>
-      <c r="E70" s="15"/>
+      <c r="A70" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B70" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" s="15" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
@@ -2240,6 +2250,7 @@
     <hyperlink ref="A66" r:id="rId66" xr:uid="{379263CA-9474-4231-8514-9F7E6B66B20D}"/>
     <hyperlink ref="A68" r:id="rId67" xr:uid="{22CC5744-9D59-4AB0-BE68-FE916F156417}"/>
     <hyperlink ref="A69" r:id="rId68" xr:uid="{BAB53D87-6B55-49A5-9EBF-F061429D61E4}"/>
+    <hyperlink ref="A70" r:id="rId69" xr:uid="{B95FD375-C58E-472D-A97A-585AACDC449F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed the script and integrated
</commit_message>
<xml_diff>
--- a/development/Integrated Mods.xlsx
+++ b/development/Integrated Mods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\S.T.A.L.K.E.R\Anomaly Mods\mods\Back-to-roots-wip\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CB6F56-84D2-4569-BF70-15EE7FF2AC24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CF6889-16CB-4A79-A648-FD07B4398360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="118">
   <si>
     <t>Filename</t>
   </si>
@@ -338,9 +338,6 @@
     <t>dynamic_npc_armor_visuals.script</t>
   </si>
   <si>
-    <t>Keep Crafting Window Open</t>
-  </si>
-  <si>
     <t>demonized_time_events.script</t>
   </si>
   <si>
@@ -372,13 +369,34 @@
   </si>
   <si>
     <t>ilrathcxv</t>
+  </si>
+  <si>
+    <t>Hit Impulse Restored</t>
+  </si>
+  <si>
+    <t>space_kirill</t>
+  </si>
+  <si>
+    <t>XR-danger script</t>
+  </si>
+  <si>
+    <t>Attachment icon fix</t>
+  </si>
+  <si>
+    <t>Vanila weapons files must be edited for these to work</t>
+  </si>
+  <si>
+    <t>_EverybodyLies_</t>
+  </si>
+  <si>
+    <t>config/items/weapons/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,8 +433,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="0.79998168889431442"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -489,8 +514,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -527,12 +564,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -576,8 +644,33 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -915,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8700934C-DA8F-46A3-9CCC-A5B0203FB02B}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44:E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,7 +1040,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="28" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -959,14 +1052,12 @@
       <c r="D2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="32" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>5</v>
-      </c>
+      <c r="A3" s="29"/>
       <c r="B3" s="20" t="s">
         <v>12</v>
       </c>
@@ -976,9 +1067,7 @@
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>6</v>
-      </c>
+      <c r="E3" s="33"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -993,12 +1082,12 @@
       <c r="D4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="29" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="21" t="s">
@@ -1010,14 +1099,12 @@
       <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="33" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="A6" s="29"/>
       <c r="B6" s="19" t="s">
         <v>20</v>
       </c>
@@ -1027,14 +1114,10 @@
       <c r="D6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="15" t="s">
-        <v>18</v>
-      </c>
+      <c r="E6" s="33"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>17</v>
-      </c>
+      <c r="A7" s="29"/>
       <c r="B7" s="20" t="s">
         <v>22</v>
       </c>
@@ -1044,14 +1127,10 @@
       <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>18</v>
-      </c>
+      <c r="E7" s="33"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="A8" s="29"/>
       <c r="B8" s="19" t="s">
         <v>23</v>
       </c>
@@ -1061,14 +1140,10 @@
       <c r="D8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>18</v>
-      </c>
+      <c r="E8" s="33"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>17</v>
-      </c>
+      <c r="A9" s="29"/>
       <c r="B9" s="20" t="s">
         <v>24</v>
       </c>
@@ -1078,14 +1153,10 @@
       <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>18</v>
-      </c>
+      <c r="E9" s="33"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="A10" s="29"/>
       <c r="B10" s="19" t="s">
         <v>25</v>
       </c>
@@ -1095,14 +1166,10 @@
       <c r="D10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="15" t="s">
-        <v>18</v>
-      </c>
+      <c r="E10" s="33"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>17</v>
-      </c>
+      <c r="A11" s="29"/>
       <c r="B11" s="20" t="s">
         <v>26</v>
       </c>
@@ -1112,14 +1179,10 @@
       <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>18</v>
-      </c>
+      <c r="E11" s="33"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="A12" s="29"/>
       <c r="B12" s="19" t="s">
         <v>25</v>
       </c>
@@ -1129,14 +1192,10 @@
       <c r="D12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>18</v>
-      </c>
+      <c r="E12" s="33"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>17</v>
-      </c>
+      <c r="A13" s="29"/>
       <c r="B13" s="20" t="s">
         <v>26</v>
       </c>
@@ -1146,12 +1205,10 @@
       <c r="D13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>18</v>
-      </c>
+      <c r="E13" s="33"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="27" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="22" t="s">
@@ -1163,14 +1220,10 @@
       <c r="D14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>18</v>
-      </c>
+      <c r="E14" s="33"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="A15" s="27"/>
       <c r="B15" s="20" t="s">
         <v>31</v>
       </c>
@@ -1180,14 +1233,10 @@
       <c r="D15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="14" t="s">
-        <v>18</v>
-      </c>
+      <c r="E15" s="33"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>30</v>
-      </c>
+      <c r="A16" s="27"/>
       <c r="B16" s="19" t="s">
         <v>32</v>
       </c>
@@ -1197,14 +1246,10 @@
       <c r="D16" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="15" t="s">
-        <v>18</v>
-      </c>
+      <c r="E16" s="33"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="A17" s="27"/>
       <c r="B17" s="20" t="s">
         <v>33</v>
       </c>
@@ -1214,14 +1259,10 @@
       <c r="D17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="14" t="s">
-        <v>18</v>
-      </c>
+      <c r="E17" s="33"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>30</v>
-      </c>
+      <c r="A18" s="27"/>
       <c r="B18" s="19" t="s">
         <v>34</v>
       </c>
@@ -1231,14 +1272,10 @@
       <c r="D18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="15" t="s">
-        <v>18</v>
-      </c>
+      <c r="E18" s="33"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="A19" s="27"/>
       <c r="B19" s="20" t="s">
         <v>35</v>
       </c>
@@ -1248,14 +1285,10 @@
       <c r="D19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="14" t="s">
-        <v>18</v>
-      </c>
+      <c r="E19" s="33"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>30</v>
-      </c>
+      <c r="A20" s="27"/>
       <c r="B20" s="19" t="s">
         <v>36</v>
       </c>
@@ -1265,14 +1298,10 @@
       <c r="D20" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="15" t="s">
-        <v>18</v>
-      </c>
+      <c r="E20" s="33"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="A21" s="27"/>
       <c r="B21" s="20" t="s">
         <v>37</v>
       </c>
@@ -1282,14 +1311,10 @@
       <c r="D21" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="14" t="s">
-        <v>18</v>
-      </c>
+      <c r="E21" s="33"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
-        <v>30</v>
-      </c>
+      <c r="A22" s="27"/>
       <c r="B22" s="19" t="s">
         <v>38</v>
       </c>
@@ -1299,14 +1324,10 @@
       <c r="D22" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="15" t="s">
-        <v>18</v>
-      </c>
+      <c r="E22" s="33"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="A23" s="27"/>
       <c r="B23" s="20" t="s">
         <v>39</v>
       </c>
@@ -1316,14 +1337,10 @@
       <c r="D23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="14" t="s">
-        <v>18</v>
-      </c>
+      <c r="E23" s="33"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
-        <v>30</v>
-      </c>
+      <c r="A24" s="27"/>
       <c r="B24" s="19" t="s">
         <v>40</v>
       </c>
@@ -1333,14 +1350,10 @@
       <c r="D24" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="15" t="s">
-        <v>18</v>
-      </c>
+      <c r="E24" s="33"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="A25" s="27"/>
       <c r="B25" s="20" t="s">
         <v>40</v>
       </c>
@@ -1350,12 +1363,10 @@
       <c r="D25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="14" t="s">
-        <v>18</v>
-      </c>
+      <c r="E25" s="33"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="13" t="s">
         <v>42</v>
       </c>
       <c r="B26" s="19" t="s">
@@ -1367,12 +1378,12 @@
       <c r="D26" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="E26" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="27" t="s">
         <v>45</v>
       </c>
       <c r="B27" s="21" t="s">
@@ -1384,14 +1395,12 @@
       <c r="D27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="33" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>45</v>
-      </c>
+      <c r="A28" s="27"/>
       <c r="B28" s="22" t="s">
         <v>19</v>
       </c>
@@ -1401,14 +1410,10 @@
       <c r="D28" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="15" t="s">
-        <v>46</v>
-      </c>
+      <c r="E28" s="33"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>45</v>
-      </c>
+      <c r="A29" s="27"/>
       <c r="B29" s="21" t="s">
         <v>19</v>
       </c>
@@ -1418,12 +1423,10 @@
       <c r="D29" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="14" t="s">
-        <v>46</v>
-      </c>
+      <c r="E29" s="33"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="13" t="s">
         <v>47</v>
       </c>
       <c r="B30" s="19" t="s">
@@ -1435,12 +1438,12 @@
       <c r="D30" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="14" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="27" t="s">
         <v>54</v>
       </c>
       <c r="B31" s="20" t="s">
@@ -1452,14 +1455,12 @@
       <c r="D31" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="33" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>54</v>
-      </c>
+      <c r="A32" s="27"/>
       <c r="B32" s="19" t="s">
         <v>56</v>
       </c>
@@ -1469,82 +1470,56 @@
       <c r="D32" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="15" t="s">
-        <v>55</v>
-      </c>
+      <c r="E32" s="33"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>54</v>
-      </c>
+      <c r="A33" s="27"/>
       <c r="B33" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="27" t="s">
+      <c r="C33" s="31" t="s">
         <v>63</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="E33" s="14" t="s">
-        <v>55</v>
-      </c>
+      <c r="E33" s="33"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
-        <v>54</v>
-      </c>
+      <c r="A34" s="27"/>
       <c r="B34" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="28" t="s">
-        <v>63</v>
-      </c>
+      <c r="C34" s="31"/>
       <c r="D34" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="E34" s="15" t="s">
-        <v>55</v>
-      </c>
+      <c r="E34" s="33"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
-        <v>54</v>
-      </c>
+      <c r="A35" s="27"/>
       <c r="B35" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C35" s="27" t="s">
-        <v>63</v>
-      </c>
+      <c r="C35" s="31"/>
       <c r="D35" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="E35" s="14" t="s">
-        <v>55</v>
-      </c>
+      <c r="E35" s="33"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
-        <v>54</v>
-      </c>
+      <c r="A36" s="27"/>
       <c r="B36" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="28" t="s">
-        <v>63</v>
-      </c>
+      <c r="C36" s="31"/>
       <c r="D36" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="E36" s="15" t="s">
-        <v>55</v>
-      </c>
+      <c r="E36" s="33"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
-        <v>54</v>
-      </c>
+      <c r="A37" s="27"/>
       <c r="B37" s="20" t="s">
         <v>62</v>
       </c>
@@ -1554,14 +1529,10 @@
       <c r="D37" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="14" t="s">
-        <v>55</v>
-      </c>
+      <c r="E37" s="33"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
-        <v>54</v>
-      </c>
+      <c r="A38" s="27"/>
       <c r="B38" s="19" t="s">
         <v>64</v>
       </c>
@@ -1571,14 +1542,10 @@
       <c r="D38" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="15" t="s">
-        <v>55</v>
-      </c>
+      <c r="E38" s="33"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>54</v>
-      </c>
+      <c r="A39" s="27"/>
       <c r="B39" s="20" t="s">
         <v>65</v>
       </c>
@@ -1588,14 +1555,10 @@
       <c r="D39" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E39" s="14" t="s">
-        <v>55</v>
-      </c>
+      <c r="E39" s="33"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
-        <v>54</v>
-      </c>
+      <c r="A40" s="27"/>
       <c r="B40" s="19" t="s">
         <v>66</v>
       </c>
@@ -1605,14 +1568,10 @@
       <c r="D40" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="15" t="s">
-        <v>55</v>
-      </c>
+      <c r="E40" s="33"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
-        <v>54</v>
-      </c>
+      <c r="A41" s="27"/>
       <c r="B41" s="20" t="s">
         <v>67</v>
       </c>
@@ -1622,14 +1581,10 @@
       <c r="D41" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E41" s="14" t="s">
-        <v>55</v>
-      </c>
+      <c r="E41" s="33"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
-        <v>54</v>
-      </c>
+      <c r="A42" s="27"/>
       <c r="B42" s="22" t="s">
         <v>19</v>
       </c>
@@ -1639,14 +1594,10 @@
       <c r="D42" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="15" t="s">
-        <v>55</v>
-      </c>
+      <c r="E42" s="33"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
-        <v>54</v>
-      </c>
+      <c r="A43" s="27"/>
       <c r="B43" s="20" t="s">
         <v>69</v>
       </c>
@@ -1656,12 +1607,10 @@
       <c r="D43" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E43" s="14" t="s">
-        <v>55</v>
-      </c>
+      <c r="E43" s="33"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
+      <c r="A44" s="29" t="s">
         <v>71</v>
       </c>
       <c r="B44" s="19" t="s">
@@ -1673,14 +1622,12 @@
       <c r="D44" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E44" s="15" t="s">
+      <c r="E44" s="34" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
-        <v>71</v>
-      </c>
+      <c r="A45" s="29"/>
       <c r="B45" s="20" t="s">
         <v>73</v>
       </c>
@@ -1690,14 +1637,10 @@
       <c r="D45" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E45" s="14" t="s">
-        <v>72</v>
-      </c>
+      <c r="E45" s="34"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
-        <v>71</v>
-      </c>
+      <c r="A46" s="29"/>
       <c r="B46" s="19" t="s">
         <v>74</v>
       </c>
@@ -1707,14 +1650,10 @@
       <c r="D46" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E46" s="15" t="s">
-        <v>72</v>
-      </c>
+      <c r="E46" s="34"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
-        <v>71</v>
-      </c>
+      <c r="A47" s="29"/>
       <c r="B47" s="20" t="s">
         <v>75</v>
       </c>
@@ -1724,14 +1663,10 @@
       <c r="D47" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E47" s="14" t="s">
-        <v>72</v>
-      </c>
+      <c r="E47" s="34"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="12" t="s">
-        <v>71</v>
-      </c>
+      <c r="A48" s="29"/>
       <c r="B48" s="19" t="s">
         <v>76</v>
       </c>
@@ -1741,14 +1676,10 @@
       <c r="D48" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E48" s="15" t="s">
-        <v>72</v>
-      </c>
+      <c r="E48" s="34"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
-        <v>71</v>
-      </c>
+      <c r="A49" s="29"/>
       <c r="B49" s="20" t="s">
         <v>77</v>
       </c>
@@ -1758,9 +1689,7 @@
       <c r="D49" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="14" t="s">
-        <v>72</v>
-      </c>
+      <c r="E49" s="34"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
@@ -1780,7 +1709,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="29" t="s">
         <v>80</v>
       </c>
       <c r="B51" s="20" t="s">
@@ -1792,14 +1721,12 @@
       <c r="D51" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E51" s="14" t="s">
+      <c r="E51" s="34" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="12" t="s">
-        <v>80</v>
-      </c>
+      <c r="A52" s="29"/>
       <c r="B52" s="19" t="s">
         <v>84</v>
       </c>
@@ -1809,14 +1736,10 @@
       <c r="D52" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E52" s="15" t="s">
-        <v>81</v>
-      </c>
+      <c r="E52" s="34"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="s">
-        <v>80</v>
-      </c>
+      <c r="A53" s="29"/>
       <c r="B53" s="20" t="s">
         <v>84</v>
       </c>
@@ -1826,14 +1749,10 @@
       <c r="D53" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E53" s="14" t="s">
-        <v>81</v>
-      </c>
+      <c r="E53" s="34"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="12" t="s">
-        <v>80</v>
-      </c>
+      <c r="A54" s="29"/>
       <c r="B54" s="19" t="s">
         <v>85</v>
       </c>
@@ -1843,14 +1762,10 @@
       <c r="D54" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E54" s="15" t="s">
-        <v>81</v>
-      </c>
+      <c r="E54" s="34"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="13" t="s">
-        <v>80</v>
-      </c>
+      <c r="A55" s="29"/>
       <c r="B55" s="20" t="s">
         <v>86</v>
       </c>
@@ -1860,14 +1775,10 @@
       <c r="D55" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E55" s="14" t="s">
-        <v>81</v>
-      </c>
+      <c r="E55" s="34"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="12" t="s">
-        <v>80</v>
-      </c>
+      <c r="A56" s="29"/>
       <c r="B56" s="19" t="s">
         <v>87</v>
       </c>
@@ -1877,14 +1788,10 @@
       <c r="D56" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E56" s="15" t="s">
-        <v>81</v>
-      </c>
+      <c r="E56" s="34"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
-        <v>80</v>
-      </c>
+      <c r="A57" s="29"/>
       <c r="B57" s="20" t="s">
         <v>88</v>
       </c>
@@ -1894,14 +1801,10 @@
       <c r="D57" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E57" s="14" t="s">
-        <v>81</v>
-      </c>
+      <c r="E57" s="34"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
-        <v>80</v>
-      </c>
+      <c r="A58" s="29"/>
       <c r="B58" s="19" t="s">
         <v>89</v>
       </c>
@@ -1911,14 +1814,10 @@
       <c r="D58" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E58" s="15" t="s">
-        <v>81</v>
-      </c>
+      <c r="E58" s="34"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="13" t="s">
-        <v>80</v>
-      </c>
+      <c r="A59" s="29"/>
       <c r="B59" s="20" t="s">
         <v>90</v>
       </c>
@@ -1928,14 +1827,10 @@
       <c r="D59" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E59" s="14" t="s">
-        <v>81</v>
-      </c>
+      <c r="E59" s="34"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="12" t="s">
-        <v>80</v>
-      </c>
+      <c r="A60" s="29"/>
       <c r="B60" s="19" t="s">
         <v>92</v>
       </c>
@@ -1945,12 +1840,10 @@
       <c r="D60" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E60" s="15" t="s">
-        <v>81</v>
-      </c>
+      <c r="E60" s="34"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
+      <c r="A61" s="12" t="s">
         <v>93</v>
       </c>
       <c r="B61" s="20" t="s">
@@ -1962,12 +1855,12 @@
       <c r="D61" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E61" s="14" t="s">
+      <c r="E61" s="15" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="12" t="s">
+      <c r="A62" s="29" t="s">
         <v>97</v>
       </c>
       <c r="B62" s="19" t="s">
@@ -1979,14 +1872,12 @@
       <c r="D62" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E62" s="15" t="s">
+      <c r="E62" s="34" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
-        <v>97</v>
-      </c>
+      <c r="A63" s="29"/>
       <c r="B63" s="20" t="s">
         <v>99</v>
       </c>
@@ -1996,110 +1887,90 @@
       <c r="D63" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E63" s="14" t="s">
-        <v>55</v>
-      </c>
+      <c r="E63" s="34"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="12" t="s">
+      <c r="A64" s="29"/>
+      <c r="B64" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="B64" s="19" t="s">
+      <c r="C64" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="29"/>
+      <c r="B65" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="C64" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E64" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B65" s="20" t="s">
+      <c r="C65" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="33"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="29"/>
+      <c r="B66" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C65" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E65" s="14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="B66" s="19" t="s">
+      <c r="C66" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" s="33"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="29"/>
+      <c r="B67" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="C66" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E66" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B67" s="20" t="s">
+      <c r="C67" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="33"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="29"/>
+      <c r="B68" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="C67" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E67" s="14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="B68" s="19" t="s">
-        <v>105</v>
-      </c>
       <c r="C68" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D68" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E68" s="15" t="s">
-        <v>72</v>
-      </c>
+      <c r="E68" s="33"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B69" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B69" s="20" t="s">
+      <c r="C69" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" s="14" t="s">
         <v>107</v>
-      </c>
-      <c r="C69" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E69" s="14" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2121,38 +1992,56 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B71" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B71" s="20" t="s">
+      <c r="C71" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C71" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E71" s="14" t="s">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="12" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-      <c r="B72" s="19"/>
-      <c r="C72" s="11"/>
-      <c r="D72" s="9"/>
-      <c r="E72" s="15"/>
+      <c r="B72" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C72" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="D72" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E72" s="15" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="20"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="14"/>
+      <c r="A73" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B73" s="35"/>
+      <c r="C73" s="31"/>
+      <c r="D73" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E73" s="14" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
-      <c r="B74" s="19"/>
+      <c r="A74" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B74" s="30"/>
       <c r="C74" s="11"/>
       <c r="D74" s="9"/>
       <c r="E74" s="15"/>
@@ -2200,77 +2089,47 @@
       <c r="E80" s="15"/>
     </row>
   </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E5:E25"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="E31:E43"/>
+    <mergeCell ref="E44:E49"/>
+    <mergeCell ref="E51:E60"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="E64:E68"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A5:A13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A31:A43"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="A51:A60"/>
+    <mergeCell ref="A62:A68"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{D01E85B4-1DB0-475A-87DE-364916E7DA22}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{9C32D888-2A2C-4792-89DE-21C048A67B43}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{6DC9B457-A97D-43C1-B925-29BBAE81D28D}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{0CEEAA07-CCE4-482B-A880-7BF042506AFE}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{3EDA65A1-1DC5-4B24-BB1B-A2B13113E508}"/>
-    <hyperlink ref="A14" r:id="rId6" xr:uid="{7417E636-5018-4213-B7A7-56D7326D2B8E}"/>
-    <hyperlink ref="A15" r:id="rId7" xr:uid="{3C431D88-C5CA-4118-AA9B-19370BBDC948}"/>
-    <hyperlink ref="A16" r:id="rId8" xr:uid="{2BBD4D12-9A1D-4E02-BEEE-0EB9C4EDE997}"/>
-    <hyperlink ref="A18" r:id="rId9" xr:uid="{8C20C878-EAD2-4A3A-BCB6-519E8C153083}"/>
-    <hyperlink ref="A20" r:id="rId10" xr:uid="{7EB06454-3C4D-40CF-93E9-D82036CA9954}"/>
-    <hyperlink ref="A22" r:id="rId11" xr:uid="{886211A2-9E3B-4A21-BFD0-0E12AE7EFB2C}"/>
-    <hyperlink ref="A17" r:id="rId12" xr:uid="{B7EE9BAB-ED56-455F-B92A-27FA6759A85B}"/>
-    <hyperlink ref="A19" r:id="rId13" xr:uid="{4B6558AD-89E7-452C-97A2-FE459AACD2D2}"/>
-    <hyperlink ref="A21" r:id="rId14" xr:uid="{D4C60355-B0FB-4A18-9443-9C43834BC7B8}"/>
-    <hyperlink ref="A23" r:id="rId15" xr:uid="{3F3B0406-D67A-47AA-8FC9-B5287B0EF720}"/>
-    <hyperlink ref="A25" r:id="rId16" xr:uid="{94557B4D-1AC3-4BB5-A1A0-85583F61062C}"/>
-    <hyperlink ref="A24" r:id="rId17" xr:uid="{08B015F2-443A-4B2E-BE3E-59CDB6D7E12B}"/>
-    <hyperlink ref="A26" r:id="rId18" xr:uid="{8AC3304D-47D0-4E90-A162-34FFE64C55E4}"/>
-    <hyperlink ref="A27" r:id="rId19" xr:uid="{67434F82-E4BA-4FEA-8F7B-B4A0C40B78E6}"/>
-    <hyperlink ref="A28" r:id="rId20" xr:uid="{6DA97BD3-CC17-403F-B7FF-02F7068EF17B}"/>
-    <hyperlink ref="A29" r:id="rId21" xr:uid="{E7AA11F1-A609-4836-B9BF-13DFAE7D731F}"/>
-    <hyperlink ref="A30" r:id="rId22" xr:uid="{C82EC4B2-2E87-4D62-A803-5967541F5C45}"/>
-    <hyperlink ref="A31" r:id="rId23" xr:uid="{51617730-5764-4AB3-B20B-07520480AAAA}"/>
-    <hyperlink ref="A32" r:id="rId24" xr:uid="{47FFEFD9-016A-4EB2-82E1-F653D4FD39AE}"/>
-    <hyperlink ref="A34" r:id="rId25" xr:uid="{4B409849-CA84-4878-B2FF-A57C7992B888}"/>
-    <hyperlink ref="A36" r:id="rId26" xr:uid="{7FF75CC5-5A26-469D-AB1C-70E19B4316F6}"/>
-    <hyperlink ref="A33" r:id="rId27" xr:uid="{B248F343-0D24-4CEF-96BA-71B832E308C6}"/>
-    <hyperlink ref="A35" r:id="rId28" xr:uid="{D8E230CB-7AEC-4A77-A365-D868FD04D348}"/>
-    <hyperlink ref="A37" r:id="rId29" xr:uid="{BD6D143A-6A15-46A3-A1CC-7CD9D6CA899D}"/>
-    <hyperlink ref="A39" r:id="rId30" xr:uid="{F9C89859-B6BC-4418-9668-A11B86FC207B}"/>
-    <hyperlink ref="A38" r:id="rId31" xr:uid="{AF7A7DA1-2C60-4F6C-9DE0-8D0A22F2F8F4}"/>
-    <hyperlink ref="A40" r:id="rId32" xr:uid="{97547C1D-97C3-4AA8-87D3-E0570D4AA386}"/>
-    <hyperlink ref="A41" r:id="rId33" xr:uid="{90EBA847-6BE3-4A5F-98F9-33A3BFE8AD55}"/>
-    <hyperlink ref="A42" r:id="rId34" xr:uid="{AEB930B8-F348-4B11-9BC6-7E89C9B97A2F}"/>
-    <hyperlink ref="A43" r:id="rId35" xr:uid="{D9DC5DEF-87AC-4F8D-8276-297627A9413C}"/>
-    <hyperlink ref="A44" r:id="rId36" xr:uid="{D33F6994-5A97-46A8-9B3C-5DF835643C25}"/>
-    <hyperlink ref="A8" r:id="rId37" xr:uid="{2D59AB75-03FA-4F2B-96E5-6F2E6F4158C2}"/>
-    <hyperlink ref="A10" r:id="rId38" xr:uid="{49F32376-7630-4C72-84C3-27F16658A30F}"/>
-    <hyperlink ref="A12" r:id="rId39" xr:uid="{F7688210-1E5B-4FBA-89BD-029C6583D26D}"/>
-    <hyperlink ref="A7" r:id="rId40" xr:uid="{F7EC5AEE-79E5-4938-8D0A-7F41572766D4}"/>
-    <hyperlink ref="A9" r:id="rId41" xr:uid="{DAA7C740-B987-4F6D-AAB2-C9DE4B132718}"/>
-    <hyperlink ref="A11" r:id="rId42" xr:uid="{95729464-37DF-40FD-9AA8-37B389C12FD0}"/>
-    <hyperlink ref="A13" r:id="rId43" xr:uid="{A1CB40CF-8E81-410A-B880-E13ED1BEE1C0}"/>
-    <hyperlink ref="A45" r:id="rId44" xr:uid="{514A65D1-F6B9-42FF-9F46-CF61B4BABB73}"/>
-    <hyperlink ref="A46" r:id="rId45" xr:uid="{A64F811F-9AAD-441E-BFD8-BF6A725C9C0B}"/>
-    <hyperlink ref="A47" r:id="rId46" xr:uid="{D425635E-2660-44CA-9C7E-B7FA22046102}"/>
-    <hyperlink ref="A49" r:id="rId47" xr:uid="{C98AC16A-5431-4F8E-A2D1-1D91D98DD1DE}"/>
-    <hyperlink ref="A48" r:id="rId48" xr:uid="{FDC54CF5-7771-49C5-B449-F212EDD30098}"/>
-    <hyperlink ref="A50" r:id="rId49" xr:uid="{8601F3BB-9CCE-402B-8AF4-24726719897B}"/>
-    <hyperlink ref="A51" r:id="rId50" xr:uid="{18DE0E86-929C-424F-AC35-C0FA8D68A848}"/>
-    <hyperlink ref="A52" r:id="rId51" xr:uid="{125C8295-5040-4F84-9236-ACD694D73394}"/>
-    <hyperlink ref="A53" r:id="rId52" xr:uid="{FB1FBC3A-90E6-41CD-8267-52EF6423909F}"/>
-    <hyperlink ref="A55" r:id="rId53" xr:uid="{84C8251D-DCDA-4BB0-A8A4-99D756953C8B}"/>
-    <hyperlink ref="A54" r:id="rId54" xr:uid="{1AF8D1BB-D16A-40D2-90AA-0F9CB0A2BDFA}"/>
-    <hyperlink ref="A57" r:id="rId55" xr:uid="{6C228717-AF08-4622-8319-D429FFBE8334}"/>
-    <hyperlink ref="A59" r:id="rId56" xr:uid="{A38A6402-C986-41C5-9EEC-ECC2F20C752A}"/>
-    <hyperlink ref="A56" r:id="rId57" xr:uid="{39ED4D2F-27DF-4B9A-AEEF-0E73600F1BFD}"/>
-    <hyperlink ref="A58" r:id="rId58" xr:uid="{A2E5CB28-9FEB-4358-A570-CB5269A4E6ED}"/>
-    <hyperlink ref="A60" r:id="rId59" xr:uid="{CD3666E4-7555-4823-ACEB-7FB286F67920}"/>
-    <hyperlink ref="A61" r:id="rId60" xr:uid="{A572B6C2-66A5-4D87-9090-08B079BF76A0}"/>
-    <hyperlink ref="A62" r:id="rId61" xr:uid="{D246E613-2245-4094-AC96-6442AA4B4E19}"/>
-    <hyperlink ref="A63" r:id="rId62" xr:uid="{B8C510F9-4DEB-4D0A-A1D3-0D32D77DBB59}"/>
-    <hyperlink ref="A64" r:id="rId63" xr:uid="{5EADEBA0-C928-4DF7-A41D-11B7FD9D5D75}"/>
-    <hyperlink ref="A65" r:id="rId64" xr:uid="{007E020F-E8D2-4458-B7F8-60A200D98DE5}"/>
-    <hyperlink ref="A67" r:id="rId65" xr:uid="{5B018734-69DA-4E66-A6CB-9859F6F46663}"/>
-    <hyperlink ref="A66" r:id="rId66" xr:uid="{379263CA-9474-4231-8514-9F7E6B66B20D}"/>
-    <hyperlink ref="A68" r:id="rId67" xr:uid="{22CC5744-9D59-4AB0-BE68-FE916F156417}"/>
-    <hyperlink ref="A69" r:id="rId68" xr:uid="{BAB53D87-6B55-49A5-9EBF-F061429D61E4}"/>
-    <hyperlink ref="A70" r:id="rId69" xr:uid="{B95FD375-C58E-472D-A97A-585AACDC449F}"/>
-    <hyperlink ref="A71" r:id="rId70" xr:uid="{68D48912-0729-4E51-951C-589C23D0AA49}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{6DC9B457-A97D-43C1-B925-29BBAE81D28D}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{0CEEAA07-CCE4-482B-A880-7BF042506AFE}"/>
+    <hyperlink ref="A14" r:id="rId4" xr:uid="{7417E636-5018-4213-B7A7-56D7326D2B8E}"/>
+    <hyperlink ref="A26" r:id="rId5" xr:uid="{8AC3304D-47D0-4E90-A162-34FFE64C55E4}"/>
+    <hyperlink ref="A27" r:id="rId6" xr:uid="{67434F82-E4BA-4FEA-8F7B-B4A0C40B78E6}"/>
+    <hyperlink ref="A30" r:id="rId7" xr:uid="{C82EC4B2-2E87-4D62-A803-5967541F5C45}"/>
+    <hyperlink ref="A31" r:id="rId8" xr:uid="{51617730-5764-4AB3-B20B-07520480AAAA}"/>
+    <hyperlink ref="A44" r:id="rId9" xr:uid="{D33F6994-5A97-46A8-9B3C-5DF835643C25}"/>
+    <hyperlink ref="A50" r:id="rId10" xr:uid="{8601F3BB-9CCE-402B-8AF4-24726719897B}"/>
+    <hyperlink ref="A51" r:id="rId11" xr:uid="{18DE0E86-929C-424F-AC35-C0FA8D68A848}"/>
+    <hyperlink ref="A61" r:id="rId12" xr:uid="{A572B6C2-66A5-4D87-9090-08B079BF76A0}"/>
+    <hyperlink ref="A62" r:id="rId13" xr:uid="{D246E613-2245-4094-AC96-6442AA4B4E19}"/>
+    <hyperlink ref="A69" r:id="rId14" xr:uid="{BAB53D87-6B55-49A5-9EBF-F061429D61E4}"/>
+    <hyperlink ref="A70" r:id="rId15" xr:uid="{B95FD375-C58E-472D-A97A-585AACDC449F}"/>
+    <hyperlink ref="A71" r:id="rId16" xr:uid="{68D48912-0729-4E51-951C-589C23D0AA49}"/>
+    <hyperlink ref="A72" r:id="rId17" xr:uid="{AB056329-5430-4555-8CF3-98B3E35CFC48}"/>
+    <hyperlink ref="A74" r:id="rId18" xr:uid="{3B22816C-344C-494A-9DEE-E1DCBFD8E1DB}"/>
+    <hyperlink ref="A73" r:id="rId19" xr:uid="{3C0C31EC-2080-40A3-A100-ABA2FB6F399B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Something else too. Idk what I did here
</commit_message>
<xml_diff>
--- a/development/Integrated Mods.xlsx
+++ b/development/Integrated Mods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\S.T.A.L.K.E.R\Anomaly Mods\mods\Back-to-roots-wip\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CF6889-16CB-4A79-A648-FD07B4398360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578A4824-F243-4BA7-87C3-B20EAE4C7D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="127">
   <si>
     <t>Filename</t>
   </si>
@@ -390,6 +390,33 @@
   </si>
   <si>
     <t>config/items/weapons/</t>
+  </si>
+  <si>
+    <t>configs/ai_tweaks/</t>
+  </si>
+  <si>
+    <t>xr_danger.ltx</t>
+  </si>
+  <si>
+    <t>xr_danger.script</t>
+  </si>
+  <si>
+    <t>xr_danger.script.bkp2</t>
+  </si>
+  <si>
+    <t>No weapon drop from damage</t>
+  </si>
+  <si>
+    <t>mod_system_burer_drop_disabler.ltx</t>
+  </si>
+  <si>
+    <t>actor_effects.script</t>
+  </si>
+  <si>
+    <t>xr_meet.script</t>
+  </si>
+  <si>
+    <t>xrs_facer.script</t>
   </si>
 </sst>
 </file>
@@ -435,7 +462,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="8" tint="0.79998168889431442"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -600,12 +626,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1008,14 +1032,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8700934C-DA8F-46A3-9CCC-A5B0203FB02B}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:E49"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="48.5703125" style="25" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="48.5703125" style="23" customWidth="1"/>
     <col min="3" max="3" width="36.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" customWidth="1"/>
@@ -1023,1073 +1047,1124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="32" t="s">
+      <c r="D2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="30" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="20" t="s">
+      <c r="A3" s="27"/>
+      <c r="B3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="33"/>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="14" t="s">
+      <c r="C4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="33" t="s">
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="31" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="27"/>
+      <c r="B6" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="33"/>
+      <c r="C6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="31"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
-      <c r="B7" s="20" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="33"/>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="31"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="19" t="s">
+      <c r="A8" s="27"/>
+      <c r="B8" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="33"/>
+      <c r="D8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="31"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="20" t="s">
+      <c r="A9" s="27"/>
+      <c r="B9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="33"/>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="31"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="19" t="s">
+      <c r="A10" s="27"/>
+      <c r="B10" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="33"/>
+      <c r="D10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="31"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="20" t="s">
+      <c r="A11" s="27"/>
+      <c r="B11" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="33"/>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="31"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="19" t="s">
+      <c r="A12" s="27"/>
+      <c r="B12" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="33"/>
+      <c r="D12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="31"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="20" t="s">
+      <c r="A13" s="27"/>
+      <c r="B13" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="33"/>
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="31"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="33"/>
+      <c r="D14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="31"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="20" t="s">
+      <c r="A15" s="25"/>
+      <c r="B15" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="33"/>
+      <c r="C15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="31"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="19" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="33"/>
+      <c r="C16" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="31"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="20" t="s">
+      <c r="A17" s="25"/>
+      <c r="B17" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="33"/>
+      <c r="D17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="31"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="19" t="s">
+      <c r="A18" s="25"/>
+      <c r="B18" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="33"/>
+      <c r="D18" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="31"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="20" t="s">
+      <c r="A19" s="25"/>
+      <c r="B19" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="33"/>
+      <c r="D19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="31"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="19" t="s">
+      <c r="A20" s="25"/>
+      <c r="B20" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="33"/>
+      <c r="D20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="31"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="20" t="s">
+      <c r="A21" s="25"/>
+      <c r="B21" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="33"/>
+      <c r="E21" s="31"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="19" t="s">
+      <c r="A22" s="25"/>
+      <c r="B22" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="33"/>
+      <c r="D22" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="31"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
-      <c r="B23" s="20" t="s">
+      <c r="A23" s="25"/>
+      <c r="B23" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="33"/>
+      <c r="D23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="31"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="19" t="s">
+      <c r="A24" s="25"/>
+      <c r="B24" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="33"/>
+      <c r="D24" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="31"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="20" t="s">
+      <c r="A25" s="25"/>
+      <c r="B25" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="33"/>
+      <c r="D25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="31"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="14" t="s">
+      <c r="C26" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="12" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="33" t="s">
+      <c r="D27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="31" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
-      <c r="B28" s="22" t="s">
+      <c r="A28" s="25"/>
+      <c r="B28" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="33"/>
+      <c r="D28" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="31"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="21" t="s">
+      <c r="A29" s="25"/>
+      <c r="B29" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="33"/>
+      <c r="D29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="31"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="14" t="s">
+      <c r="D30" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="12" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="33" t="s">
+      <c r="D31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="31" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
-      <c r="B32" s="19" t="s">
+      <c r="A32" s="25"/>
+      <c r="B32" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="33"/>
+      <c r="D32" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="31"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
-      <c r="B33" s="23" t="s">
+      <c r="A33" s="25"/>
+      <c r="B33" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="17" t="s">
+      <c r="D33" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E33" s="33"/>
+      <c r="E33" s="31"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="27"/>
-      <c r="B34" s="24" t="s">
+      <c r="A34" s="25"/>
+      <c r="B34" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="26" t="s">
+      <c r="C34" s="29"/>
+      <c r="D34" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="E34" s="33"/>
+      <c r="E34" s="31"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
-      <c r="B35" s="23" t="s">
+      <c r="A35" s="25"/>
+      <c r="B35" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="17" t="s">
+      <c r="C35" s="29"/>
+      <c r="D35" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E35" s="33"/>
+      <c r="E35" s="31"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="27"/>
-      <c r="B36" s="24" t="s">
+      <c r="A36" s="25"/>
+      <c r="B36" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="26" t="s">
+      <c r="C36" s="29"/>
+      <c r="D36" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="E36" s="33"/>
+      <c r="E36" s="31"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="27"/>
-      <c r="B37" s="20" t="s">
+      <c r="A37" s="25"/>
+      <c r="B37" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="33"/>
+      <c r="D37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="31"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="27"/>
-      <c r="B38" s="19" t="s">
+      <c r="A38" s="25"/>
+      <c r="B38" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C38" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="33"/>
+      <c r="C38" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="31"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
-      <c r="B39" s="20" t="s">
+      <c r="A39" s="25"/>
+      <c r="B39" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C39" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="33"/>
+      <c r="C39" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="31"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="27"/>
-      <c r="B40" s="19" t="s">
+      <c r="A40" s="25"/>
+      <c r="B40" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C40" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="33"/>
+      <c r="C40" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="31"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="27"/>
-      <c r="B41" s="20" t="s">
+      <c r="A41" s="25"/>
+      <c r="B41" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C41" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" s="33"/>
+      <c r="C41" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="31"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="27"/>
-      <c r="B42" s="22" t="s">
+      <c r="A42" s="25"/>
+      <c r="B42" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D42" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" s="33"/>
+      <c r="D42" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="31"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="27"/>
-      <c r="B43" s="20" t="s">
+      <c r="A43" s="25"/>
+      <c r="B43" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" s="33"/>
+      <c r="D43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="31"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="29" t="s">
+      <c r="A44" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="34" t="s">
+      <c r="D44" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="32" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="29"/>
-      <c r="B45" s="20" t="s">
+      <c r="A45" s="27"/>
+      <c r="B45" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="34"/>
+      <c r="D45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="32"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="29"/>
-      <c r="B46" s="19" t="s">
+      <c r="A46" s="27"/>
+      <c r="B46" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="34"/>
+      <c r="D46" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="32"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="29"/>
-      <c r="B47" s="20" t="s">
+      <c r="A47" s="27"/>
+      <c r="B47" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="34"/>
+      <c r="D47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="32"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="29"/>
-      <c r="B48" s="19" t="s">
+      <c r="A48" s="27"/>
+      <c r="B48" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="C48" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" s="34"/>
+      <c r="C48" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="32"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="29"/>
-      <c r="B49" s="20" t="s">
+      <c r="A49" s="27"/>
+      <c r="B49" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="C49" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" s="34"/>
+      <c r="C49" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="32"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="12" t="s">
+      <c r="A50" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B50" s="19" t="s">
+      <c r="B50" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="C50" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E50" s="15" t="s">
+      <c r="C50" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="13" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="29" t="s">
+      <c r="A51" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="B51" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E51" s="34" t="s">
+      <c r="D51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="32" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="29"/>
-      <c r="B52" s="19" t="s">
+      <c r="A52" s="27"/>
+      <c r="B52" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D52" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E52" s="34"/>
+      <c r="D52" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="32"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="29"/>
-      <c r="B53" s="20" t="s">
+      <c r="A53" s="27"/>
+      <c r="B53" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C53" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="34"/>
+      <c r="D53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="32"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="29"/>
-      <c r="B54" s="19" t="s">
+      <c r="A54" s="27"/>
+      <c r="B54" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D54" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E54" s="34"/>
+      <c r="D54" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="32"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="29"/>
-      <c r="B55" s="20" t="s">
+      <c r="A55" s="27"/>
+      <c r="B55" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C55" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E55" s="34"/>
+      <c r="D55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="32"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="29"/>
-      <c r="B56" s="19" t="s">
+      <c r="A56" s="27"/>
+      <c r="B56" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C56" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E56" s="34"/>
+      <c r="C56" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="32"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="29"/>
-      <c r="B57" s="20" t="s">
+      <c r="A57" s="27"/>
+      <c r="B57" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C57" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E57" s="34"/>
+      <c r="C57" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="32"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="29"/>
-      <c r="B58" s="19" t="s">
+      <c r="A58" s="27"/>
+      <c r="B58" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="C58" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E58" s="34"/>
+      <c r="C58" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="32"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="29"/>
-      <c r="B59" s="20" t="s">
+      <c r="A59" s="27"/>
+      <c r="B59" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="C59" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E59" s="34"/>
+      <c r="C59" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="32"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="29"/>
-      <c r="B60" s="19" t="s">
+      <c r="A60" s="27"/>
+      <c r="B60" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="C60" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D60" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E60" s="34"/>
+      <c r="D60" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="32"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="12" t="s">
+      <c r="A61" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="C61" s="10" t="s">
+      <c r="C61" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E61" s="15" t="s">
+      <c r="D61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="13" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="29" t="s">
+      <c r="A62" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B62" s="19" t="s">
+      <c r="B62" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C62" s="11" t="s">
+      <c r="C62" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D62" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E62" s="34" t="s">
+      <c r="D62" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="32" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="29"/>
-      <c r="B63" s="20" t="s">
+      <c r="A63" s="27"/>
+      <c r="B63" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C63" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E63" s="34"/>
+      <c r="C63" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="32"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="29"/>
-      <c r="B64" s="19" t="s">
+      <c r="A64" s="27"/>
+      <c r="B64" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C64" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E64" s="33" t="s">
-        <v>72</v>
-      </c>
+      <c r="C64" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="32"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="29"/>
-      <c r="B65" s="20" t="s">
+      <c r="A65" s="27"/>
+      <c r="B65" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C65" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E65" s="33"/>
+      <c r="C65" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="32"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="29"/>
-      <c r="B66" s="19" t="s">
+      <c r="A66" s="27"/>
+      <c r="B66" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C66" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E66" s="33"/>
+      <c r="C66" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" s="32"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="29"/>
-      <c r="B67" s="20" t="s">
+      <c r="A67" s="27"/>
+      <c r="B67" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C67" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E67" s="33"/>
+      <c r="C67" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="32"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="29"/>
-      <c r="B68" s="19" t="s">
+      <c r="A68" s="27"/>
+      <c r="B68" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C68" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D68" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E68" s="33"/>
+      <c r="C68" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="32"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="13" t="s">
+      <c r="A69" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="B69" s="20" t="s">
+      <c r="B69" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C69" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E69" s="14" t="s">
+      <c r="C69" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" s="13" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="12" t="s">
+      <c r="A70" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B70" s="19" t="s">
+      <c r="B70" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="C70" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E70" s="15" t="s">
+      <c r="C70" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" s="12" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="13" t="s">
+      <c r="A71" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B71" s="20" t="s">
+      <c r="B71" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C71" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E71" s="14" t="s">
+      <c r="C71" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" s="13" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="12" t="s">
+      <c r="A72" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="B72" s="35" t="s">
+      <c r="B72" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="C72" s="31" t="s">
+      <c r="C72" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="D72" s="26" t="s">
+      <c r="D72" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="E72" s="15" t="s">
+      <c r="E72" s="12" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="13" t="s">
+      <c r="A73" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="B73" s="35"/>
-      <c r="C73" s="31"/>
-      <c r="D73" s="17" t="s">
+      <c r="B73" s="33"/>
+      <c r="C73" s="29"/>
+      <c r="D73" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E73" s="14" t="s">
+      <c r="E73" s="13" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="12" t="s">
+      <c r="A74" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="B74" s="30"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="9"/>
-      <c r="E74" s="15"/>
+      <c r="B74" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" s="32" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-      <c r="B75" s="20"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="14"/>
+      <c r="A75" s="27"/>
+      <c r="B75" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E75" s="32"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
-      <c r="B76" s="19"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="9"/>
-      <c r="E76" s="15"/>
+      <c r="A76" s="27"/>
+      <c r="B76" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" s="32"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-      <c r="B77" s="20"/>
-      <c r="C77" s="10"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="14"/>
+      <c r="A77" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="B77" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" s="31" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="B78" s="19"/>
-      <c r="C78" s="11"/>
-      <c r="D78" s="9"/>
-      <c r="E78" s="15"/>
+      <c r="A78" s="25"/>
+      <c r="B78" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" s="31"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
-      <c r="B79" s="20"/>
-      <c r="C79" s="10"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="14"/>
+      <c r="A79" s="25"/>
+      <c r="B79" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79" s="31"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
-      <c r="B80" s="19"/>
-      <c r="C80" s="11"/>
-      <c r="D80" s="9"/>
-      <c r="E80" s="15"/>
+      <c r="A80" s="25"/>
+      <c r="B80" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="22">
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="E74:E76"/>
+    <mergeCell ref="E62:E68"/>
+    <mergeCell ref="A77:A80"/>
+    <mergeCell ref="E77:E80"/>
     <mergeCell ref="C72:C73"/>
     <mergeCell ref="C33:C36"/>
     <mergeCell ref="E2:E3"/>
@@ -2098,8 +2173,6 @@
     <mergeCell ref="E31:E43"/>
     <mergeCell ref="E44:E49"/>
     <mergeCell ref="E51:E60"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="E64:E68"/>
     <mergeCell ref="B72:B73"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A5:A13"/>
@@ -2130,6 +2203,7 @@
     <hyperlink ref="A72" r:id="rId17" xr:uid="{AB056329-5430-4555-8CF3-98B3E35CFC48}"/>
     <hyperlink ref="A74" r:id="rId18" xr:uid="{3B22816C-344C-494A-9DEE-E1DCBFD8E1DB}"/>
     <hyperlink ref="A73" r:id="rId19" xr:uid="{3C0C31EC-2080-40A3-A100-ABA2FB6F399B}"/>
+    <hyperlink ref="A77" r:id="rId20" xr:uid="{ABD9644B-2379-4071-A0CA-3BF1DAFBAE14}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
God knows what I did here
</commit_message>
<xml_diff>
--- a/development/Integrated Mods.xlsx
+++ b/development/Integrated Mods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\S.T.A.L.K.E.R\Anomaly Mods\mods\Back-to-roots-wip\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578A4824-F243-4BA7-87C3-B20EAE4C7D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5E57D3-8EFD-4D25-853E-F617D7E34074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="143">
   <si>
     <t>Filename</t>
   </si>
@@ -417,13 +417,61 @@
   </si>
   <si>
     <t>xrs_facer.script</t>
+  </si>
+  <si>
+    <t>Disable Burnt Fuzz</t>
+  </si>
+  <si>
+    <t>configs/zones/</t>
+  </si>
+  <si>
+    <t>zone_burningfuzz.ltx</t>
+  </si>
+  <si>
+    <t>Companion Tweaks</t>
+  </si>
+  <si>
+    <t>configs/misc/</t>
+  </si>
+  <si>
+    <t>story_npc_carryweights.ltx</t>
+  </si>
+  <si>
+    <t>dynamic_companion_carryweight.script</t>
+  </si>
+  <si>
+    <t>Faction Identification UI</t>
+  </si>
+  <si>
+    <t>Grokitach</t>
+  </si>
+  <si>
+    <t>ui_st_factionID.xml</t>
+  </si>
+  <si>
+    <t>ui_patches.xml</t>
+  </si>
+  <si>
+    <t>factionID_hud_mcm.script</t>
+  </si>
+  <si>
+    <t>textures/id/</t>
+  </si>
+  <si>
+    <t>Xanotech Behavior</t>
+  </si>
+  <si>
+    <t>configs/scripts</t>
+  </si>
+  <si>
+    <t>(Bunch of ltx files)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -462,6 +510,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -626,8 +681,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -692,8 +748,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1030,16 +1101,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8700934C-DA8F-46A3-9CCC-A5B0203FB02B}">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84:E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="48.5703125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="48.5703125" style="24" customWidth="1"/>
     <col min="3" max="3" width="36.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" customWidth="1"/>
@@ -1047,1119 +1118,1304 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="30" t="s">
+      <c r="D2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="31" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="18" t="s">
+      <c r="A3" s="28"/>
+      <c r="B3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="31"/>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="32"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="C4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="31" t="s">
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="32" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="17" t="s">
+      <c r="A6" s="28"/>
+      <c r="B6" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="31"/>
+      <c r="C6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="18" t="s">
+      <c r="A7" s="28"/>
+      <c r="B7" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="31"/>
+      <c r="D7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="32"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="17" t="s">
+      <c r="A8" s="28"/>
+      <c r="B8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="31"/>
+      <c r="D8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="32"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="18" t="s">
+      <c r="A9" s="28"/>
+      <c r="B9" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="31"/>
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="32"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="17" t="s">
+      <c r="A10" s="28"/>
+      <c r="B10" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="31"/>
+      <c r="D10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="32"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="18" t="s">
+      <c r="A11" s="28"/>
+      <c r="B11" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="31"/>
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="32"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="17" t="s">
+      <c r="A12" s="28"/>
+      <c r="B12" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="31"/>
+      <c r="D12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="32"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="18" t="s">
+      <c r="A13" s="28"/>
+      <c r="B13" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="31"/>
+      <c r="D13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="32"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="31"/>
+      <c r="D14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="32"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="18" t="s">
+      <c r="A15" s="26"/>
+      <c r="B15" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="31"/>
+      <c r="C15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="32"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="17" t="s">
+      <c r="A16" s="26"/>
+      <c r="B16" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="31"/>
+      <c r="C16" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="32"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="18" t="s">
+      <c r="A17" s="26"/>
+      <c r="B17" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="31"/>
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="32"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="17" t="s">
+      <c r="A18" s="26"/>
+      <c r="B18" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="31"/>
+      <c r="D18" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="32"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="18" t="s">
+      <c r="A19" s="26"/>
+      <c r="B19" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="31"/>
+      <c r="D19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="32"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="17" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="31"/>
+      <c r="D20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="32"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
-      <c r="B21" s="18" t="s">
+      <c r="A21" s="26"/>
+      <c r="B21" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="31"/>
+      <c r="E21" s="32"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="17" t="s">
+      <c r="A22" s="26"/>
+      <c r="B22" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="31"/>
+      <c r="D22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="32"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="18" t="s">
+      <c r="A23" s="26"/>
+      <c r="B23" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="31"/>
+      <c r="D23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="32"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="17" t="s">
+      <c r="A24" s="26"/>
+      <c r="B24" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="31"/>
+      <c r="D24" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="32"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
-      <c r="B25" s="18" t="s">
+      <c r="A25" s="26"/>
+      <c r="B25" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="31"/>
+      <c r="D25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="32"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="12" t="s">
+      <c r="C26" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="31" t="s">
+      <c r="D27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="32" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
-      <c r="B28" s="20" t="s">
+      <c r="A28" s="26"/>
+      <c r="B28" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="31"/>
+      <c r="D28" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="32"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
-      <c r="B29" s="19" t="s">
+      <c r="A29" s="26"/>
+      <c r="B29" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="31"/>
+      <c r="D29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="32"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="12" t="s">
+      <c r="D30" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="13" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="31" t="s">
+      <c r="D31" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="32" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
-      <c r="B32" s="17" t="s">
+      <c r="A32" s="26"/>
+      <c r="B32" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="31"/>
+      <c r="D32" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="32"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
-      <c r="B33" s="21" t="s">
+      <c r="A33" s="26"/>
+      <c r="B33" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E33" s="31"/>
+      <c r="E33" s="32"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
-      <c r="B34" s="22" t="s">
+      <c r="A34" s="26"/>
+      <c r="B34" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="29"/>
-      <c r="D34" s="24" t="s">
+      <c r="C34" s="30"/>
+      <c r="D34" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="E34" s="31"/>
+      <c r="E34" s="32"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
-      <c r="B35" s="21" t="s">
+      <c r="A35" s="26"/>
+      <c r="B35" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C35" s="29"/>
-      <c r="D35" s="15" t="s">
+      <c r="C35" s="30"/>
+      <c r="D35" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E35" s="31"/>
+      <c r="E35" s="32"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="25"/>
-      <c r="B36" s="22" t="s">
+      <c r="A36" s="26"/>
+      <c r="B36" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="29"/>
-      <c r="D36" s="24" t="s">
+      <c r="C36" s="30"/>
+      <c r="D36" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="E36" s="31"/>
+      <c r="E36" s="32"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="18" t="s">
+      <c r="A37" s="26"/>
+      <c r="B37" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="31"/>
+      <c r="D37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="32"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
-      <c r="B38" s="17" t="s">
+      <c r="A38" s="26"/>
+      <c r="B38" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="31"/>
+      <c r="C38" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="32"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
-      <c r="B39" s="18" t="s">
+      <c r="A39" s="26"/>
+      <c r="B39" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C39" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="31"/>
+      <c r="C39" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="32"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
-      <c r="B40" s="17" t="s">
+      <c r="A40" s="26"/>
+      <c r="B40" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="31"/>
+      <c r="C40" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="32"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="25"/>
-      <c r="B41" s="18" t="s">
+      <c r="A41" s="26"/>
+      <c r="B41" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C41" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" s="31"/>
+      <c r="C41" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="32"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
-      <c r="B42" s="20" t="s">
+      <c r="A42" s="26"/>
+      <c r="B42" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D42" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" s="31"/>
+      <c r="D42" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="32"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
-      <c r="B43" s="18" t="s">
+      <c r="A43" s="26"/>
+      <c r="B43" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" s="31"/>
+      <c r="D43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="32"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D44" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="32" t="s">
+      <c r="D44" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="33" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="27"/>
-      <c r="B45" s="18" t="s">
+      <c r="A45" s="28"/>
+      <c r="B45" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="32"/>
+      <c r="D45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="33"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="27"/>
-      <c r="B46" s="17" t="s">
+      <c r="A46" s="28"/>
+      <c r="B46" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="32"/>
+      <c r="D46" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="33"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="27"/>
-      <c r="B47" s="18" t="s">
+      <c r="A47" s="28"/>
+      <c r="B47" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="32"/>
+      <c r="D47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="33"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="27"/>
-      <c r="B48" s="17" t="s">
+      <c r="A48" s="28"/>
+      <c r="B48" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C48" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" s="32"/>
+      <c r="C48" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="33"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="27"/>
-      <c r="B49" s="18" t="s">
+      <c r="A49" s="28"/>
+      <c r="B49" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C49" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" s="32"/>
+      <c r="C49" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="33"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C50" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E50" s="13" t="s">
+      <c r="C50" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="14" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="27" t="s">
+      <c r="A51" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B51" s="18" t="s">
+      <c r="B51" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E51" s="32" t="s">
+      <c r="D51" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="33" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="27"/>
-      <c r="B52" s="17" t="s">
+      <c r="A52" s="28"/>
+      <c r="B52" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D52" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E52" s="32"/>
+      <c r="D52" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="33"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="27"/>
-      <c r="B53" s="18" t="s">
+      <c r="A53" s="28"/>
+      <c r="B53" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="32"/>
+      <c r="D53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="33"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="27"/>
-      <c r="B54" s="17" t="s">
+      <c r="A54" s="28"/>
+      <c r="B54" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C54" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D54" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E54" s="32"/>
+      <c r="D54" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="33"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="27"/>
-      <c r="B55" s="18" t="s">
+      <c r="A55" s="28"/>
+      <c r="B55" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E55" s="32"/>
+      <c r="D55" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="33"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="27"/>
-      <c r="B56" s="17" t="s">
+      <c r="A56" s="28"/>
+      <c r="B56" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C56" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E56" s="32"/>
+      <c r="C56" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="33"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="27"/>
-      <c r="B57" s="18" t="s">
+      <c r="A57" s="28"/>
+      <c r="B57" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C57" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E57" s="32"/>
+      <c r="C57" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="33"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="27"/>
-      <c r="B58" s="17" t="s">
+      <c r="A58" s="28"/>
+      <c r="B58" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C58" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E58" s="32"/>
+      <c r="C58" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="33"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="27"/>
-      <c r="B59" s="18" t="s">
+      <c r="A59" s="28"/>
+      <c r="B59" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C59" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E59" s="32"/>
+      <c r="C59" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="33"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="27"/>
-      <c r="B60" s="17" t="s">
+      <c r="A60" s="28"/>
+      <c r="B60" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C60" s="9" t="s">
+      <c r="C60" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D60" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E60" s="32"/>
+      <c r="D60" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="33"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="10" t="s">
+      <c r="A61" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B61" s="18" t="s">
+      <c r="B61" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C61" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E61" s="13" t="s">
+      <c r="D61" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="14" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="27" t="s">
+      <c r="A62" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="B62" s="17" t="s">
+      <c r="B62" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C62" s="9" t="s">
+      <c r="C62" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D62" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E62" s="32" t="s">
+      <c r="D62" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="33" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="27"/>
-      <c r="B63" s="18" t="s">
+      <c r="A63" s="28"/>
+      <c r="B63" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C63" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E63" s="32"/>
+      <c r="C63" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="33"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="27"/>
-      <c r="B64" s="17" t="s">
+      <c r="A64" s="28"/>
+      <c r="B64" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C64" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D64" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E64" s="32"/>
+      <c r="C64" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="33"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="27"/>
-      <c r="B65" s="18" t="s">
+      <c r="A65" s="28"/>
+      <c r="B65" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="C65" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E65" s="32"/>
+      <c r="C65" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="33"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="27"/>
-      <c r="B66" s="17" t="s">
+      <c r="A66" s="28"/>
+      <c r="B66" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C66" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D66" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E66" s="32"/>
+      <c r="C66" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" s="33"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="27"/>
-      <c r="B67" s="18" t="s">
+      <c r="A67" s="28"/>
+      <c r="B67" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="C67" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E67" s="32"/>
+      <c r="C67" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="33"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="27"/>
-      <c r="B68" s="17" t="s">
+      <c r="A68" s="28"/>
+      <c r="B68" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C68" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E68" s="32"/>
+      <c r="C68" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="33"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="10" t="s">
+      <c r="A69" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B69" s="18" t="s">
+      <c r="B69" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="C69" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E69" s="13" t="s">
+      <c r="C69" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" s="14" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
+      <c r="A70" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B70" s="17" t="s">
+      <c r="B70" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C70" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D70" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E70" s="12" t="s">
+      <c r="C70" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" s="13" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="B71" s="18" t="s">
+      <c r="B71" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C71" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E71" s="13" t="s">
+      <c r="C71" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" s="14" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="11" t="s">
+      <c r="A72" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="B72" s="33" t="s">
+      <c r="B72" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="C72" s="29" t="s">
+      <c r="C72" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="D72" s="24" t="s">
+      <c r="D72" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="E72" s="12" t="s">
+      <c r="E72" s="13" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="10" t="s">
+      <c r="A73" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="B73" s="33"/>
-      <c r="C73" s="29"/>
-      <c r="D73" s="15" t="s">
+      <c r="B73" s="38"/>
+      <c r="C73" s="30"/>
+      <c r="D73" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E73" s="13" t="s">
+      <c r="E73" s="14" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="27" t="s">
+      <c r="A74" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="B74" s="28" t="s">
+      <c r="B74" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="C74" s="9" t="s">
+      <c r="C74" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D74" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E74" s="32" t="s">
+      <c r="D74" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" s="33" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="27"/>
-      <c r="B75" s="18" t="s">
+      <c r="A75" s="28"/>
+      <c r="B75" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="C75" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E75" s="32"/>
+      <c r="C75" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E75" s="33"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="27"/>
-      <c r="B76" s="17" t="s">
+      <c r="A76" s="28"/>
+      <c r="B76" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C76" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D76" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E76" s="32"/>
+      <c r="C76" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" s="33"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="25" t="s">
+      <c r="A77" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="B77" s="18" t="s">
+      <c r="B77" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="C77" s="8" t="s">
+      <c r="C77" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E77" s="31" t="s">
+      <c r="D77" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" s="32" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="25"/>
-      <c r="B78" s="17" t="s">
+      <c r="A78" s="26"/>
+      <c r="B78" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="C78" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E78" s="31"/>
+      <c r="C78" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" s="32"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="25"/>
-      <c r="B79" s="18" t="s">
+      <c r="A79" s="26"/>
+      <c r="B79" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="C79" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E79" s="31"/>
+      <c r="C79" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79" s="32"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="25"/>
-      <c r="B80" s="17" t="s">
+      <c r="A80" s="26"/>
+      <c r="B80" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C80" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E80" s="31"/>
+      <c r="C80" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80" s="32"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B81" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" s="1"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="B82" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" s="36"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="37"/>
+      <c r="B83" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" s="36"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="B84" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="C84" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E84" s="39" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="39"/>
+      <c r="B85" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E85" s="39"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="39"/>
+      <c r="B86" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E86" s="39"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="39"/>
+      <c r="B87" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E87" s="39"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="39"/>
+      <c r="B88" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C88" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E88" s="39"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B89" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B90" s="35"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="8"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B91" s="34"/>
+      <c r="C91" s="9"/>
+      <c r="D91" s="3"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B92" s="35"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="8"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B93" s="34"/>
+      <c r="C93" s="9"/>
+      <c r="D93" s="3"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B94" s="35"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="8"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B95" s="34"/>
+      <c r="C95" s="9"/>
+      <c r="D95" s="3"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B96" s="35"/>
+      <c r="C96" s="10"/>
+      <c r="D96" s="8"/>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="34"/>
+      <c r="C97" s="9"/>
+      <c r="D97" s="3"/>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="35"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="8"/>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="34"/>
+      <c r="C99" s="9"/>
+      <c r="D99" s="3"/>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="35"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="26">
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="A84:A88"/>
+    <mergeCell ref="E84:E88"/>
     <mergeCell ref="A74:A76"/>
     <mergeCell ref="E74:E76"/>
     <mergeCell ref="E62:E68"/>
@@ -2204,7 +2460,9 @@
     <hyperlink ref="A74" r:id="rId18" xr:uid="{3B22816C-344C-494A-9DEE-E1DCBFD8E1DB}"/>
     <hyperlink ref="A73" r:id="rId19" xr:uid="{3C0C31EC-2080-40A3-A100-ABA2FB6F399B}"/>
     <hyperlink ref="A77" r:id="rId20" xr:uid="{ABD9644B-2379-4071-A0CA-3BF1DAFBAE14}"/>
+    <hyperlink ref="A89" r:id="rId21" xr:uid="{92668D3C-4260-4890-BCB5-25F8810B0A07}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lots of other stuff
</commit_message>
<xml_diff>
--- a/development/Integrated Mods.xlsx
+++ b/development/Integrated Mods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\S.T.A.L.K.E.R\Anomaly Mods\mods\Back-to-roots-wip\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B48D8A4-B5CF-40B2-938F-6A3E9F6F3588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8094BA8A-D7D4-49B5-817F-16FB32326BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15645" windowHeight="15600" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
+    <workbookView xWindow="75" yWindow="0" windowWidth="16140" windowHeight="15600" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="190">
   <si>
     <t>Filename</t>
   </si>
@@ -546,6 +546,66 @@
   </si>
   <si>
     <t>_STYX_</t>
+  </si>
+  <si>
+    <t>Companion Inventory Unlock</t>
+  </si>
+  <si>
+    <t>aaaanon</t>
+  </si>
+  <si>
+    <t>ui_st_companion_inventory_fix.xml</t>
+  </si>
+  <si>
+    <t>rax_persistent_highlight.script</t>
+  </si>
+  <si>
+    <t>zz_companion_inventory_fix_mcm.script</t>
+  </si>
+  <si>
+    <t>MotZ_dialogue_unlocker</t>
+  </si>
+  <si>
+    <t>configs/gameplay/</t>
+  </si>
+  <si>
+    <t>character_desc_marsh.xml</t>
+  </si>
+  <si>
+    <t>Hisalute</t>
+  </si>
+  <si>
+    <t>zz_parts_in_tooltip.script</t>
+  </si>
+  <si>
+    <t>Parts in tooltip mod</t>
+  </si>
+  <si>
+    <t>FF Response and Actor Surrender</t>
+  </si>
+  <si>
+    <t>gameplay_surrender_friendly_fire.script</t>
+  </si>
+  <si>
+    <t>modxml_ui_custom_msgs_aggravation_bar.script</t>
+  </si>
+  <si>
+    <t>SFSS</t>
+  </si>
+  <si>
+    <t>configs/creatures/</t>
+  </si>
+  <si>
+    <t>m_stalker.ltx</t>
+  </si>
+  <si>
+    <t>xr_combat_ignore.script</t>
+  </si>
+  <si>
+    <t>gameplay_disguise.script</t>
+  </si>
+  <si>
+    <t>Undercover Communication</t>
   </si>
 </sst>
 </file>
@@ -768,7 +828,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -848,14 +908,32 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1192,15 +1270,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8700934C-DA8F-46A3-9CCC-A5B0203FB02B}">
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F117" sqref="F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="48.5703125" style="21" customWidth="1"/>
     <col min="3" max="3" width="36.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
@@ -2338,7 +2416,7 @@
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="40" t="s">
+      <c r="A82" s="44" t="s">
         <v>130</v>
       </c>
       <c r="B82" s="25" t="s">
@@ -2355,7 +2433,7 @@
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="40"/>
+      <c r="A83" s="44"/>
       <c r="B83" s="24" t="s">
         <v>133</v>
       </c>
@@ -2368,7 +2446,7 @@
       <c r="E83" s="38"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="41" t="s">
+      <c r="A84" s="45" t="s">
         <v>134</v>
       </c>
       <c r="B84" s="25" t="s">
@@ -2380,12 +2458,12 @@
       <c r="D84" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E84" s="39" t="s">
+      <c r="E84" s="40" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="41"/>
+      <c r="A85" s="45"/>
       <c r="B85" s="24" t="s">
         <v>136</v>
       </c>
@@ -2395,10 +2473,10 @@
       <c r="D85" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E85" s="39"/>
+      <c r="E85" s="40"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="41"/>
+      <c r="A86" s="45"/>
       <c r="B86" s="25" t="s">
         <v>137</v>
       </c>
@@ -2408,10 +2486,10 @@
       <c r="D86" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E86" s="39"/>
+      <c r="E86" s="40"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="41"/>
+      <c r="A87" s="45"/>
       <c r="B87" s="24" t="s">
         <v>138</v>
       </c>
@@ -2421,10 +2499,10 @@
       <c r="D87" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E87" s="39"/>
+      <c r="E87" s="40"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="41"/>
+      <c r="A88" s="45"/>
       <c r="B88" s="18" t="s">
         <v>19</v>
       </c>
@@ -2434,7 +2512,7 @@
       <c r="D88" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E88" s="39"/>
+      <c r="E88" s="40"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
@@ -2488,7 +2566,7 @@
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="41" t="s">
+      <c r="A92" s="45" t="s">
         <v>149</v>
       </c>
       <c r="B92" s="25" t="s">
@@ -2500,12 +2578,12 @@
       <c r="D92" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E92" s="39" t="s">
+      <c r="E92" s="40" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="41"/>
+      <c r="A93" s="45"/>
       <c r="B93" s="24" t="s">
         <v>152</v>
       </c>
@@ -2515,10 +2593,10 @@
       <c r="D93" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E93" s="39"/>
+      <c r="E93" s="40"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="41"/>
+      <c r="A94" s="45"/>
       <c r="B94" s="25" t="s">
         <v>153</v>
       </c>
@@ -2528,10 +2606,10 @@
       <c r="D94" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E94" s="39"/>
+      <c r="E94" s="40"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="41"/>
+      <c r="A95" s="45"/>
       <c r="B95" s="24" t="s">
         <v>154</v>
       </c>
@@ -2541,10 +2619,10 @@
       <c r="D95" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E95" s="39"/>
+      <c r="E95" s="40"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="41"/>
+      <c r="A96" s="45"/>
       <c r="B96" s="25" t="s">
         <v>155</v>
       </c>
@@ -2554,10 +2632,10 @@
       <c r="D96" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E96" s="39"/>
+      <c r="E96" s="40"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="41"/>
+      <c r="A97" s="45"/>
       <c r="B97" s="24" t="s">
         <v>156</v>
       </c>
@@ -2567,10 +2645,10 @@
       <c r="D97" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E97" s="39"/>
+      <c r="E97" s="40"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="40" t="s">
+      <c r="A98" s="44" t="s">
         <v>157</v>
       </c>
       <c r="B98" s="25" t="s">
@@ -2587,7 +2665,7 @@
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="40"/>
+      <c r="A99" s="44"/>
       <c r="B99" s="24" t="s">
         <v>158</v>
       </c>
@@ -2600,7 +2678,7 @@
       <c r="E99" s="38"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="40"/>
+      <c r="A100" s="44"/>
       <c r="B100" s="25" t="s">
         <v>159</v>
       </c>
@@ -2613,7 +2691,7 @@
       <c r="E100" s="38"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="40"/>
+      <c r="A101" s="44"/>
       <c r="B101" s="24" t="s">
         <v>160</v>
       </c>
@@ -2626,7 +2704,7 @@
       <c r="E101" s="38"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="40"/>
+      <c r="A102" s="44"/>
       <c r="B102" s="25" t="s">
         <v>161</v>
       </c>
@@ -2639,7 +2717,7 @@
       <c r="E102" s="38"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="40"/>
+      <c r="A103" s="44"/>
       <c r="B103" s="17" t="s">
         <v>163</v>
       </c>
@@ -2652,37 +2730,212 @@
       <c r="E103" s="38"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B104" s="25"/>
-      <c r="C104" s="8"/>
-      <c r="D104" s="6"/>
+      <c r="A104" s="45" t="s">
+        <v>170</v>
+      </c>
+      <c r="B104" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E104" s="40" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B105" s="24"/>
-      <c r="C105" s="7"/>
-      <c r="D105" s="3"/>
+      <c r="A105" s="45"/>
+      <c r="B105" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" s="40"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B106" s="25"/>
-      <c r="C106" s="8"/>
-      <c r="D106" s="6"/>
+      <c r="A106" s="45"/>
+      <c r="B106" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E106" s="40"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B107" s="24"/>
-      <c r="C107" s="7"/>
-      <c r="D107" s="3"/>
+      <c r="A107" s="45"/>
+      <c r="B107" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E107" s="40"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B108" s="25"/>
-      <c r="C108" s="8"/>
-      <c r="D108" s="6"/>
+      <c r="A108" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B108" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="C108" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E108" s="43" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B109" s="24"/>
-      <c r="C109" s="7"/>
-      <c r="D109" s="3"/>
+      <c r="A109" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B109" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E109" s="42"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="B110" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="C110" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E110" s="39"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="38"/>
+      <c r="B111" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E111" s="39"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="B112" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="C112" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E112" s="41"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="40"/>
+      <c r="B113" s="47" t="s">
+        <v>187</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E113" s="41"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="B114" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="C114" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E114" s="26"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D115" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D116" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D117" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D118" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D119" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D120" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D121" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D122" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="36">
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="E112:E113"/>
+    <mergeCell ref="A104:A107"/>
+    <mergeCell ref="E104:E107"/>
+    <mergeCell ref="A110:A111"/>
+    <mergeCell ref="E110:E111"/>
     <mergeCell ref="E92:E97"/>
     <mergeCell ref="A92:A97"/>
     <mergeCell ref="E98:E103"/>
@@ -2743,8 +2996,10 @@
     <hyperlink ref="A82:A83" r:id="rId26" display="Companion Tweaks" xr:uid="{CF434ECD-6EEF-4AC0-BCCD-B6BE22DD1DAD}"/>
     <hyperlink ref="A84:A88" r:id="rId27" display="Faction Identification UI" xr:uid="{C1669F17-A49B-46A7-8935-937FC40B07C8}"/>
     <hyperlink ref="A81" r:id="rId28" xr:uid="{95C2A189-284D-4C96-A9E9-A540B49A9BA8}"/>
+    <hyperlink ref="A104:A107" r:id="rId29" display="Companion Inventory Unlock" xr:uid="{4142B9D6-B95F-482F-BD3F-A9EDB9C78FD5}"/>
+    <hyperlink ref="A108" r:id="rId30" xr:uid="{142E6B99-C7A8-42F1-833F-F6B912146B8D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId29"/>
+  <pageSetup orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Integrated hit impulse restored
</commit_message>
<xml_diff>
--- a/development/Integrated Mods.xlsx
+++ b/development/Integrated Mods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\S.T.A.L.K.E.R\Anomaly Mods\mods\Back-to-roots-wip\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1929FD-6C75-4A3E-9CEC-815F9AF4C7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA18FCB-5950-42B7-86DF-0F5D40B85E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
   </bookViews>
@@ -1287,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8700934C-DA8F-46A3-9CCC-A5B0203FB02B}">
   <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H87" sqref="H87"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
God have mercy on my soul
</commit_message>
<xml_diff>
--- a/development/Integrated Mods.xlsx
+++ b/development/Integrated Mods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\S.T.A.L.K.E.R\Anomaly Mods\mods\Back-to-roots-wip\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA18FCB-5950-42B7-86DF-0F5D40B85E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF889742-0CE4-499C-AD9A-3E86FE657756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="196">
   <si>
     <t>Filename</t>
   </si>
@@ -621,6 +621,9 @@
   </si>
   <si>
     <t>npc_fleeing_mcm.script</t>
+  </si>
+  <si>
+    <t>utils_ui_icon_rotation_fix_mcm.script</t>
   </si>
 </sst>
 </file>
@@ -843,7 +846,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -896,6 +899,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1285,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8700934C-DA8F-46A3-9CCC-A5B0203FB02B}">
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,7 +1328,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="49" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="15" t="s">
@@ -1331,12 +1340,12 @@
       <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="48" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
+      <c r="A3" s="42"/>
       <c r="B3" s="16" t="s">
         <v>12</v>
       </c>
@@ -1346,7 +1355,7 @@
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="43"/>
+      <c r="E3" s="45"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -1366,7 +1375,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="42" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="17" t="s">
@@ -1378,12 +1387,12 @@
       <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="45" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="15" t="s">
         <v>20</v>
       </c>
@@ -1393,10 +1402,10 @@
       <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="43"/>
+      <c r="E6" s="45"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="16" t="s">
         <v>22</v>
       </c>
@@ -1406,10 +1415,10 @@
       <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="43"/>
+      <c r="E7" s="45"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="15" t="s">
         <v>23</v>
       </c>
@@ -1419,10 +1428,10 @@
       <c r="D8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="43"/>
+      <c r="E8" s="45"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="16" t="s">
         <v>24</v>
       </c>
@@ -1432,10 +1441,10 @@
       <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="43"/>
+      <c r="E9" s="45"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="15" t="s">
         <v>25</v>
       </c>
@@ -1445,10 +1454,10 @@
       <c r="D10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="43"/>
+      <c r="E10" s="45"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="16" t="s">
         <v>26</v>
       </c>
@@ -1458,10 +1467,10 @@
       <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="43"/>
+      <c r="E11" s="45"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
+      <c r="A12" s="42"/>
       <c r="B12" s="15" t="s">
         <v>25</v>
       </c>
@@ -1471,10 +1480,10 @@
       <c r="D12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="43"/>
+      <c r="E12" s="45"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="16" t="s">
         <v>26</v>
       </c>
@@ -1484,10 +1493,10 @@
       <c r="D13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="43"/>
+      <c r="E13" s="45"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="44" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="18" t="s">
@@ -1499,10 +1508,10 @@
       <c r="D14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="43"/>
+      <c r="E14" s="45"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="16" t="s">
         <v>31</v>
       </c>
@@ -1512,10 +1521,10 @@
       <c r="D15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="43"/>
+      <c r="E15" s="45"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="15" t="s">
         <v>32</v>
       </c>
@@ -1525,10 +1534,10 @@
       <c r="D16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="43"/>
+      <c r="E16" s="45"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="16" t="s">
         <v>33</v>
       </c>
@@ -1538,10 +1547,10 @@
       <c r="D17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="43"/>
+      <c r="E17" s="45"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="42"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="15" t="s">
         <v>34</v>
       </c>
@@ -1551,10 +1560,10 @@
       <c r="D18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="43"/>
+      <c r="E18" s="45"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="16" t="s">
         <v>35</v>
       </c>
@@ -1564,10 +1573,10 @@
       <c r="D19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="43"/>
+      <c r="E19" s="45"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="15" t="s">
         <v>36</v>
       </c>
@@ -1577,10 +1586,10 @@
       <c r="D20" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="43"/>
+      <c r="E20" s="45"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
+      <c r="A21" s="44"/>
       <c r="B21" s="16" t="s">
         <v>37</v>
       </c>
@@ -1590,10 +1599,10 @@
       <c r="D21" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="43"/>
+      <c r="E21" s="45"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
+      <c r="A22" s="44"/>
       <c r="B22" s="15" t="s">
         <v>38</v>
       </c>
@@ -1603,10 +1612,10 @@
       <c r="D22" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="43"/>
+      <c r="E22" s="45"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
+      <c r="A23" s="44"/>
       <c r="B23" s="16" t="s">
         <v>39</v>
       </c>
@@ -1616,10 +1625,10 @@
       <c r="D23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="43"/>
+      <c r="E23" s="45"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="15" t="s">
         <v>40</v>
       </c>
@@ -1629,10 +1638,10 @@
       <c r="D24" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="43"/>
+      <c r="E24" s="45"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="16" t="s">
         <v>40</v>
       </c>
@@ -1642,7 +1651,7 @@
       <c r="D25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="43"/>
+      <c r="E25" s="45"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
@@ -1662,7 +1671,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="44" t="s">
         <v>45</v>
       </c>
       <c r="B27" s="17" t="s">
@@ -1674,12 +1683,12 @@
       <c r="D27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="43" t="s">
+      <c r="E27" s="45" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="18" t="s">
         <v>19</v>
       </c>
@@ -1689,10 +1698,10 @@
       <c r="D28" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="43"/>
+      <c r="E28" s="45"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="42"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="17" t="s">
         <v>19</v>
       </c>
@@ -1702,7 +1711,7 @@
       <c r="D29" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="43"/>
+      <c r="E29" s="45"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
@@ -1722,7 +1731,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="42" t="s">
+      <c r="A31" s="44" t="s">
         <v>54</v>
       </c>
       <c r="B31" s="16" t="s">
@@ -1734,12 +1743,12 @@
       <c r="D31" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="43" t="s">
+      <c r="E31" s="45" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="42"/>
+      <c r="A32" s="44"/>
       <c r="B32" s="15" t="s">
         <v>56</v>
       </c>
@@ -1749,56 +1758,56 @@
       <c r="D32" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="43"/>
+      <c r="E32" s="45"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="42"/>
+      <c r="A33" s="44"/>
       <c r="B33" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="44" t="s">
+      <c r="C33" s="46" t="s">
         <v>63</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="E33" s="43"/>
+      <c r="E33" s="45"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="42"/>
+      <c r="A34" s="44"/>
       <c r="B34" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="44"/>
+      <c r="C34" s="46"/>
       <c r="D34" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="E34" s="43"/>
+      <c r="E34" s="45"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="42"/>
+      <c r="A35" s="44"/>
       <c r="B35" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C35" s="44"/>
+      <c r="C35" s="46"/>
       <c r="D35" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="E35" s="43"/>
+      <c r="E35" s="45"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="42"/>
+      <c r="A36" s="44"/>
       <c r="B36" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="44"/>
+      <c r="C36" s="46"/>
       <c r="D36" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="E36" s="43"/>
+      <c r="E36" s="45"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="42"/>
+      <c r="A37" s="44"/>
       <c r="B37" s="16" t="s">
         <v>62</v>
       </c>
@@ -1808,10 +1817,10 @@
       <c r="D37" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="43"/>
+      <c r="E37" s="45"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="42"/>
+      <c r="A38" s="44"/>
       <c r="B38" s="15" t="s">
         <v>64</v>
       </c>
@@ -1821,10 +1830,10 @@
       <c r="D38" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="43"/>
+      <c r="E38" s="45"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="42"/>
+      <c r="A39" s="44"/>
       <c r="B39" s="16" t="s">
         <v>65</v>
       </c>
@@ -1834,10 +1843,10 @@
       <c r="D39" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E39" s="43"/>
+      <c r="E39" s="45"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="42"/>
+      <c r="A40" s="44"/>
       <c r="B40" s="15" t="s">
         <v>66</v>
       </c>
@@ -1847,10 +1856,10 @@
       <c r="D40" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="43"/>
+      <c r="E40" s="45"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="42"/>
+      <c r="A41" s="44"/>
       <c r="B41" s="16" t="s">
         <v>67</v>
       </c>
@@ -1860,10 +1869,10 @@
       <c r="D41" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E41" s="43"/>
+      <c r="E41" s="45"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="42"/>
+      <c r="A42" s="44"/>
       <c r="B42" s="18" t="s">
         <v>19</v>
       </c>
@@ -1873,10 +1882,10 @@
       <c r="D42" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="43"/>
+      <c r="E42" s="45"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="42"/>
+      <c r="A43" s="44"/>
       <c r="B43" s="16" t="s">
         <v>69</v>
       </c>
@@ -1886,10 +1895,10 @@
       <c r="D43" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E43" s="43"/>
+      <c r="E43" s="45"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="40" t="s">
+      <c r="A44" s="42" t="s">
         <v>71</v>
       </c>
       <c r="B44" s="15" t="s">
@@ -1901,12 +1910,12 @@
       <c r="D44" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E44" s="41" t="s">
+      <c r="E44" s="43" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="40"/>
+      <c r="A45" s="42"/>
       <c r="B45" s="16" t="s">
         <v>73</v>
       </c>
@@ -1916,10 +1925,10 @@
       <c r="D45" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E45" s="41"/>
+      <c r="E45" s="43"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="40"/>
+      <c r="A46" s="42"/>
       <c r="B46" s="15" t="s">
         <v>74</v>
       </c>
@@ -1929,10 +1938,10 @@
       <c r="D46" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E46" s="41"/>
+      <c r="E46" s="43"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="40"/>
+      <c r="A47" s="42"/>
       <c r="B47" s="16" t="s">
         <v>75</v>
       </c>
@@ -1942,10 +1951,10 @@
       <c r="D47" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E47" s="41"/>
+      <c r="E47" s="43"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="40"/>
+      <c r="A48" s="42"/>
       <c r="B48" s="15" t="s">
         <v>76</v>
       </c>
@@ -1955,10 +1964,10 @@
       <c r="D48" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E48" s="41"/>
+      <c r="E48" s="43"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="40"/>
+      <c r="A49" s="42"/>
       <c r="B49" s="16" t="s">
         <v>77</v>
       </c>
@@ -1968,7 +1977,7 @@
       <c r="D49" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="41"/>
+      <c r="E49" s="43"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
@@ -1988,7 +1997,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="40" t="s">
+      <c r="A51" s="42" t="s">
         <v>80</v>
       </c>
       <c r="B51" s="16" t="s">
@@ -2000,12 +2009,12 @@
       <c r="D51" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E51" s="41" t="s">
+      <c r="E51" s="43" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="40"/>
+      <c r="A52" s="42"/>
       <c r="B52" s="15" t="s">
         <v>84</v>
       </c>
@@ -2015,10 +2024,10 @@
       <c r="D52" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E52" s="41"/>
+      <c r="E52" s="43"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="40"/>
+      <c r="A53" s="42"/>
       <c r="B53" s="16" t="s">
         <v>84</v>
       </c>
@@ -2028,10 +2037,10 @@
       <c r="D53" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E53" s="41"/>
+      <c r="E53" s="43"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="40"/>
+      <c r="A54" s="42"/>
       <c r="B54" s="15" t="s">
         <v>85</v>
       </c>
@@ -2041,10 +2050,10 @@
       <c r="D54" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E54" s="41"/>
+      <c r="E54" s="43"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="40"/>
+      <c r="A55" s="42"/>
       <c r="B55" s="16" t="s">
         <v>86</v>
       </c>
@@ -2054,10 +2063,10 @@
       <c r="D55" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E55" s="41"/>
+      <c r="E55" s="43"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="40"/>
+      <c r="A56" s="42"/>
       <c r="B56" s="15" t="s">
         <v>87</v>
       </c>
@@ -2067,10 +2076,10 @@
       <c r="D56" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E56" s="41"/>
+      <c r="E56" s="43"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="40"/>
+      <c r="A57" s="42"/>
       <c r="B57" s="16" t="s">
         <v>88</v>
       </c>
@@ -2080,10 +2089,10 @@
       <c r="D57" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E57" s="41"/>
+      <c r="E57" s="43"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="40"/>
+      <c r="A58" s="42"/>
       <c r="B58" s="15" t="s">
         <v>89</v>
       </c>
@@ -2093,10 +2102,10 @@
       <c r="D58" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E58" s="41"/>
+      <c r="E58" s="43"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="40"/>
+      <c r="A59" s="42"/>
       <c r="B59" s="16" t="s">
         <v>90</v>
       </c>
@@ -2106,10 +2115,10 @@
       <c r="D59" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E59" s="41"/>
+      <c r="E59" s="43"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="40"/>
+      <c r="A60" s="42"/>
       <c r="B60" s="15" t="s">
         <v>92</v>
       </c>
@@ -2119,7 +2128,7 @@
       <c r="D60" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E60" s="41"/>
+      <c r="E60" s="43"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
@@ -2139,7 +2148,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="40" t="s">
+      <c r="A62" s="42" t="s">
         <v>97</v>
       </c>
       <c r="B62" s="15" t="s">
@@ -2151,12 +2160,12 @@
       <c r="D62" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E62" s="41" t="s">
+      <c r="E62" s="43" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="40"/>
+      <c r="A63" s="42"/>
       <c r="B63" s="16" t="s">
         <v>99</v>
       </c>
@@ -2166,10 +2175,10 @@
       <c r="D63" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E63" s="41"/>
+      <c r="E63" s="43"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="40"/>
+      <c r="A64" s="42"/>
       <c r="B64" s="15" t="s">
         <v>100</v>
       </c>
@@ -2179,10 +2188,10 @@
       <c r="D64" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E64" s="41"/>
+      <c r="E64" s="43"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="40"/>
+      <c r="A65" s="42"/>
       <c r="B65" s="16" t="s">
         <v>101</v>
       </c>
@@ -2192,10 +2201,10 @@
       <c r="D65" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="41"/>
+      <c r="E65" s="43"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="40"/>
+      <c r="A66" s="42"/>
       <c r="B66" s="15" t="s">
         <v>102</v>
       </c>
@@ -2205,10 +2214,10 @@
       <c r="D66" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E66" s="41"/>
+      <c r="E66" s="43"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="40"/>
+      <c r="A67" s="42"/>
       <c r="B67" s="16" t="s">
         <v>103</v>
       </c>
@@ -2218,10 +2227,10 @@
       <c r="D67" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E67" s="41"/>
+      <c r="E67" s="43"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="40"/>
+      <c r="A68" s="42"/>
       <c r="B68" s="15" t="s">
         <v>104</v>
       </c>
@@ -2231,7 +2240,7 @@
       <c r="D68" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E68" s="41"/>
+      <c r="E68" s="43"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
@@ -2288,10 +2297,10 @@
       <c r="A72" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="B72" s="45" t="s">
+      <c r="B72" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="C72" s="44" t="s">
+      <c r="C72" s="46" t="s">
         <v>117</v>
       </c>
       <c r="D72" s="22" t="s">
@@ -2302,691 +2311,704 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="9" t="s">
+      <c r="A73" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="B73" s="45"/>
-      <c r="C73" s="44"/>
+      <c r="B73" s="47"/>
+      <c r="C73" s="46"/>
       <c r="D73" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E73" s="12" t="s">
+      <c r="E73" s="45" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="40" t="s">
+      <c r="A74" s="44"/>
+      <c r="B74" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="C74" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D74" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E74" s="45"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="B74" s="23" t="s">
+      <c r="B75" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="C74" s="8" t="s">
+      <c r="C75" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="D74" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E74" s="41" t="s">
+      <c r="D75" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E75" s="43" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="40"/>
-      <c r="B75" s="16" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="42"/>
+      <c r="B76" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="C75" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E75" s="41"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="40"/>
-      <c r="B76" s="15" t="s">
+      <c r="C76" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" s="43"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="42"/>
+      <c r="B77" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="C76" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E76" s="41"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="42" t="s">
+      <c r="C77" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" s="43"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="B77" s="16" t="s">
+      <c r="B78" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C77" s="7" t="s">
+      <c r="C78" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D77" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E77" s="43" t="s">
+      <c r="D78" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" s="45" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="42"/>
-      <c r="B78" s="15" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="44"/>
+      <c r="B79" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C78" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E78" s="43"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="42"/>
-      <c r="B79" s="16" t="s">
+      <c r="C79" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79" s="45"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="44"/>
+      <c r="B80" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="C79" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E79" s="43"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="42"/>
-      <c r="B80" s="15" t="s">
+      <c r="C80" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80" s="45"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="44"/>
+      <c r="B81" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="C80" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E80" s="43"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="10" t="s">
+      <c r="C81" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" s="45"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B81" s="24" t="s">
+      <c r="B82" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="C81" s="7" t="s">
+      <c r="C82" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="D81" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E81" s="1" t="s">
+      <c r="D82" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="39" t="s">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="B82" s="25" t="s">
+      <c r="B83" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C82" s="8" t="s">
+      <c r="C83" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="D82" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E82" s="37" t="s">
+      <c r="D83" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" s="39" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="39"/>
-      <c r="B83" s="24" t="s">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="41"/>
+      <c r="B84" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="C83" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E83" s="37"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="36" t="s">
+      <c r="C84" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E84" s="39"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="B84" s="25" t="s">
+      <c r="B85" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="C84" s="8" t="s">
+      <c r="C85" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D84" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E84" s="34" t="s">
+      <c r="D85" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E85" s="36" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="36"/>
-      <c r="B85" s="24" t="s">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="38"/>
+      <c r="B86" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="C85" s="7" t="s">
+      <c r="C86" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D85" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E85" s="34"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="36"/>
-      <c r="B86" s="25" t="s">
+      <c r="D86" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E86" s="36"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="38"/>
+      <c r="B87" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="C86" s="8" t="s">
+      <c r="C87" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D86" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E86" s="34"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="36"/>
-      <c r="B87" s="24" t="s">
+      <c r="D87" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E87" s="36"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="38"/>
+      <c r="B88" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="C87" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D87" s="14" t="s">
+      <c r="C88" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D88" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E87" s="34"/>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="36"/>
-      <c r="B88" s="18" t="s">
+      <c r="E88" s="36"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="38"/>
+      <c r="B89" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C88" s="8" t="s">
+      <c r="C89" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="D88" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E88" s="34"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="9" t="s">
+      <c r="D89" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E89" s="36"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B89" s="17" t="s">
+      <c r="B90" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="C89" s="7" t="s">
+      <c r="C90" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D89" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E89" s="26" t="s">
+      <c r="D90" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E90" s="26" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="10" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="B90" s="18" t="s">
+      <c r="B91" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="C90" s="8" t="s">
+      <c r="C91" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="D90" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E90" s="1" t="s">
+      <c r="D91" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E91" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="9" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="B91" s="24" t="s">
+      <c r="B92" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="C91" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E91" s="26" t="s">
+      <c r="C92" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E92" s="26" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="36" t="s">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="B92" s="25" t="s">
+      <c r="B93" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="C92" s="8" t="s">
+      <c r="C93" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D92" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E92" s="34" t="s">
+      <c r="D93" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E93" s="36" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="36"/>
-      <c r="B93" s="24" t="s">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="38"/>
+      <c r="B94" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="C93" s="7" t="s">
+      <c r="C94" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D93" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E93" s="34"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="36"/>
-      <c r="B94" s="25" t="s">
+      <c r="D94" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E94" s="36"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="38"/>
+      <c r="B95" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="C94" s="8" t="s">
+      <c r="C95" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D94" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E94" s="34"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="36"/>
-      <c r="B95" s="24" t="s">
+      <c r="D95" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E95" s="36"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="38"/>
+      <c r="B96" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="C95" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E95" s="34"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="36"/>
-      <c r="B96" s="25" t="s">
+      <c r="C96" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E96" s="36"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="38"/>
+      <c r="B97" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="C96" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D96" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E96" s="34"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="36"/>
-      <c r="B97" s="24" t="s">
+      <c r="C97" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E97" s="36"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="38"/>
+      <c r="B98" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="C97" s="7" t="s">
+      <c r="C98" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D97" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E97" s="34"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="39" t="s">
+      <c r="D98" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E98" s="36"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="B98" s="25" t="s">
+      <c r="B99" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="C98" s="8" t="s">
+      <c r="C99" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D98" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E98" s="37" t="s">
+      <c r="D99" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E99" s="39" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="39"/>
-      <c r="B99" s="24" t="s">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="41"/>
+      <c r="B100" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="C99" s="7" t="s">
+      <c r="C100" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D99" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E99" s="37"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="39"/>
-      <c r="B100" s="25" t="s">
+      <c r="D100" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E100" s="39"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="41"/>
+      <c r="B101" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="C100" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D100" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E100" s="37"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="39"/>
-      <c r="B101" s="24" t="s">
+      <c r="C101" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E101" s="39"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="41"/>
+      <c r="B102" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="C101" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D101" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E101" s="37"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="39"/>
-      <c r="B102" s="25" t="s">
+      <c r="C102" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E102" s="39"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="41"/>
+      <c r="B103" s="25" t="s">
         <v>161</v>
       </c>
-      <c r="C102" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D102" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E102" s="37"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="39"/>
-      <c r="B103" s="17" t="s">
+      <c r="C103" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E103" s="39"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="41"/>
+      <c r="B104" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="C103" s="7" t="s">
+      <c r="C104" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="D103" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E103" s="37"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="36" t="s">
+      <c r="D104" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E104" s="39"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="B104" s="25" t="s">
+      <c r="B105" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="C104" s="8" t="s">
+      <c r="C105" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D104" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E104" s="34" t="s">
+      <c r="D105" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" s="36" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="36"/>
-      <c r="B105" s="24" t="s">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="38"/>
+      <c r="B106" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="C105" s="7" t="s">
+      <c r="C106" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D105" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E105" s="34"/>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="36"/>
-      <c r="B106" s="25" t="s">
+      <c r="D106" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E106" s="36"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="38"/>
+      <c r="B107" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="C106" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D106" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E106" s="34"/>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="36"/>
-      <c r="B107" s="24" t="s">
+      <c r="C107" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D107" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E107" s="36"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="38"/>
+      <c r="B108" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="C107" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E107" s="34"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="9" t="s">
+      <c r="C108" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E108" s="36"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="B108" s="25" t="s">
+      <c r="B109" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="C108" s="8" t="s">
+      <c r="C109" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="D108" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E108" s="31" t="s">
+      <c r="D109" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E109" s="33" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B109" s="24" t="s">
+      <c r="B110" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="C109" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D109" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E109" s="30"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="37" t="s">
+      <c r="C110" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E110" s="32"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="B110" s="25" t="s">
+      <c r="B111" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="C110" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D110" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E110" s="38"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="37"/>
-      <c r="B111" s="24" t="s">
+      <c r="C111" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E111" s="40"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="39"/>
+      <c r="B112" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="C111" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E111" s="38"/>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="34" t="s">
+      <c r="C112" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E112" s="40"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="B112" s="32" t="s">
+      <c r="B113" s="34" t="s">
         <v>186</v>
       </c>
-      <c r="C112" s="8" t="s">
+      <c r="C113" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="D112" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E112" s="35"/>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="34"/>
-      <c r="B113" s="33" t="s">
+      <c r="D113" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E113" s="37"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="36"/>
+      <c r="B114" s="35" t="s">
         <v>187</v>
       </c>
-      <c r="C113" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E113" s="35"/>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="26" t="s">
+      <c r="C114" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E114" s="37"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="26" t="s">
         <v>189</v>
       </c>
-      <c r="B114" s="25" t="s">
+      <c r="B115" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="C114" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D114" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E114" s="26"/>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="34" t="s">
+      <c r="C115" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E115" s="26"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="B115" s="33" t="s">
+      <c r="B116" s="35" t="s">
         <v>191</v>
       </c>
-      <c r="C115" s="7" t="s">
+      <c r="C116" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D115" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E115" s="35"/>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="34"/>
-      <c r="B116" s="25" t="s">
+      <c r="D116" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E116" s="37"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="36"/>
+      <c r="B117" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="C116" s="8" t="s">
+      <c r="C117" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D116" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E116" s="35"/>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" s="34"/>
-      <c r="B117" s="33" t="s">
+      <c r="D117" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E117" s="37"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="36"/>
+      <c r="B118" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="C117" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E117" s="35"/>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="34"/>
-      <c r="B118" s="25" t="s">
+      <c r="C118" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E118" s="37"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="36"/>
+      <c r="B119" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="C118" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D118" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E118" s="35"/>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="34"/>
-      <c r="B119" s="33" t="s">
+      <c r="C119" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D119" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E119" s="37"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="36"/>
+      <c r="B120" s="35" t="s">
         <v>194</v>
       </c>
-      <c r="C119" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D119" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E119" s="35"/>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D120" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="C120" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E120" s="37"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D121" s="3" t="s">
+      <c r="D121" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D122" s="6" t="s">
+      <c r="D122" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D123" s="6" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="40">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="A14:A25"/>
@@ -3003,28 +3025,30 @@
     <mergeCell ref="A44:A49"/>
     <mergeCell ref="A51:A60"/>
     <mergeCell ref="A62:A68"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="E74:E76"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="E75:E77"/>
     <mergeCell ref="E62:E68"/>
-    <mergeCell ref="A77:A80"/>
-    <mergeCell ref="E77:E80"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="E78:E81"/>
     <mergeCell ref="C72:C73"/>
-    <mergeCell ref="E92:E97"/>
-    <mergeCell ref="A92:A97"/>
-    <mergeCell ref="E98:E103"/>
-    <mergeCell ref="A98:A103"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="A84:A88"/>
-    <mergeCell ref="E84:E88"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="E112:E113"/>
-    <mergeCell ref="A115:A119"/>
-    <mergeCell ref="E115:E119"/>
-    <mergeCell ref="A104:A107"/>
-    <mergeCell ref="E104:E107"/>
-    <mergeCell ref="A110:A111"/>
-    <mergeCell ref="E110:E111"/>
+    <mergeCell ref="E93:E98"/>
+    <mergeCell ref="A93:A98"/>
+    <mergeCell ref="E99:E104"/>
+    <mergeCell ref="A99:A104"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="E83:E84"/>
+    <mergeCell ref="A85:A89"/>
+    <mergeCell ref="E85:E89"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="E113:E114"/>
+    <mergeCell ref="A116:A120"/>
+    <mergeCell ref="E116:E120"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="E105:E108"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="E111:E112"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{D01E85B4-1DB0-475A-87DE-364916E7DA22}"/>
@@ -3044,19 +3068,19 @@
     <hyperlink ref="A70" r:id="rId15" xr:uid="{B95FD375-C58E-472D-A97A-585AACDC449F}"/>
     <hyperlink ref="A71" r:id="rId16" xr:uid="{68D48912-0729-4E51-951C-589C23D0AA49}"/>
     <hyperlink ref="A72" r:id="rId17" xr:uid="{AB056329-5430-4555-8CF3-98B3E35CFC48}"/>
-    <hyperlink ref="A74" r:id="rId18" xr:uid="{3B22816C-344C-494A-9DEE-E1DCBFD8E1DB}"/>
+    <hyperlink ref="A75" r:id="rId18" xr:uid="{3B22816C-344C-494A-9DEE-E1DCBFD8E1DB}"/>
     <hyperlink ref="A73" r:id="rId19" xr:uid="{3C0C31EC-2080-40A3-A100-ABA2FB6F399B}"/>
-    <hyperlink ref="A77" r:id="rId20" xr:uid="{ABD9644B-2379-4071-A0CA-3BF1DAFBAE14}"/>
-    <hyperlink ref="A89" r:id="rId21" xr:uid="{92668D3C-4260-4890-BCB5-25F8810B0A07}"/>
-    <hyperlink ref="A98:A103" r:id="rId22" display="Exo Servomotor Sounds" xr:uid="{4C647516-14B0-42EE-92BE-10C69BB93F13}"/>
-    <hyperlink ref="A92:A97" r:id="rId23" display="Campfire Healing" xr:uid="{428C437E-0CA8-499F-9462-F2EB9B7D4A46}"/>
-    <hyperlink ref="A91" r:id="rId24" xr:uid="{E66EB141-6133-4A7F-BD3E-0A04AEBD5D2D}"/>
-    <hyperlink ref="A90" r:id="rId25" xr:uid="{A12C9A94-1493-4038-9561-4B2EED259B4A}"/>
-    <hyperlink ref="A82:A83" r:id="rId26" display="Companion Tweaks" xr:uid="{CF434ECD-6EEF-4AC0-BCCD-B6BE22DD1DAD}"/>
-    <hyperlink ref="A84:A88" r:id="rId27" display="Faction Identification UI" xr:uid="{C1669F17-A49B-46A7-8935-937FC40B07C8}"/>
-    <hyperlink ref="A81" r:id="rId28" xr:uid="{95C2A189-284D-4C96-A9E9-A540B49A9BA8}"/>
-    <hyperlink ref="A104:A107" r:id="rId29" display="Companion Inventory Unlock" xr:uid="{4142B9D6-B95F-482F-BD3F-A9EDB9C78FD5}"/>
-    <hyperlink ref="A108" r:id="rId30" xr:uid="{142E6B99-C7A8-42F1-833F-F6B912146B8D}"/>
+    <hyperlink ref="A78" r:id="rId20" xr:uid="{ABD9644B-2379-4071-A0CA-3BF1DAFBAE14}"/>
+    <hyperlink ref="A90" r:id="rId21" xr:uid="{92668D3C-4260-4890-BCB5-25F8810B0A07}"/>
+    <hyperlink ref="A99:A104" r:id="rId22" display="Exo Servomotor Sounds" xr:uid="{4C647516-14B0-42EE-92BE-10C69BB93F13}"/>
+    <hyperlink ref="A93:A98" r:id="rId23" display="Campfire Healing" xr:uid="{428C437E-0CA8-499F-9462-F2EB9B7D4A46}"/>
+    <hyperlink ref="A92" r:id="rId24" xr:uid="{E66EB141-6133-4A7F-BD3E-0A04AEBD5D2D}"/>
+    <hyperlink ref="A91" r:id="rId25" xr:uid="{A12C9A94-1493-4038-9561-4B2EED259B4A}"/>
+    <hyperlink ref="A83:A84" r:id="rId26" display="Companion Tweaks" xr:uid="{CF434ECD-6EEF-4AC0-BCCD-B6BE22DD1DAD}"/>
+    <hyperlink ref="A85:A89" r:id="rId27" display="Faction Identification UI" xr:uid="{C1669F17-A49B-46A7-8935-937FC40B07C8}"/>
+    <hyperlink ref="A82" r:id="rId28" xr:uid="{95C2A189-284D-4C96-A9E9-A540B49A9BA8}"/>
+    <hyperlink ref="A105:A108" r:id="rId29" display="Companion Inventory Unlock" xr:uid="{4142B9D6-B95F-482F-BD3F-A9EDB9C78FD5}"/>
+    <hyperlink ref="A109" r:id="rId30" xr:uid="{142E6B99-C7A8-42F1-833F-F6B912146B8D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId31"/>

</xml_diff>

<commit_message>
Integrated Funny Jump Sound mod
</commit_message>
<xml_diff>
--- a/development/Integrated Mods.xlsx
+++ b/development/Integrated Mods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\S.T.A.L.K.E.R\Anomaly Mods\mods\Back-to-roots-wip\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D953260-B7EC-48D6-8B0F-15CF6879A2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1AF35C-950C-4B83-BD42-D4F22E473376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="200">
   <si>
     <t>Filename</t>
   </si>
@@ -627,6 +627,15 @@
   </si>
   <si>
     <t>textures/map/</t>
+  </si>
+  <si>
+    <t>"Merc Jump Sounds"</t>
+  </si>
+  <si>
+    <t>Singustromo</t>
+  </si>
+  <si>
+    <t>jump_sounds.script</t>
   </si>
 </sst>
 </file>
@@ -849,7 +858,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -920,22 +929,34 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -944,23 +965,14 @@
     <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1299,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8700934C-DA8F-46A3-9CCC-A5B0203FB02B}">
   <dimension ref="A1:E135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D122" sqref="D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1331,7 +1343,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="49" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="15" t="s">
@@ -1343,12 +1355,12 @@
       <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="48" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
+      <c r="A3" s="42"/>
       <c r="B3" s="16" t="s">
         <v>12</v>
       </c>
@@ -1358,7 +1370,7 @@
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="40"/>
+      <c r="E3" s="45"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -1378,7 +1390,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="42" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="17" t="s">
@@ -1390,12 +1402,12 @@
       <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="40" t="s">
+      <c r="E5" s="45" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="15" t="s">
         <v>20</v>
       </c>
@@ -1405,10 +1417,10 @@
       <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="40"/>
+      <c r="E6" s="45"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="16" t="s">
         <v>22</v>
       </c>
@@ -1418,10 +1430,10 @@
       <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="40"/>
+      <c r="E7" s="45"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="15" t="s">
         <v>23</v>
       </c>
@@ -1431,10 +1443,10 @@
       <c r="D8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="40"/>
+      <c r="E8" s="45"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="16" t="s">
         <v>24</v>
       </c>
@@ -1444,10 +1456,10 @@
       <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="40"/>
+      <c r="E9" s="45"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="15" t="s">
         <v>25</v>
       </c>
@@ -1457,10 +1469,10 @@
       <c r="D10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="40"/>
+      <c r="E10" s="45"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="16" t="s">
         <v>26</v>
       </c>
@@ -1470,10 +1482,10 @@
       <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="40"/>
+      <c r="E11" s="45"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
+      <c r="A12" s="42"/>
       <c r="B12" s="15" t="s">
         <v>25</v>
       </c>
@@ -1483,10 +1495,10 @@
       <c r="D12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="40"/>
+      <c r="E12" s="45"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="16" t="s">
         <v>26</v>
       </c>
@@ -1496,10 +1508,10 @@
       <c r="D13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="40"/>
+      <c r="E13" s="45"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="44" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="18" t="s">
@@ -1511,10 +1523,10 @@
       <c r="D14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="40"/>
+      <c r="E14" s="45"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="38"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="16" t="s">
         <v>31</v>
       </c>
@@ -1524,10 +1536,10 @@
       <c r="D15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="40"/>
+      <c r="E15" s="45"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="15" t="s">
         <v>32</v>
       </c>
@@ -1537,10 +1549,10 @@
       <c r="D16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="40"/>
+      <c r="E16" s="45"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="16" t="s">
         <v>33</v>
       </c>
@@ -1550,10 +1562,10 @@
       <c r="D17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="40"/>
+      <c r="E17" s="45"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="38"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="15" t="s">
         <v>34</v>
       </c>
@@ -1563,10 +1575,10 @@
       <c r="D18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="40"/>
+      <c r="E18" s="45"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="38"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="16" t="s">
         <v>35</v>
       </c>
@@ -1576,10 +1588,10 @@
       <c r="D19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="40"/>
+      <c r="E19" s="45"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="38"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="15" t="s">
         <v>36</v>
       </c>
@@ -1589,10 +1601,10 @@
       <c r="D20" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="40"/>
+      <c r="E20" s="45"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
+      <c r="A21" s="44"/>
       <c r="B21" s="16" t="s">
         <v>37</v>
       </c>
@@ -1602,10 +1614,10 @@
       <c r="D21" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="40"/>
+      <c r="E21" s="45"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
+      <c r="A22" s="44"/>
       <c r="B22" s="15" t="s">
         <v>38</v>
       </c>
@@ -1615,10 +1627,10 @@
       <c r="D22" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="40"/>
+      <c r="E22" s="45"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="38"/>
+      <c r="A23" s="44"/>
       <c r="B23" s="16" t="s">
         <v>39</v>
       </c>
@@ -1628,10 +1640,10 @@
       <c r="D23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="40"/>
+      <c r="E23" s="45"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="38"/>
+      <c r="A24" s="44"/>
       <c r="B24" s="15" t="s">
         <v>40</v>
       </c>
@@ -1641,10 +1653,10 @@
       <c r="D24" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="40"/>
+      <c r="E24" s="45"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="38"/>
+      <c r="A25" s="44"/>
       <c r="B25" s="16" t="s">
         <v>40</v>
       </c>
@@ -1654,7 +1666,7 @@
       <c r="D25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="40"/>
+      <c r="E25" s="45"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
@@ -1674,7 +1686,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="44" t="s">
         <v>45</v>
       </c>
       <c r="B27" s="17" t="s">
@@ -1686,12 +1698,12 @@
       <c r="D27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="40" t="s">
+      <c r="E27" s="45" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="38"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="18" t="s">
         <v>19</v>
       </c>
@@ -1701,10 +1713,10 @@
       <c r="D28" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="40"/>
+      <c r="E28" s="45"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="38"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="17" t="s">
         <v>19</v>
       </c>
@@ -1714,7 +1726,7 @@
       <c r="D29" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="40"/>
+      <c r="E29" s="45"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
@@ -1734,7 +1746,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="44" t="s">
         <v>53</v>
       </c>
       <c r="B31" s="16" t="s">
@@ -1746,12 +1758,12 @@
       <c r="D31" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="40" t="s">
+      <c r="E31" s="45" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="38"/>
+      <c r="A32" s="44"/>
       <c r="B32" s="15" t="s">
         <v>55</v>
       </c>
@@ -1761,56 +1773,56 @@
       <c r="D32" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="40"/>
+      <c r="E32" s="45"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="38"/>
+      <c r="A33" s="44"/>
       <c r="B33" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="46" t="s">
         <v>62</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="40"/>
+      <c r="E33" s="45"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="38"/>
+      <c r="A34" s="44"/>
       <c r="B34" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="42"/>
+      <c r="C34" s="46"/>
       <c r="D34" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="40"/>
+      <c r="E34" s="45"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="38"/>
+      <c r="A35" s="44"/>
       <c r="B35" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="42"/>
+      <c r="C35" s="46"/>
       <c r="D35" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="E35" s="40"/>
+      <c r="E35" s="45"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="38"/>
+      <c r="A36" s="44"/>
       <c r="B36" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="42"/>
+      <c r="C36" s="46"/>
       <c r="D36" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="40"/>
+      <c r="E36" s="45"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="38"/>
+      <c r="A37" s="44"/>
       <c r="B37" s="16" t="s">
         <v>61</v>
       </c>
@@ -1820,10 +1832,10 @@
       <c r="D37" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="40"/>
+      <c r="E37" s="45"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="38"/>
+      <c r="A38" s="44"/>
       <c r="B38" s="15" t="s">
         <v>63</v>
       </c>
@@ -1833,10 +1845,10 @@
       <c r="D38" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="40"/>
+      <c r="E38" s="45"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="38"/>
+      <c r="A39" s="44"/>
       <c r="B39" s="16" t="s">
         <v>64</v>
       </c>
@@ -1846,10 +1858,10 @@
       <c r="D39" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E39" s="40"/>
+      <c r="E39" s="45"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="38"/>
+      <c r="A40" s="44"/>
       <c r="B40" s="15" t="s">
         <v>65</v>
       </c>
@@ -1859,10 +1871,10 @@
       <c r="D40" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="40"/>
+      <c r="E40" s="45"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="38"/>
+      <c r="A41" s="44"/>
       <c r="B41" s="16" t="s">
         <v>66</v>
       </c>
@@ -1872,10 +1884,10 @@
       <c r="D41" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E41" s="40"/>
+      <c r="E41" s="45"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="38"/>
+      <c r="A42" s="44"/>
       <c r="B42" s="18" t="s">
         <v>19</v>
       </c>
@@ -1885,10 +1897,10 @@
       <c r="D42" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="40"/>
+      <c r="E42" s="45"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="38"/>
+      <c r="A43" s="44"/>
       <c r="B43" s="16" t="s">
         <v>68</v>
       </c>
@@ -1898,10 +1910,10 @@
       <c r="D43" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E43" s="40"/>
+      <c r="E43" s="45"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="37" t="s">
+      <c r="A44" s="42" t="s">
         <v>70</v>
       </c>
       <c r="B44" s="15" t="s">
@@ -1913,12 +1925,12 @@
       <c r="D44" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E44" s="41" t="s">
+      <c r="E44" s="43" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="37"/>
+      <c r="A45" s="42"/>
       <c r="B45" s="16" t="s">
         <v>72</v>
       </c>
@@ -1928,10 +1940,10 @@
       <c r="D45" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E45" s="41"/>
+      <c r="E45" s="43"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="37"/>
+      <c r="A46" s="42"/>
       <c r="B46" s="15" t="s">
         <v>73</v>
       </c>
@@ -1941,10 +1953,10 @@
       <c r="D46" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E46" s="41"/>
+      <c r="E46" s="43"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="37"/>
+      <c r="A47" s="42"/>
       <c r="B47" s="16" t="s">
         <v>74</v>
       </c>
@@ -1954,10 +1966,10 @@
       <c r="D47" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E47" s="41"/>
+      <c r="E47" s="43"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="37"/>
+      <c r="A48" s="42"/>
       <c r="B48" s="15" t="s">
         <v>75</v>
       </c>
@@ -1967,10 +1979,10 @@
       <c r="D48" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E48" s="41"/>
+      <c r="E48" s="43"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="37"/>
+      <c r="A49" s="42"/>
       <c r="B49" s="16" t="s">
         <v>76</v>
       </c>
@@ -1980,7 +1992,7 @@
       <c r="D49" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="41"/>
+      <c r="E49" s="43"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
@@ -2000,7 +2012,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="37" t="s">
+      <c r="A51" s="42" t="s">
         <v>79</v>
       </c>
       <c r="B51" s="16" t="s">
@@ -2012,12 +2024,12 @@
       <c r="D51" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E51" s="41" t="s">
+      <c r="E51" s="43" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="37"/>
+      <c r="A52" s="42"/>
       <c r="B52" s="15" t="s">
         <v>83</v>
       </c>
@@ -2027,10 +2039,10 @@
       <c r="D52" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E52" s="41"/>
+      <c r="E52" s="43"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="37"/>
+      <c r="A53" s="42"/>
       <c r="B53" s="16" t="s">
         <v>83</v>
       </c>
@@ -2040,10 +2052,10 @@
       <c r="D53" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E53" s="41"/>
+      <c r="E53" s="43"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="37"/>
+      <c r="A54" s="42"/>
       <c r="B54" s="15" t="s">
         <v>84</v>
       </c>
@@ -2053,10 +2065,10 @@
       <c r="D54" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E54" s="41"/>
+      <c r="E54" s="43"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="37"/>
+      <c r="A55" s="42"/>
       <c r="B55" s="16" t="s">
         <v>85</v>
       </c>
@@ -2066,10 +2078,10 @@
       <c r="D55" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E55" s="41"/>
+      <c r="E55" s="43"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="37"/>
+      <c r="A56" s="42"/>
       <c r="B56" s="15" t="s">
         <v>86</v>
       </c>
@@ -2079,10 +2091,10 @@
       <c r="D56" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E56" s="41"/>
+      <c r="E56" s="43"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="37"/>
+      <c r="A57" s="42"/>
       <c r="B57" s="16" t="s">
         <v>87</v>
       </c>
@@ -2092,10 +2104,10 @@
       <c r="D57" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E57" s="41"/>
+      <c r="E57" s="43"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="37"/>
+      <c r="A58" s="42"/>
       <c r="B58" s="15" t="s">
         <v>88</v>
       </c>
@@ -2105,10 +2117,10 @@
       <c r="D58" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E58" s="41"/>
+      <c r="E58" s="43"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="37"/>
+      <c r="A59" s="42"/>
       <c r="B59" s="16" t="s">
         <v>89</v>
       </c>
@@ -2118,10 +2130,10 @@
       <c r="D59" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E59" s="41"/>
+      <c r="E59" s="43"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="37"/>
+      <c r="A60" s="42"/>
       <c r="B60" s="15" t="s">
         <v>91</v>
       </c>
@@ -2131,7 +2143,7 @@
       <c r="D60" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E60" s="41"/>
+      <c r="E60" s="43"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
@@ -2151,7 +2163,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="37" t="s">
+      <c r="A62" s="42" t="s">
         <v>96</v>
       </c>
       <c r="B62" s="15" t="s">
@@ -2163,12 +2175,12 @@
       <c r="D62" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E62" s="41" t="s">
+      <c r="E62" s="43" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="37"/>
+      <c r="A63" s="42"/>
       <c r="B63" s="16" t="s">
         <v>98</v>
       </c>
@@ -2178,10 +2190,10 @@
       <c r="D63" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E63" s="41"/>
+      <c r="E63" s="43"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="37"/>
+      <c r="A64" s="42"/>
       <c r="B64" s="15" t="s">
         <v>99</v>
       </c>
@@ -2191,10 +2203,10 @@
       <c r="D64" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E64" s="41"/>
+      <c r="E64" s="43"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="37"/>
+      <c r="A65" s="42"/>
       <c r="B65" s="16" t="s">
         <v>100</v>
       </c>
@@ -2204,10 +2216,10 @@
       <c r="D65" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="41"/>
+      <c r="E65" s="43"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="37"/>
+      <c r="A66" s="42"/>
       <c r="B66" s="15" t="s">
         <v>101</v>
       </c>
@@ -2217,10 +2229,10 @@
       <c r="D66" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E66" s="41"/>
+      <c r="E66" s="43"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="37"/>
+      <c r="A67" s="42"/>
       <c r="B67" s="16" t="s">
         <v>102</v>
       </c>
@@ -2230,10 +2242,10 @@
       <c r="D67" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E67" s="41"/>
+      <c r="E67" s="43"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="37"/>
+      <c r="A68" s="42"/>
       <c r="B68" s="15" t="s">
         <v>103</v>
       </c>
@@ -2243,7 +2255,7 @@
       <c r="D68" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E68" s="41"/>
+      <c r="E68" s="43"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
@@ -2300,10 +2312,10 @@
       <c r="A72" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="B72" s="43" t="s">
+      <c r="B72" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="C72" s="42" t="s">
+      <c r="C72" s="46" t="s">
         <v>116</v>
       </c>
       <c r="D72" s="22" t="s">
@@ -2314,20 +2326,20 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="38" t="s">
+      <c r="A73" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="B73" s="43"/>
-      <c r="C73" s="42"/>
+      <c r="B73" s="47"/>
+      <c r="C73" s="46"/>
       <c r="D73" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E73" s="40" t="s">
+      <c r="E73" s="45" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="38"/>
+      <c r="A74" s="44"/>
       <c r="B74" s="31" t="s">
         <v>194</v>
       </c>
@@ -2337,10 +2349,10 @@
       <c r="D74" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E74" s="40"/>
+      <c r="E74" s="45"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="37" t="s">
+      <c r="A75" s="42" t="s">
         <v>112</v>
       </c>
       <c r="B75" s="23" t="s">
@@ -2352,12 +2364,12 @@
       <c r="D75" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E75" s="41" t="s">
+      <c r="E75" s="43" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="37"/>
+      <c r="A76" s="42"/>
       <c r="B76" s="16" t="s">
         <v>119</v>
       </c>
@@ -2367,10 +2379,10 @@
       <c r="D76" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E76" s="41"/>
+      <c r="E76" s="43"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="37"/>
+      <c r="A77" s="42"/>
       <c r="B77" s="15" t="s">
         <v>120</v>
       </c>
@@ -2380,10 +2392,10 @@
       <c r="D77" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E77" s="41"/>
+      <c r="E77" s="43"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="38" t="s">
+      <c r="A78" s="44" t="s">
         <v>121</v>
       </c>
       <c r="B78" s="16" t="s">
@@ -2395,12 +2407,12 @@
       <c r="D78" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E78" s="40" t="s">
+      <c r="E78" s="45" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="38"/>
+      <c r="A79" s="44"/>
       <c r="B79" s="15" t="s">
         <v>123</v>
       </c>
@@ -2410,10 +2422,10 @@
       <c r="D79" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E79" s="40"/>
+      <c r="E79" s="45"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="38"/>
+      <c r="A80" s="44"/>
       <c r="B80" s="16" t="s">
         <v>124</v>
       </c>
@@ -2423,10 +2435,10 @@
       <c r="D80" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E80" s="40"/>
+      <c r="E80" s="45"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="38"/>
+      <c r="A81" s="44"/>
       <c r="B81" s="15" t="s">
         <v>125</v>
       </c>
@@ -2436,7 +2448,7 @@
       <c r="D81" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E81" s="40"/>
+      <c r="E81" s="45"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
@@ -2456,7 +2468,7 @@
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="47" t="s">
+      <c r="A83" s="41" t="s">
         <v>129</v>
       </c>
       <c r="B83" s="25" t="s">
@@ -2468,12 +2480,12 @@
       <c r="D83" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E83" s="46" t="s">
+      <c r="E83" s="39" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="47"/>
+      <c r="A84" s="41"/>
       <c r="B84" s="24" t="s">
         <v>132</v>
       </c>
@@ -2483,10 +2495,10 @@
       <c r="D84" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E84" s="46"/>
+      <c r="E84" s="39"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="45" t="s">
+      <c r="A85" s="38" t="s">
         <v>133</v>
       </c>
       <c r="B85" s="25" t="s">
@@ -2498,12 +2510,12 @@
       <c r="D85" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E85" s="44" t="s">
+      <c r="E85" s="36" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="45"/>
+      <c r="A86" s="38"/>
       <c r="B86" s="24" t="s">
         <v>135</v>
       </c>
@@ -2513,10 +2525,10 @@
       <c r="D86" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E86" s="44"/>
+      <c r="E86" s="36"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="45"/>
+      <c r="A87" s="38"/>
       <c r="B87" s="25" t="s">
         <v>136</v>
       </c>
@@ -2526,10 +2538,10 @@
       <c r="D87" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E87" s="44"/>
+      <c r="E87" s="36"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="45"/>
+      <c r="A88" s="38"/>
       <c r="B88" s="24" t="s">
         <v>137</v>
       </c>
@@ -2539,10 +2551,10 @@
       <c r="D88" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E88" s="44"/>
+      <c r="E88" s="36"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="45"/>
+      <c r="A89" s="38"/>
       <c r="B89" s="18" t="s">
         <v>19</v>
       </c>
@@ -2552,7 +2564,7 @@
       <c r="D89" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E89" s="44"/>
+      <c r="E89" s="36"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
@@ -2606,7 +2618,7 @@
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="45" t="s">
+      <c r="A93" s="38" t="s">
         <v>148</v>
       </c>
       <c r="B93" s="25" t="s">
@@ -2618,12 +2630,12 @@
       <c r="D93" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E93" s="44" t="s">
+      <c r="E93" s="36" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="45"/>
+      <c r="A94" s="38"/>
       <c r="B94" s="24" t="s">
         <v>151</v>
       </c>
@@ -2633,10 +2645,10 @@
       <c r="D94" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E94" s="44"/>
+      <c r="E94" s="36"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="45"/>
+      <c r="A95" s="38"/>
       <c r="B95" s="25" t="s">
         <v>152</v>
       </c>
@@ -2646,10 +2658,10 @@
       <c r="D95" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E95" s="44"/>
+      <c r="E95" s="36"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="45"/>
+      <c r="A96" s="38"/>
       <c r="B96" s="24" t="s">
         <v>153</v>
       </c>
@@ -2659,10 +2671,10 @@
       <c r="D96" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E96" s="44"/>
+      <c r="E96" s="36"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="45"/>
+      <c r="A97" s="38"/>
       <c r="B97" s="25" t="s">
         <v>154</v>
       </c>
@@ -2672,10 +2684,10 @@
       <c r="D97" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E97" s="44"/>
+      <c r="E97" s="36"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="45"/>
+      <c r="A98" s="38"/>
       <c r="B98" s="24" t="s">
         <v>155</v>
       </c>
@@ -2685,10 +2697,10 @@
       <c r="D98" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E98" s="44"/>
+      <c r="E98" s="36"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="47" t="s">
+      <c r="A99" s="41" t="s">
         <v>156</v>
       </c>
       <c r="B99" s="25" t="s">
@@ -2700,12 +2712,12 @@
       <c r="D99" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E99" s="46" t="s">
+      <c r="E99" s="39" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="47"/>
+      <c r="A100" s="41"/>
       <c r="B100" s="24" t="s">
         <v>157</v>
       </c>
@@ -2715,10 +2727,10 @@
       <c r="D100" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E100" s="46"/>
+      <c r="E100" s="39"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="47"/>
+      <c r="A101" s="41"/>
       <c r="B101" s="25" t="s">
         <v>158</v>
       </c>
@@ -2728,10 +2740,10 @@
       <c r="D101" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E101" s="46"/>
+      <c r="E101" s="39"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="47"/>
+      <c r="A102" s="41"/>
       <c r="B102" s="24" t="s">
         <v>159</v>
       </c>
@@ -2741,10 +2753,10 @@
       <c r="D102" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E102" s="46"/>
+      <c r="E102" s="39"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="47"/>
+      <c r="A103" s="41"/>
       <c r="B103" s="25" t="s">
         <v>160</v>
       </c>
@@ -2754,10 +2766,10 @@
       <c r="D103" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E103" s="46"/>
+      <c r="E103" s="39"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="47"/>
+      <c r="A104" s="41"/>
       <c r="B104" s="17" t="s">
         <v>162</v>
       </c>
@@ -2767,10 +2779,10 @@
       <c r="D104" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E104" s="46"/>
+      <c r="E104" s="39"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="45" t="s">
+      <c r="A105" s="38" t="s">
         <v>169</v>
       </c>
       <c r="B105" s="25" t="s">
@@ -2782,12 +2794,12 @@
       <c r="D105" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E105" s="44" t="s">
+      <c r="E105" s="36" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="45"/>
+      <c r="A106" s="38"/>
       <c r="B106" s="24" t="s">
         <v>171</v>
       </c>
@@ -2797,10 +2809,10 @@
       <c r="D106" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E106" s="44"/>
+      <c r="E106" s="36"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="45"/>
+      <c r="A107" s="38"/>
       <c r="B107" s="25" t="s">
         <v>172</v>
       </c>
@@ -2810,10 +2822,10 @@
       <c r="D107" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E107" s="44"/>
+      <c r="E107" s="36"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="45"/>
+      <c r="A108" s="38"/>
       <c r="B108" s="24" t="s">
         <v>173</v>
       </c>
@@ -2823,7 +2835,7 @@
       <c r="D108" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E108" s="44"/>
+      <c r="E108" s="36"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
@@ -2858,7 +2870,7 @@
       <c r="E110" s="32"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="46" t="s">
+      <c r="A111" s="39" t="s">
         <v>180</v>
       </c>
       <c r="B111" s="25" t="s">
@@ -2870,10 +2882,10 @@
       <c r="D111" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E111" s="49"/>
+      <c r="E111" s="40"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="46"/>
+      <c r="A112" s="39"/>
       <c r="B112" s="24" t="s">
         <v>182</v>
       </c>
@@ -2883,10 +2895,10 @@
       <c r="D112" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E112" s="49"/>
+      <c r="E112" s="40"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="44" t="s">
+      <c r="A113" s="36" t="s">
         <v>183</v>
       </c>
       <c r="B113" s="34" t="s">
@@ -2898,10 +2910,10 @@
       <c r="D113" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E113" s="48"/>
+      <c r="E113" s="37"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="44"/>
+      <c r="A114" s="36"/>
       <c r="B114" s="35" t="s">
         <v>186</v>
       </c>
@@ -2911,7 +2923,7 @@
       <c r="D114" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E114" s="48"/>
+      <c r="E114" s="37"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="26" t="s">
@@ -2929,7 +2941,7 @@
       <c r="E115" s="26"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="44" t="s">
+      <c r="A116" s="36" t="s">
         <v>189</v>
       </c>
       <c r="B116" s="35" t="s">
@@ -2941,10 +2953,10 @@
       <c r="D116" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E116" s="48"/>
+      <c r="E116" s="37"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" s="44"/>
+      <c r="A117" s="36"/>
       <c r="B117" s="25" t="s">
         <v>190</v>
       </c>
@@ -2954,10 +2966,10 @@
       <c r="D117" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E117" s="48"/>
+      <c r="E117" s="37"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="44"/>
+      <c r="A118" s="36"/>
       <c r="B118" s="35" t="s">
         <v>191</v>
       </c>
@@ -2967,10 +2979,10 @@
       <c r="D118" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E118" s="48"/>
+      <c r="E118" s="37"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="44"/>
+      <c r="A119" s="36"/>
       <c r="B119" s="25" t="s">
         <v>192</v>
       </c>
@@ -2980,10 +2992,10 @@
       <c r="D119" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E119" s="48"/>
+      <c r="E119" s="37"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" s="44"/>
+      <c r="A120" s="36"/>
       <c r="B120" s="35" t="s">
         <v>193</v>
       </c>
@@ -2993,7 +3005,7 @@
       <c r="D120" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E120" s="48"/>
+      <c r="E120" s="37"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="26" t="s">
@@ -3007,25 +3019,39 @@
       <c r="E121" s="26"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B122" s="35"/>
-      <c r="C122" s="7"/>
+      <c r="A122" s="50" t="s">
+        <v>197</v>
+      </c>
+      <c r="B122" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="D122" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="E122" s="36" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="50"/>
       <c r="B123" s="25"/>
       <c r="C123" s="8"/>
       <c r="D123" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="E123" s="36"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="50"/>
       <c r="B124" s="35"/>
       <c r="C124" s="7"/>
       <c r="D124" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="E124" s="36"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B125" s="25"/>
@@ -3105,7 +3131,41 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="42">
+    <mergeCell ref="A122:A124"/>
+    <mergeCell ref="E122:E124"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A5:A13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A31:A43"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E5:E25"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="E31:E43"/>
+    <mergeCell ref="E44:E49"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="E51:E60"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="A51:A60"/>
+    <mergeCell ref="A62:A68"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="E75:E77"/>
+    <mergeCell ref="E62:E68"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="E78:E81"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="E93:E98"/>
+    <mergeCell ref="A93:A98"/>
+    <mergeCell ref="E99:E104"/>
+    <mergeCell ref="A99:A104"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="E83:E84"/>
+    <mergeCell ref="A85:A89"/>
+    <mergeCell ref="E85:E89"/>
     <mergeCell ref="A113:A114"/>
     <mergeCell ref="E113:E114"/>
     <mergeCell ref="A116:A120"/>
@@ -3114,38 +3174,6 @@
     <mergeCell ref="E105:E108"/>
     <mergeCell ref="A111:A112"/>
     <mergeCell ref="E111:E112"/>
-    <mergeCell ref="E93:E98"/>
-    <mergeCell ref="A93:A98"/>
-    <mergeCell ref="E99:E104"/>
-    <mergeCell ref="A99:A104"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="E83:E84"/>
-    <mergeCell ref="A85:A89"/>
-    <mergeCell ref="E85:E89"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="E75:E77"/>
-    <mergeCell ref="E62:E68"/>
-    <mergeCell ref="A78:A81"/>
-    <mergeCell ref="E78:E81"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="C33:C36"/>
-    <mergeCell ref="E51:E60"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="A51:A60"/>
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="E73:E74"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="E5:E25"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="E31:E43"/>
-    <mergeCell ref="E44:E49"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A5:A13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A31:A43"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{D01E85B4-1DB0-475A-87DE-364916E7DA22}"/>

</xml_diff>

<commit_message>
Several cool changes for making development easier
</commit_message>
<xml_diff>
--- a/development/Integrated Mods.xlsx
+++ b/development/Integrated Mods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\S.T.A.L.K.E.R\Anomaly Mods\mods\Back-to-roots-wip\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1AF35C-950C-4B83-BD42-D4F22E473376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073735B7-7058-42BB-AD27-00ECE05DEC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="200">
   <si>
     <t>Filename</t>
   </si>
@@ -858,7 +858,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -972,7 +972,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1312,7 +1315,7 @@
   <dimension ref="A1:E135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A101" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D122" sqref="D122"/>
+      <selection activeCell="D124" sqref="D124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3031,27 +3034,23 @@
       <c r="D122" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E122" s="36" t="s">
+      <c r="E122" s="32" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" s="50"/>
+      <c r="A123" s="51"/>
       <c r="B123" s="25"/>
       <c r="C123" s="8"/>
-      <c r="D123" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E123" s="36"/>
+      <c r="D123" s="6"/>
+      <c r="E123" s="33"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="50"/>
       <c r="B124" s="35"/>
       <c r="C124" s="7"/>
-      <c r="D124" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E124" s="36"/>
+      <c r="D124" s="6"/>
+      <c r="E124" s="32"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B125" s="25"/>
@@ -3131,9 +3130,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="42">
-    <mergeCell ref="A122:A124"/>
-    <mergeCell ref="E122:E124"/>
+  <mergeCells count="40">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="A14:A25"/>

</xml_diff>

<commit_message>
Actually integrated Movable NPCs mod
</commit_message>
<xml_diff>
--- a/development/Integrated Mods.xlsx
+++ b/development/Integrated Mods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\S.T.A.L.K.E.R\Anomaly Mods\mods\Back-to-roots-wip\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBFF963-F280-4895-976A-0FCD0F53D19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6842C31B-B544-4179-BB05-EED7D9A4037F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="211">
   <si>
     <t>Filename</t>
   </si>
@@ -666,6 +666,9 @@
   </si>
   <si>
     <t>Banjaji</t>
+  </si>
+  <si>
+    <t>mod_system_actor1.ltx</t>
   </si>
 </sst>
 </file>
@@ -968,22 +971,34 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -992,23 +1007,11 @@
     <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1347,8 +1350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8700934C-DA8F-46A3-9CCC-A5B0203FB02B}">
   <dimension ref="A1:E135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N113" sqref="N113"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,7 +1382,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="52" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="15" t="s">
@@ -1391,12 +1394,12 @@
       <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="51" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
+      <c r="A3" s="45"/>
       <c r="B3" s="16" t="s">
         <v>12</v>
       </c>
@@ -1406,7 +1409,7 @@
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="43"/>
+      <c r="E3" s="48"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -1426,7 +1429,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="45" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="17" t="s">
@@ -1438,12 +1441,12 @@
       <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="48" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="15" t="s">
         <v>20</v>
       </c>
@@ -1453,10 +1456,10 @@
       <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="43"/>
+      <c r="E6" s="48"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="16" t="s">
         <v>22</v>
       </c>
@@ -1466,10 +1469,10 @@
       <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="43"/>
+      <c r="E7" s="48"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="15" t="s">
         <v>23</v>
       </c>
@@ -1479,10 +1482,10 @@
       <c r="D8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="43"/>
+      <c r="E8" s="48"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="16" t="s">
         <v>24</v>
       </c>
@@ -1492,10 +1495,10 @@
       <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="43"/>
+      <c r="E9" s="48"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
+      <c r="A10" s="45"/>
       <c r="B10" s="15" t="s">
         <v>25</v>
       </c>
@@ -1505,10 +1508,10 @@
       <c r="D10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="43"/>
+      <c r="E10" s="48"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="16" t="s">
         <v>26</v>
       </c>
@@ -1518,10 +1521,10 @@
       <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="43"/>
+      <c r="E11" s="48"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
+      <c r="A12" s="45"/>
       <c r="B12" s="15" t="s">
         <v>25</v>
       </c>
@@ -1531,10 +1534,10 @@
       <c r="D12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="43"/>
+      <c r="E12" s="48"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="16" t="s">
         <v>26</v>
       </c>
@@ -1544,10 +1547,10 @@
       <c r="D13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="43"/>
+      <c r="E13" s="48"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="47" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="18" t="s">
@@ -1559,10 +1562,10 @@
       <c r="D14" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="43"/>
+      <c r="E14" s="48"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
+      <c r="A15" s="47"/>
       <c r="B15" s="16" t="s">
         <v>31</v>
       </c>
@@ -1572,10 +1575,10 @@
       <c r="D15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="43"/>
+      <c r="E15" s="48"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="15" t="s">
         <v>32</v>
       </c>
@@ -1585,10 +1588,10 @@
       <c r="D16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="43"/>
+      <c r="E16" s="48"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="16" t="s">
         <v>33</v>
       </c>
@@ -1598,10 +1601,10 @@
       <c r="D17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="43"/>
+      <c r="E17" s="48"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="15" t="s">
         <v>34</v>
       </c>
@@ -1611,10 +1614,10 @@
       <c r="D18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="43"/>
+      <c r="E18" s="48"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
+      <c r="A19" s="47"/>
       <c r="B19" s="16" t="s">
         <v>35</v>
       </c>
@@ -1624,10 +1627,10 @@
       <c r="D19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="43"/>
+      <c r="E19" s="48"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
+      <c r="A20" s="47"/>
       <c r="B20" s="15" t="s">
         <v>36</v>
       </c>
@@ -1637,10 +1640,10 @@
       <c r="D20" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="43"/>
+      <c r="E20" s="48"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="41"/>
+      <c r="A21" s="47"/>
       <c r="B21" s="16" t="s">
         <v>37</v>
       </c>
@@ -1650,10 +1653,10 @@
       <c r="D21" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="43"/>
+      <c r="E21" s="48"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
+      <c r="A22" s="47"/>
       <c r="B22" s="15" t="s">
         <v>38</v>
       </c>
@@ -1663,10 +1666,10 @@
       <c r="D22" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="43"/>
+      <c r="E22" s="48"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
+      <c r="A23" s="47"/>
       <c r="B23" s="16" t="s">
         <v>39</v>
       </c>
@@ -1676,10 +1679,10 @@
       <c r="D23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="43"/>
+      <c r="E23" s="48"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
+      <c r="A24" s="47"/>
       <c r="B24" s="15" t="s">
         <v>40</v>
       </c>
@@ -1689,10 +1692,10 @@
       <c r="D24" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="43"/>
+      <c r="E24" s="48"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
+      <c r="A25" s="47"/>
       <c r="B25" s="16" t="s">
         <v>40</v>
       </c>
@@ -1702,7 +1705,7 @@
       <c r="D25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="43"/>
+      <c r="E25" s="48"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
@@ -1722,7 +1725,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="47" t="s">
         <v>45</v>
       </c>
       <c r="B27" s="17" t="s">
@@ -1734,12 +1737,12 @@
       <c r="D27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="43" t="s">
+      <c r="E27" s="48" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="41"/>
+      <c r="A28" s="47"/>
       <c r="B28" s="18" t="s">
         <v>19</v>
       </c>
@@ -1749,10 +1752,10 @@
       <c r="D28" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="43"/>
+      <c r="E28" s="48"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
+      <c r="A29" s="47"/>
       <c r="B29" s="17" t="s">
         <v>19</v>
       </c>
@@ -1762,7 +1765,7 @@
       <c r="D29" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="43"/>
+      <c r="E29" s="48"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
@@ -1782,7 +1785,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="47" t="s">
         <v>53</v>
       </c>
       <c r="B31" s="16" t="s">
@@ -1794,12 +1797,12 @@
       <c r="D31" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="43" t="s">
+      <c r="E31" s="48" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="41"/>
+      <c r="A32" s="47"/>
       <c r="B32" s="15" t="s">
         <v>55</v>
       </c>
@@ -1809,56 +1812,56 @@
       <c r="D32" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="43"/>
+      <c r="E32" s="48"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="41"/>
+      <c r="A33" s="47"/>
       <c r="B33" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="45" t="s">
+      <c r="C33" s="49" t="s">
         <v>62</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="43"/>
+      <c r="E33" s="48"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="41"/>
+      <c r="A34" s="47"/>
       <c r="B34" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="45"/>
+      <c r="C34" s="49"/>
       <c r="D34" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="43"/>
+      <c r="E34" s="48"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="41"/>
+      <c r="A35" s="47"/>
       <c r="B35" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="45"/>
+      <c r="C35" s="49"/>
       <c r="D35" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="E35" s="43"/>
+      <c r="E35" s="48"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="41"/>
+      <c r="A36" s="47"/>
       <c r="B36" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="45"/>
+      <c r="C36" s="49"/>
       <c r="D36" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="43"/>
+      <c r="E36" s="48"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="41"/>
+      <c r="A37" s="47"/>
       <c r="B37" s="16" t="s">
         <v>61</v>
       </c>
@@ -1868,10 +1871,10 @@
       <c r="D37" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="43"/>
+      <c r="E37" s="48"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="41"/>
+      <c r="A38" s="47"/>
       <c r="B38" s="15" t="s">
         <v>63</v>
       </c>
@@ -1881,10 +1884,10 @@
       <c r="D38" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="43"/>
+      <c r="E38" s="48"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="41"/>
+      <c r="A39" s="47"/>
       <c r="B39" s="16" t="s">
         <v>64</v>
       </c>
@@ -1894,10 +1897,10 @@
       <c r="D39" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E39" s="43"/>
+      <c r="E39" s="48"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="41"/>
+      <c r="A40" s="47"/>
       <c r="B40" s="15" t="s">
         <v>65</v>
       </c>
@@ -1907,10 +1910,10 @@
       <c r="D40" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="43"/>
+      <c r="E40" s="48"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="41"/>
+      <c r="A41" s="47"/>
       <c r="B41" s="16" t="s">
         <v>66</v>
       </c>
@@ -1920,10 +1923,10 @@
       <c r="D41" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E41" s="43"/>
+      <c r="E41" s="48"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="41"/>
+      <c r="A42" s="47"/>
       <c r="B42" s="18" t="s">
         <v>19</v>
       </c>
@@ -1933,10 +1936,10 @@
       <c r="D42" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="43"/>
+      <c r="E42" s="48"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="41"/>
+      <c r="A43" s="47"/>
       <c r="B43" s="16" t="s">
         <v>68</v>
       </c>
@@ -1946,10 +1949,10 @@
       <c r="D43" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E43" s="43"/>
+      <c r="E43" s="48"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="40" t="s">
+      <c r="A44" s="45" t="s">
         <v>70</v>
       </c>
       <c r="B44" s="15" t="s">
@@ -1961,12 +1964,12 @@
       <c r="D44" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E44" s="44" t="s">
+      <c r="E44" s="46" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="40"/>
+      <c r="A45" s="45"/>
       <c r="B45" s="16" t="s">
         <v>72</v>
       </c>
@@ -1976,10 +1979,10 @@
       <c r="D45" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E45" s="44"/>
+      <c r="E45" s="46"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="40"/>
+      <c r="A46" s="45"/>
       <c r="B46" s="15" t="s">
         <v>73</v>
       </c>
@@ -1989,10 +1992,10 @@
       <c r="D46" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E46" s="44"/>
+      <c r="E46" s="46"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="40"/>
+      <c r="A47" s="45"/>
       <c r="B47" s="16" t="s">
         <v>74</v>
       </c>
@@ -2002,10 +2005,10 @@
       <c r="D47" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E47" s="44"/>
+      <c r="E47" s="46"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="40"/>
+      <c r="A48" s="45"/>
       <c r="B48" s="15" t="s">
         <v>75</v>
       </c>
@@ -2015,10 +2018,10 @@
       <c r="D48" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E48" s="44"/>
+      <c r="E48" s="46"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="40"/>
+      <c r="A49" s="45"/>
       <c r="B49" s="16" t="s">
         <v>76</v>
       </c>
@@ -2028,7 +2031,7 @@
       <c r="D49" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="44"/>
+      <c r="E49" s="46"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
@@ -2048,7 +2051,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="40" t="s">
+      <c r="A51" s="45" t="s">
         <v>79</v>
       </c>
       <c r="B51" s="16" t="s">
@@ -2060,12 +2063,12 @@
       <c r="D51" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E51" s="44" t="s">
+      <c r="E51" s="46" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="40"/>
+      <c r="A52" s="45"/>
       <c r="B52" s="15" t="s">
         <v>83</v>
       </c>
@@ -2075,10 +2078,10 @@
       <c r="D52" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E52" s="44"/>
+      <c r="E52" s="46"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="40"/>
+      <c r="A53" s="45"/>
       <c r="B53" s="16" t="s">
         <v>83</v>
       </c>
@@ -2088,10 +2091,10 @@
       <c r="D53" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E53" s="44"/>
+      <c r="E53" s="46"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="40"/>
+      <c r="A54" s="45"/>
       <c r="B54" s="15" t="s">
         <v>84</v>
       </c>
@@ -2101,10 +2104,10 @@
       <c r="D54" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E54" s="44"/>
+      <c r="E54" s="46"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="40"/>
+      <c r="A55" s="45"/>
       <c r="B55" s="16" t="s">
         <v>85</v>
       </c>
@@ -2114,10 +2117,10 @@
       <c r="D55" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E55" s="44"/>
+      <c r="E55" s="46"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="40"/>
+      <c r="A56" s="45"/>
       <c r="B56" s="15" t="s">
         <v>86</v>
       </c>
@@ -2127,10 +2130,10 @@
       <c r="D56" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E56" s="44"/>
+      <c r="E56" s="46"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="40"/>
+      <c r="A57" s="45"/>
       <c r="B57" s="16" t="s">
         <v>87</v>
       </c>
@@ -2140,10 +2143,10 @@
       <c r="D57" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E57" s="44"/>
+      <c r="E57" s="46"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="40"/>
+      <c r="A58" s="45"/>
       <c r="B58" s="15" t="s">
         <v>88</v>
       </c>
@@ -2153,10 +2156,10 @@
       <c r="D58" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E58" s="44"/>
+      <c r="E58" s="46"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="40"/>
+      <c r="A59" s="45"/>
       <c r="B59" s="16" t="s">
         <v>89</v>
       </c>
@@ -2166,10 +2169,10 @@
       <c r="D59" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E59" s="44"/>
+      <c r="E59" s="46"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="40"/>
+      <c r="A60" s="45"/>
       <c r="B60" s="15" t="s">
         <v>91</v>
       </c>
@@ -2179,7 +2182,7 @@
       <c r="D60" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E60" s="44"/>
+      <c r="E60" s="46"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
@@ -2199,7 +2202,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="40" t="s">
+      <c r="A62" s="45" t="s">
         <v>96</v>
       </c>
       <c r="B62" s="15" t="s">
@@ -2211,12 +2214,12 @@
       <c r="D62" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E62" s="44" t="s">
+      <c r="E62" s="46" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="40"/>
+      <c r="A63" s="45"/>
       <c r="B63" s="16" t="s">
         <v>98</v>
       </c>
@@ -2226,10 +2229,10 @@
       <c r="D63" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E63" s="44"/>
+      <c r="E63" s="46"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="40"/>
+      <c r="A64" s="45"/>
       <c r="B64" s="15" t="s">
         <v>99</v>
       </c>
@@ -2239,10 +2242,10 @@
       <c r="D64" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E64" s="44"/>
+      <c r="E64" s="46"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="40"/>
+      <c r="A65" s="45"/>
       <c r="B65" s="16" t="s">
         <v>100</v>
       </c>
@@ -2252,10 +2255,10 @@
       <c r="D65" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="44"/>
+      <c r="E65" s="46"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="40"/>
+      <c r="A66" s="45"/>
       <c r="B66" s="15" t="s">
         <v>101</v>
       </c>
@@ -2265,10 +2268,10 @@
       <c r="D66" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E66" s="44"/>
+      <c r="E66" s="46"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="40"/>
+      <c r="A67" s="45"/>
       <c r="B67" s="16" t="s">
         <v>102</v>
       </c>
@@ -2278,10 +2281,10 @@
       <c r="D67" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E67" s="44"/>
+      <c r="E67" s="46"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="40"/>
+      <c r="A68" s="45"/>
       <c r="B68" s="15" t="s">
         <v>103</v>
       </c>
@@ -2291,7 +2294,7 @@
       <c r="D68" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E68" s="44"/>
+      <c r="E68" s="46"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
@@ -2348,10 +2351,10 @@
       <c r="A72" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="B72" s="46" t="s">
+      <c r="B72" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="C72" s="45" t="s">
+      <c r="C72" s="49" t="s">
         <v>116</v>
       </c>
       <c r="D72" s="22" t="s">
@@ -2362,20 +2365,20 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="41" t="s">
+      <c r="A73" s="47" t="s">
         <v>113</v>
       </c>
-      <c r="B73" s="46"/>
-      <c r="C73" s="45"/>
+      <c r="B73" s="50"/>
+      <c r="C73" s="49"/>
       <c r="D73" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E73" s="43" t="s">
+      <c r="E73" s="48" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="41"/>
+      <c r="A74" s="47"/>
       <c r="B74" s="31" t="s">
         <v>194</v>
       </c>
@@ -2385,10 +2388,10 @@
       <c r="D74" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E74" s="43"/>
+      <c r="E74" s="48"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="40" t="s">
+      <c r="A75" s="45" t="s">
         <v>112</v>
       </c>
       <c r="B75" s="23" t="s">
@@ -2400,12 +2403,12 @@
       <c r="D75" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E75" s="44" t="s">
+      <c r="E75" s="46" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="40"/>
+      <c r="A76" s="45"/>
       <c r="B76" s="16" t="s">
         <v>119</v>
       </c>
@@ -2415,10 +2418,10 @@
       <c r="D76" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E76" s="44"/>
+      <c r="E76" s="46"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="40"/>
+      <c r="A77" s="45"/>
       <c r="B77" s="15" t="s">
         <v>120</v>
       </c>
@@ -2428,10 +2431,10 @@
       <c r="D77" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E77" s="44"/>
+      <c r="E77" s="46"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="41" t="s">
+      <c r="A78" s="47" t="s">
         <v>121</v>
       </c>
       <c r="B78" s="16" t="s">
@@ -2443,12 +2446,12 @@
       <c r="D78" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E78" s="43" t="s">
+      <c r="E78" s="48" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="41"/>
+      <c r="A79" s="47"/>
       <c r="B79" s="15" t="s">
         <v>123</v>
       </c>
@@ -2458,10 +2461,10 @@
       <c r="D79" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E79" s="43"/>
+      <c r="E79" s="48"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="41"/>
+      <c r="A80" s="47"/>
       <c r="B80" s="16" t="s">
         <v>124</v>
       </c>
@@ -2471,10 +2474,10 @@
       <c r="D80" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E80" s="43"/>
+      <c r="E80" s="48"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="41"/>
+      <c r="A81" s="47"/>
       <c r="B81" s="15" t="s">
         <v>125</v>
       </c>
@@ -2484,7 +2487,7 @@
       <c r="D81" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E81" s="43"/>
+      <c r="E81" s="48"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
@@ -2504,7 +2507,7 @@
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="50" t="s">
+      <c r="A83" s="44" t="s">
         <v>129</v>
       </c>
       <c r="B83" s="25" t="s">
@@ -2516,12 +2519,12 @@
       <c r="D83" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E83" s="49" t="s">
+      <c r="E83" s="39" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="50"/>
+      <c r="A84" s="44"/>
       <c r="B84" s="24" t="s">
         <v>132</v>
       </c>
@@ -2531,10 +2534,10 @@
       <c r="D84" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E84" s="49"/>
+      <c r="E84" s="39"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="48" t="s">
+      <c r="A85" s="42" t="s">
         <v>133</v>
       </c>
       <c r="B85" s="25" t="s">
@@ -2546,12 +2549,12 @@
       <c r="D85" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E85" s="47" t="s">
+      <c r="E85" s="40" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="48"/>
+      <c r="A86" s="42"/>
       <c r="B86" s="24" t="s">
         <v>135</v>
       </c>
@@ -2561,10 +2564,10 @@
       <c r="D86" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E86" s="47"/>
+      <c r="E86" s="40"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="48"/>
+      <c r="A87" s="42"/>
       <c r="B87" s="25" t="s">
         <v>136</v>
       </c>
@@ -2574,10 +2577,10 @@
       <c r="D87" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E87" s="47"/>
+      <c r="E87" s="40"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="48"/>
+      <c r="A88" s="42"/>
       <c r="B88" s="24" t="s">
         <v>137</v>
       </c>
@@ -2587,10 +2590,10 @@
       <c r="D88" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E88" s="47"/>
+      <c r="E88" s="40"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="48"/>
+      <c r="A89" s="42"/>
       <c r="B89" s="18" t="s">
         <v>19</v>
       </c>
@@ -2600,7 +2603,7 @@
       <c r="D89" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E89" s="47"/>
+      <c r="E89" s="40"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
@@ -2654,7 +2657,7 @@
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="48" t="s">
+      <c r="A93" s="42" t="s">
         <v>148</v>
       </c>
       <c r="B93" s="25" t="s">
@@ -2666,12 +2669,12 @@
       <c r="D93" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E93" s="47" t="s">
+      <c r="E93" s="40" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="48"/>
+      <c r="A94" s="42"/>
       <c r="B94" s="24" t="s">
         <v>151</v>
       </c>
@@ -2681,10 +2684,10 @@
       <c r="D94" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E94" s="47"/>
+      <c r="E94" s="40"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="48"/>
+      <c r="A95" s="42"/>
       <c r="B95" s="25" t="s">
         <v>152</v>
       </c>
@@ -2694,10 +2697,10 @@
       <c r="D95" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E95" s="47"/>
+      <c r="E95" s="40"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="48"/>
+      <c r="A96" s="42"/>
       <c r="B96" s="24" t="s">
         <v>153</v>
       </c>
@@ -2707,10 +2710,10 @@
       <c r="D96" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E96" s="47"/>
+      <c r="E96" s="40"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="48"/>
+      <c r="A97" s="42"/>
       <c r="B97" s="25" t="s">
         <v>154</v>
       </c>
@@ -2720,10 +2723,10 @@
       <c r="D97" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E97" s="47"/>
+      <c r="E97" s="40"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="48"/>
+      <c r="A98" s="42"/>
       <c r="B98" s="24" t="s">
         <v>155</v>
       </c>
@@ -2733,10 +2736,10 @@
       <c r="D98" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E98" s="47"/>
+      <c r="E98" s="40"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="50" t="s">
+      <c r="A99" s="44" t="s">
         <v>156</v>
       </c>
       <c r="B99" s="25" t="s">
@@ -2748,12 +2751,12 @@
       <c r="D99" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E99" s="49" t="s">
+      <c r="E99" s="39" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="50"/>
+      <c r="A100" s="44"/>
       <c r="B100" s="24" t="s">
         <v>157</v>
       </c>
@@ -2763,10 +2766,10 @@
       <c r="D100" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E100" s="49"/>
+      <c r="E100" s="39"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="50"/>
+      <c r="A101" s="44"/>
       <c r="B101" s="25" t="s">
         <v>158</v>
       </c>
@@ -2776,10 +2779,10 @@
       <c r="D101" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E101" s="49"/>
+      <c r="E101" s="39"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="50"/>
+      <c r="A102" s="44"/>
       <c r="B102" s="24" t="s">
         <v>159</v>
       </c>
@@ -2789,10 +2792,10 @@
       <c r="D102" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E102" s="49"/>
+      <c r="E102" s="39"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="50"/>
+      <c r="A103" s="44"/>
       <c r="B103" s="25" t="s">
         <v>160</v>
       </c>
@@ -2802,10 +2805,10 @@
       <c r="D103" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E103" s="49"/>
+      <c r="E103" s="39"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="50"/>
+      <c r="A104" s="44"/>
       <c r="B104" s="17" t="s">
         <v>162</v>
       </c>
@@ -2815,10 +2818,10 @@
       <c r="D104" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E104" s="49"/>
+      <c r="E104" s="39"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="48" t="s">
+      <c r="A105" s="42" t="s">
         <v>169</v>
       </c>
       <c r="B105" s="25" t="s">
@@ -2830,12 +2833,12 @@
       <c r="D105" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E105" s="47" t="s">
+      <c r="E105" s="40" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="48"/>
+      <c r="A106" s="42"/>
       <c r="B106" s="24" t="s">
         <v>171</v>
       </c>
@@ -2845,10 +2848,10 @@
       <c r="D106" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E106" s="47"/>
+      <c r="E106" s="40"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="48"/>
+      <c r="A107" s="42"/>
       <c r="B107" s="25" t="s">
         <v>172</v>
       </c>
@@ -2858,10 +2861,10 @@
       <c r="D107" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E107" s="47"/>
+      <c r="E107" s="40"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="48"/>
+      <c r="A108" s="42"/>
       <c r="B108" s="24" t="s">
         <v>173</v>
       </c>
@@ -2871,7 +2874,7 @@
       <c r="D108" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E108" s="47"/>
+      <c r="E108" s="40"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="9" t="s">
@@ -2906,7 +2909,7 @@
       <c r="E110" s="32"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="49" t="s">
+      <c r="A111" s="39" t="s">
         <v>180</v>
       </c>
       <c r="B111" s="25" t="s">
@@ -2918,10 +2921,10 @@
       <c r="D111" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E111" s="52"/>
+      <c r="E111" s="43"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="49"/>
+      <c r="A112" s="39"/>
       <c r="B112" s="24" t="s">
         <v>182</v>
       </c>
@@ -2931,10 +2934,10 @@
       <c r="D112" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E112" s="52"/>
+      <c r="E112" s="43"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="47" t="s">
+      <c r="A113" s="40" t="s">
         <v>183</v>
       </c>
       <c r="B113" s="34" t="s">
@@ -2946,10 +2949,10 @@
       <c r="D113" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E113" s="51"/>
+      <c r="E113" s="41"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="47"/>
+      <c r="A114" s="40"/>
       <c r="B114" s="35" t="s">
         <v>186</v>
       </c>
@@ -2959,7 +2962,7 @@
       <c r="D114" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E114" s="51"/>
+      <c r="E114" s="41"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="26" t="s">
@@ -2977,7 +2980,7 @@
       <c r="E115" s="26"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="47" t="s">
+      <c r="A116" s="40" t="s">
         <v>189</v>
       </c>
       <c r="B116" s="35" t="s">
@@ -2989,10 +2992,10 @@
       <c r="D116" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E116" s="51"/>
+      <c r="E116" s="41"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" s="47"/>
+      <c r="A117" s="40"/>
       <c r="B117" s="25" t="s">
         <v>190</v>
       </c>
@@ -3002,10 +3005,10 @@
       <c r="D117" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E117" s="51"/>
+      <c r="E117" s="41"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="47"/>
+      <c r="A118" s="40"/>
       <c r="B118" s="35" t="s">
         <v>191</v>
       </c>
@@ -3015,10 +3018,10 @@
       <c r="D118" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E118" s="51"/>
+      <c r="E118" s="41"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="47"/>
+      <c r="A119" s="40"/>
       <c r="B119" s="25" t="s">
         <v>192</v>
       </c>
@@ -3028,10 +3031,10 @@
       <c r="D119" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E119" s="51"/>
+      <c r="E119" s="41"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" s="47"/>
+      <c r="A120" s="40"/>
       <c r="B120" s="35" t="s">
         <v>193</v>
       </c>
@@ -3041,14 +3044,18 @@
       <c r="D120" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E120" s="51"/>
+      <c r="E120" s="41"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="26" t="s">
         <v>195</v>
       </c>
-      <c r="B121" s="25"/>
-      <c r="C121" s="8"/>
+      <c r="B121" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="C121" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="D121" s="6" t="s">
         <v>8</v>
       </c>
@@ -3086,7 +3093,7 @@
       <c r="E124" s="32"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" s="49" t="s">
+      <c r="A125" s="39" t="s">
         <v>200</v>
       </c>
       <c r="B125" s="25" t="s">
@@ -3098,12 +3105,12 @@
       <c r="D125" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E125" s="49" t="s">
+      <c r="E125" s="39" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="49"/>
+      <c r="A126" s="39"/>
       <c r="B126" s="35" t="s">
         <v>203</v>
       </c>
@@ -3113,10 +3120,10 @@
       <c r="D126" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E126" s="49"/>
+      <c r="E126" s="39"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" s="49"/>
+      <c r="A127" s="39"/>
       <c r="B127" s="25" t="s">
         <v>204</v>
       </c>
@@ -3126,10 +3133,10 @@
       <c r="D127" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E127" s="49"/>
+      <c r="E127" s="39"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" s="49"/>
+      <c r="A128" s="39"/>
       <c r="B128" s="35" t="s">
         <v>205</v>
       </c>
@@ -3139,10 +3146,10 @@
       <c r="D128" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E128" s="49"/>
+      <c r="E128" s="39"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" s="49"/>
+      <c r="A129" s="39"/>
       <c r="B129" s="25" t="s">
         <v>206</v>
       </c>
@@ -3152,10 +3159,10 @@
       <c r="D129" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E129" s="49"/>
+      <c r="E129" s="39"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" s="49"/>
+      <c r="A130" s="39"/>
       <c r="B130" s="35" t="s">
         <v>207</v>
       </c>
@@ -3165,7 +3172,7 @@
       <c r="D130" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E130" s="49"/>
+      <c r="E130" s="39"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="36"/>
@@ -3214,26 +3221,16 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="A125:A130"/>
-    <mergeCell ref="E125:E130"/>
-    <mergeCell ref="A113:A114"/>
-    <mergeCell ref="E113:E114"/>
-    <mergeCell ref="A116:A120"/>
-    <mergeCell ref="E116:E120"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="E105:E108"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="E111:E112"/>
-    <mergeCell ref="E93:E98"/>
-    <mergeCell ref="A93:A98"/>
-    <mergeCell ref="E99:E104"/>
-    <mergeCell ref="A99:A104"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="E83:E84"/>
-    <mergeCell ref="A85:A89"/>
-    <mergeCell ref="E85:E89"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="E75:E77"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A5:A13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A31:A43"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E5:E25"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="E31:E43"/>
+    <mergeCell ref="E44:E49"/>
     <mergeCell ref="E62:E68"/>
     <mergeCell ref="A78:A81"/>
     <mergeCell ref="E78:E81"/>
@@ -3246,16 +3243,26 @@
     <mergeCell ref="A62:A68"/>
     <mergeCell ref="A73:A74"/>
     <mergeCell ref="E73:E74"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="E5:E25"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="E31:E43"/>
-    <mergeCell ref="E44:E49"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A5:A13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A31:A43"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="E83:E84"/>
+    <mergeCell ref="A85:A89"/>
+    <mergeCell ref="E85:E89"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="E75:E77"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="E105:E108"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="E111:E112"/>
+    <mergeCell ref="E93:E98"/>
+    <mergeCell ref="A93:A98"/>
+    <mergeCell ref="E99:E104"/>
+    <mergeCell ref="A99:A104"/>
+    <mergeCell ref="A125:A130"/>
+    <mergeCell ref="E125:E130"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="E113:E114"/>
+    <mergeCell ref="A116:A120"/>
+    <mergeCell ref="E116:E120"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{D01E85B4-1DB0-475A-87DE-364916E7DA22}"/>

</xml_diff>

<commit_message>
Integrated SOC style artifacts
</commit_message>
<xml_diff>
--- a/development/Integrated Mods.xlsx
+++ b/development/Integrated Mods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\S.T.A.L.K.E.R\Anomaly Mods\mods\Back-to-roots-wip\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6842C31B-B544-4179-BB05-EED7D9A4037F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1485D046-8EF0-4A41-801D-50553090E024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="214">
   <si>
     <t>Filename</t>
   </si>
@@ -669,6 +669,15 @@
   </si>
   <si>
     <t>mod_system_actor1.ltx</t>
+  </si>
+  <si>
+    <t>SOC Style Artifacts</t>
+  </si>
+  <si>
+    <t>mod_system_soclikearts.ltx</t>
+  </si>
+  <si>
+    <t>MaxSpringer</t>
   </si>
 </sst>
 </file>
@@ -1350,8 +1359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8700934C-DA8F-46A3-9CCC-A5B0203FB02B}">
   <dimension ref="A1:E135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E121" sqref="E121"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A132" sqref="A132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3184,13 +3193,21 @@
       <c r="E131" s="33"/>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" s="37"/>
-      <c r="B132" s="35"/>
-      <c r="C132" s="7"/>
+      <c r="A132" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="B132" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="C132" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="D132" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E132" s="32"/>
+      <c r="E132" s="32" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="26"/>

</xml_diff>

<commit_message>
Added authors for all mods
</commit_message>
<xml_diff>
--- a/development/Integrated Mods.xlsx
+++ b/development/Integrated Mods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\S.T.A.L.K.E.R\Anomaly Mods\mods\Back-to-roots-wip\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1485D046-8EF0-4A41-801D-50553090E024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAC2F3F-F08B-4713-B28C-D1D4F294A489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="217">
   <si>
     <t>Filename</t>
   </si>
@@ -678,6 +678,15 @@
   </si>
   <si>
     <t>MaxSpringer</t>
+  </si>
+  <si>
+    <t>dEmergence</t>
+  </si>
+  <si>
+    <t>Mirci33sClone</t>
+  </si>
+  <si>
+    <t>NewbieRus</t>
   </si>
 </sst>
 </file>
@@ -900,9 +909,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -947,7 +955,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -959,44 +966,11 @@
     <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1021,6 +995,34 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1357,16 +1359,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8700934C-DA8F-46A3-9CCC-A5B0203FB02B}">
-  <dimension ref="A1:E135"/>
+  <dimension ref="A1:E134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A132" sqref="A132"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="48.5703125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="48.5703125" style="20" customWidth="1"/>
     <col min="3" max="3" width="36.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" customWidth="1"/>
@@ -1374,1867 +1376,1870 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="51" t="s">
+      <c r="D2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="38" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="16" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="48"/>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="35"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="11" t="s">
+      <c r="C4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="48" t="s">
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="35" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="32"/>
+      <c r="B6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="48"/>
+      <c r="C6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="35"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
-      <c r="B7" s="16" t="s">
+      <c r="A7" s="32"/>
+      <c r="B7" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="48"/>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="35"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="32"/>
+      <c r="B8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="48"/>
+      <c r="D8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="35"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
-      <c r="B9" s="16" t="s">
+      <c r="A9" s="32"/>
+      <c r="B9" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="48"/>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="35"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
-      <c r="B10" s="15" t="s">
+      <c r="A10" s="32"/>
+      <c r="B10" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="48"/>
+      <c r="D10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="35"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
-      <c r="B11" s="16" t="s">
+      <c r="A11" s="32"/>
+      <c r="B11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="48"/>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="35"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
-      <c r="B12" s="15" t="s">
+      <c r="A12" s="32"/>
+      <c r="B12" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="48"/>
+      <c r="D12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="35"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
-      <c r="B13" s="16" t="s">
+      <c r="A13" s="32"/>
+      <c r="B13" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="48"/>
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="35"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="48"/>
+      <c r="D14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="35"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
-      <c r="B15" s="16" t="s">
+      <c r="A15" s="34"/>
+      <c r="B15" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="48"/>
+      <c r="C15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="35"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
-      <c r="B16" s="15" t="s">
+      <c r="A16" s="34"/>
+      <c r="B16" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="48"/>
+      <c r="C16" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="35"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
-      <c r="B17" s="16" t="s">
+      <c r="A17" s="34"/>
+      <c r="B17" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="48"/>
+      <c r="D17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="35"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
-      <c r="B18" s="15" t="s">
+      <c r="A18" s="34"/>
+      <c r="B18" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="48"/>
+      <c r="D18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="35"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
-      <c r="B19" s="16" t="s">
+      <c r="A19" s="34"/>
+      <c r="B19" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="48"/>
+      <c r="D19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="35"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="15" t="s">
+      <c r="A20" s="34"/>
+      <c r="B20" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="48"/>
+      <c r="D20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="35"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
-      <c r="B21" s="16" t="s">
+      <c r="A21" s="34"/>
+      <c r="B21" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="48"/>
+      <c r="E21" s="35"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
-      <c r="B22" s="15" t="s">
+      <c r="A22" s="34"/>
+      <c r="B22" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="48"/>
+      <c r="D22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="35"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="47"/>
-      <c r="B23" s="16" t="s">
+      <c r="A23" s="34"/>
+      <c r="B23" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="48"/>
+      <c r="D23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="35"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="15" t="s">
+      <c r="A24" s="34"/>
+      <c r="B24" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="48"/>
+      <c r="D24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="35"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
-      <c r="B25" s="16" t="s">
+      <c r="A25" s="34"/>
+      <c r="B25" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="48"/>
+      <c r="D25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="35"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="11" t="s">
+      <c r="C26" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="10" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="47" t="s">
+      <c r="A27" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="48" t="s">
+      <c r="D27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="35" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
-      <c r="B28" s="18" t="s">
+      <c r="A28" s="34"/>
+      <c r="B28" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="D28" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="48"/>
+      <c r="D28" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="35"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
-      <c r="B29" s="17" t="s">
+      <c r="A29" s="34"/>
+      <c r="B29" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="48"/>
+      <c r="D29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="35"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="11" t="s">
+      <c r="D30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="10" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="48" t="s">
+      <c r="D31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="35" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="47"/>
-      <c r="B32" s="15" t="s">
+      <c r="A32" s="34"/>
+      <c r="B32" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="48"/>
+      <c r="D32" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="35"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
-      <c r="B33" s="19" t="s">
+      <c r="A33" s="34"/>
+      <c r="B33" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="49" t="s">
+      <c r="C33" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="48"/>
+      <c r="E33" s="35"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="47"/>
-      <c r="B34" s="20" t="s">
+      <c r="A34" s="34"/>
+      <c r="B34" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="49"/>
-      <c r="D34" s="22" t="s">
+      <c r="C34" s="36"/>
+      <c r="D34" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="48"/>
+      <c r="E34" s="35"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="47"/>
-      <c r="B35" s="19" t="s">
+      <c r="A35" s="34"/>
+      <c r="B35" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="49"/>
-      <c r="D35" s="14" t="s">
+      <c r="C35" s="36"/>
+      <c r="D35" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E35" s="48"/>
+      <c r="E35" s="35"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
-      <c r="B36" s="20" t="s">
+      <c r="A36" s="34"/>
+      <c r="B36" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="49"/>
-      <c r="D36" s="22" t="s">
+      <c r="C36" s="36"/>
+      <c r="D36" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="48"/>
+      <c r="E36" s="35"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="47"/>
-      <c r="B37" s="16" t="s">
+      <c r="A37" s="34"/>
+      <c r="B37" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="48"/>
+      <c r="D37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="35"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="47"/>
-      <c r="B38" s="15" t="s">
+      <c r="A38" s="34"/>
+      <c r="B38" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="48"/>
+      <c r="C38" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="35"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="47"/>
-      <c r="B39" s="16" t="s">
+      <c r="A39" s="34"/>
+      <c r="B39" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C39" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="48"/>
+      <c r="C39" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="35"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="47"/>
-      <c r="B40" s="15" t="s">
+      <c r="A40" s="34"/>
+      <c r="B40" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="48"/>
+      <c r="C40" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="35"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="47"/>
-      <c r="B41" s="16" t="s">
+      <c r="A41" s="34"/>
+      <c r="B41" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" s="48"/>
+      <c r="C41" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="35"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="47"/>
-      <c r="B42" s="18" t="s">
+      <c r="A42" s="34"/>
+      <c r="B42" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D42" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" s="48"/>
+      <c r="D42" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="35"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="47"/>
-      <c r="B43" s="16" t="s">
+      <c r="A43" s="34"/>
+      <c r="B43" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" s="48"/>
+      <c r="D43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="35"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="45" t="s">
+      <c r="A44" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D44" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="46" t="s">
+      <c r="D44" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="33" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="45"/>
-      <c r="B45" s="16" t="s">
+      <c r="A45" s="32"/>
+      <c r="B45" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="46"/>
+      <c r="D45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="33"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="45"/>
-      <c r="B46" s="15" t="s">
+      <c r="A46" s="32"/>
+      <c r="B46" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="46"/>
+      <c r="D46" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="33"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="45"/>
-      <c r="B47" s="16" t="s">
+      <c r="A47" s="32"/>
+      <c r="B47" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="46"/>
+      <c r="D47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="33"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="45"/>
-      <c r="B48" s="15" t="s">
+      <c r="A48" s="32"/>
+      <c r="B48" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C48" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" s="46"/>
+      <c r="C48" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="33"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="45"/>
-      <c r="B49" s="16" t="s">
+      <c r="A49" s="32"/>
+      <c r="B49" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C49" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" s="46"/>
+      <c r="C49" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="33"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C50" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E50" s="12" t="s">
+      <c r="C50" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="11" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="45" t="s">
+      <c r="A51" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="16" t="s">
+      <c r="B51" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C51" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E51" s="46" t="s">
+      <c r="D51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="33" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="45"/>
-      <c r="B52" s="15" t="s">
+      <c r="A52" s="32"/>
+      <c r="B52" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D52" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E52" s="46"/>
+      <c r="D52" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="33"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="45"/>
-      <c r="B53" s="16" t="s">
+      <c r="A53" s="32"/>
+      <c r="B53" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="46"/>
+      <c r="D53" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="33"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="45"/>
-      <c r="B54" s="15" t="s">
+      <c r="A54" s="32"/>
+      <c r="B54" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C54" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D54" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E54" s="46"/>
+      <c r="D54" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="33"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="45"/>
-      <c r="B55" s="16" t="s">
+      <c r="A55" s="32"/>
+      <c r="B55" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E55" s="46"/>
+      <c r="D55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="33"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="45"/>
-      <c r="B56" s="15" t="s">
+      <c r="A56" s="32"/>
+      <c r="B56" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C56" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E56" s="46"/>
+      <c r="C56" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="33"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="45"/>
-      <c r="B57" s="16" t="s">
+      <c r="A57" s="32"/>
+      <c r="B57" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C57" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E57" s="46"/>
+      <c r="C57" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="33"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="45"/>
-      <c r="B58" s="15" t="s">
+      <c r="A58" s="32"/>
+      <c r="B58" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C58" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E58" s="46"/>
+      <c r="C58" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="33"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="45"/>
-      <c r="B59" s="16" t="s">
+      <c r="A59" s="32"/>
+      <c r="B59" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C59" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E59" s="46"/>
+      <c r="C59" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="33"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="45"/>
-      <c r="B60" s="15" t="s">
+      <c r="A60" s="32"/>
+      <c r="B60" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="C60" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D60" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E60" s="46"/>
+      <c r="D60" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="33"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
+      <c r="A61" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B61" s="16" t="s">
+      <c r="B61" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E61" s="12" t="s">
+      <c r="D61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="11" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="45" t="s">
+      <c r="A62" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C62" s="8" t="s">
+      <c r="C62" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D62" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E62" s="46" t="s">
+      <c r="D62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="33" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="45"/>
-      <c r="B63" s="16" t="s">
+      <c r="A63" s="32"/>
+      <c r="B63" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="C63" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E63" s="46"/>
+      <c r="C63" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="33"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="45"/>
-      <c r="B64" s="15" t="s">
+      <c r="A64" s="32"/>
+      <c r="B64" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="C64" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E64" s="46"/>
+      <c r="C64" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="33"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="45"/>
-      <c r="B65" s="16" t="s">
+      <c r="A65" s="32"/>
+      <c r="B65" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C65" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E65" s="46"/>
+      <c r="C65" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="33"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="45"/>
-      <c r="B66" s="15" t="s">
+      <c r="A66" s="32"/>
+      <c r="B66" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="C66" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E66" s="46"/>
+      <c r="C66" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" s="33"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="45"/>
-      <c r="B67" s="16" t="s">
+      <c r="A67" s="32"/>
+      <c r="B67" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C67" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E67" s="46"/>
+      <c r="C67" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="33"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="45"/>
-      <c r="B68" s="15" t="s">
+      <c r="A68" s="32"/>
+      <c r="B68" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="C68" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E68" s="46"/>
+      <c r="C68" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="33"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="9" t="s">
+      <c r="A69" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B69" s="16" t="s">
+      <c r="B69" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C69" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E69" s="12" t="s">
+      <c r="C69" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" s="11" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="10" t="s">
+      <c r="A70" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B70" s="15" t="s">
+      <c r="B70" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C70" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E70" s="11" t="s">
+      <c r="C70" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" s="10" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="9" t="s">
+      <c r="A71" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B71" s="16" t="s">
+      <c r="B71" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C71" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E71" s="12" t="s">
+      <c r="C71" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" s="11" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="10" t="s">
+      <c r="A72" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B72" s="50" t="s">
+      <c r="B72" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="C72" s="49" t="s">
+      <c r="C72" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="D72" s="22" t="s">
+      <c r="D72" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E72" s="11" t="s">
+      <c r="E72" s="10" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="47" t="s">
+      <c r="A73" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="B73" s="50"/>
-      <c r="C73" s="49"/>
-      <c r="D73" s="14" t="s">
+      <c r="B73" s="37"/>
+      <c r="C73" s="36"/>
+      <c r="D73" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E73" s="48" t="s">
+      <c r="E73" s="35" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="47"/>
-      <c r="B74" s="31" t="s">
+      <c r="A74" s="34"/>
+      <c r="B74" s="29" t="s">
         <v>194</v>
       </c>
-      <c r="C74" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D74" s="14" t="s">
+      <c r="C74" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D74" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E74" s="48"/>
+      <c r="E74" s="35"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="45" t="s">
+      <c r="A75" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="B75" s="23" t="s">
+      <c r="B75" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="C75" s="8" t="s">
+      <c r="C75" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="D75" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E75" s="46" t="s">
+      <c r="D75" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E75" s="33" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="45"/>
-      <c r="B76" s="16" t="s">
+      <c r="A76" s="32"/>
+      <c r="B76" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="C76" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E76" s="46"/>
+      <c r="C76" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" s="33"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="45"/>
-      <c r="B77" s="15" t="s">
+      <c r="A77" s="32"/>
+      <c r="B77" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="C77" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E77" s="46"/>
+      <c r="C77" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" s="33"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="47" t="s">
+      <c r="A78" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="B78" s="16" t="s">
+      <c r="B78" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="C78" s="7" t="s">
+      <c r="C78" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D78" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E78" s="48" t="s">
+      <c r="D78" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" s="35" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="47"/>
-      <c r="B79" s="15" t="s">
+      <c r="A79" s="34"/>
+      <c r="B79" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="C79" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E79" s="48"/>
+      <c r="C79" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79" s="35"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="47"/>
-      <c r="B80" s="16" t="s">
+      <c r="A80" s="34"/>
+      <c r="B80" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C80" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E80" s="48"/>
+      <c r="C80" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80" s="35"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="47"/>
-      <c r="B81" s="15" t="s">
+      <c r="A81" s="34"/>
+      <c r="B81" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="C81" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E81" s="48"/>
+      <c r="C81" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" s="35"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="10" t="s">
+      <c r="A82" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="B82" s="24" t="s">
+      <c r="B82" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="C82" s="7" t="s">
+      <c r="C82" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="D82" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E82" s="1" t="s">
+      <c r="D82" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" s="10" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="44" t="s">
+      <c r="A83" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="B83" s="25" t="s">
+      <c r="B83" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C83" s="8" t="s">
+      <c r="C83" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="D83" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E83" s="39" t="s">
+      <c r="D83" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" s="35" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="44"/>
-      <c r="B84" s="24" t="s">
+      <c r="A84" s="34"/>
+      <c r="B84" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="C84" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E84" s="39"/>
+      <c r="C84" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E84" s="35"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="42" t="s">
+      <c r="A85" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="B85" s="25" t="s">
+      <c r="B85" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="C85" s="8" t="s">
+      <c r="C85" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D85" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E85" s="40" t="s">
+      <c r="D85" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E85" s="33" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="42"/>
-      <c r="B86" s="24" t="s">
+      <c r="A86" s="32"/>
+      <c r="B86" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="C86" s="7" t="s">
+      <c r="C86" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D86" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E86" s="40"/>
+      <c r="D86" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E86" s="33"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="42"/>
-      <c r="B87" s="25" t="s">
+      <c r="A87" s="32"/>
+      <c r="B87" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="C87" s="8" t="s">
+      <c r="C87" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D87" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E87" s="40"/>
+      <c r="D87" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E87" s="33"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="42"/>
-      <c r="B88" s="24" t="s">
+      <c r="A88" s="32"/>
+      <c r="B88" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="C88" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D88" s="14" t="s">
+      <c r="C88" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D88" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E88" s="40"/>
+      <c r="E88" s="33"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="42"/>
-      <c r="B89" s="18" t="s">
+      <c r="A89" s="32"/>
+      <c r="B89" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="C89" s="8" t="s">
+      <c r="C89" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="D89" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E89" s="40"/>
+      <c r="D89" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E89" s="33"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="9" t="s">
+      <c r="A90" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="B90" s="17" t="s">
+      <c r="B90" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="C90" s="7" t="s">
+      <c r="C90" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D90" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E90" s="26" t="s">
+      <c r="D90" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E90" s="11" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="10" t="s">
+      <c r="A91" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="B91" s="18" t="s">
+      <c r="B91" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="C91" s="8" t="s">
+      <c r="C91" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D91" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E91" s="1" t="s">
+      <c r="D91" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E91" s="10" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="9" t="s">
+      <c r="A92" s="45" t="s">
         <v>145</v>
       </c>
-      <c r="B92" s="24" t="s">
+      <c r="B92" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="C92" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E92" s="26" t="s">
+      <c r="C92" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E92" s="11" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="42" t="s">
+      <c r="A93" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="B93" s="25" t="s">
+      <c r="B93" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="C93" s="8" t="s">
+      <c r="C93" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="D93" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E93" s="40" t="s">
+      <c r="D93" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E93" s="33" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="42"/>
-      <c r="B94" s="24" t="s">
+      <c r="A94" s="32"/>
+      <c r="B94" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="C94" s="7" t="s">
+      <c r="C94" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D94" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E94" s="40"/>
+      <c r="D94" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E94" s="33"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="42"/>
-      <c r="B95" s="25" t="s">
+      <c r="A95" s="32"/>
+      <c r="B95" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="C95" s="8" t="s">
+      <c r="C95" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D95" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E95" s="40"/>
+      <c r="D95" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E95" s="33"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="42"/>
-      <c r="B96" s="24" t="s">
+      <c r="A96" s="32"/>
+      <c r="B96" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="C96" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E96" s="40"/>
+      <c r="C96" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E96" s="33"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="42"/>
-      <c r="B97" s="25" t="s">
+      <c r="A97" s="32"/>
+      <c r="B97" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="C97" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D97" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E97" s="40"/>
+      <c r="C97" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E97" s="33"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="42"/>
-      <c r="B98" s="24" t="s">
+      <c r="A98" s="32"/>
+      <c r="B98" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="C98" s="7" t="s">
+      <c r="C98" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D98" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E98" s="40"/>
+      <c r="D98" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E98" s="33"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="44" t="s">
+      <c r="A99" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="B99" s="25" t="s">
+      <c r="B99" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="C99" s="8" t="s">
+      <c r="C99" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D99" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E99" s="39" t="s">
+      <c r="D99" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E99" s="35" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="44"/>
-      <c r="B100" s="24" t="s">
+      <c r="A100" s="34"/>
+      <c r="B100" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="C100" s="7" t="s">
+      <c r="C100" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D100" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E100" s="39"/>
+      <c r="D100" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E100" s="35"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="44"/>
-      <c r="B101" s="25" t="s">
+      <c r="A101" s="34"/>
+      <c r="B101" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="C101" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D101" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E101" s="39"/>
+      <c r="C101" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E101" s="35"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="44"/>
-      <c r="B102" s="24" t="s">
+      <c r="A102" s="34"/>
+      <c r="B102" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="C102" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E102" s="39"/>
+      <c r="C102" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E102" s="35"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="44"/>
-      <c r="B103" s="25" t="s">
+      <c r="A103" s="34"/>
+      <c r="B103" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="C103" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D103" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E103" s="39"/>
+      <c r="C103" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E103" s="35"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="44"/>
-      <c r="B104" s="17" t="s">
+      <c r="A104" s="34"/>
+      <c r="B104" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="C104" s="7" t="s">
+      <c r="C104" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="D104" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E104" s="39"/>
+      <c r="D104" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E104" s="35"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="42" t="s">
+      <c r="A105" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="B105" s="25" t="s">
+      <c r="B105" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="C105" s="8" t="s">
+      <c r="C105" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D105" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E105" s="40" t="s">
+      <c r="D105" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" s="33" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="42"/>
-      <c r="B106" s="24" t="s">
+      <c r="A106" s="32"/>
+      <c r="B106" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="C106" s="7" t="s">
+      <c r="C106" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D106" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E106" s="40"/>
+      <c r="D106" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E106" s="33"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="42"/>
-      <c r="B107" s="25" t="s">
+      <c r="A107" s="32"/>
+      <c r="B107" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="C107" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D107" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E107" s="40"/>
+      <c r="C107" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E107" s="33"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="42"/>
-      <c r="B108" s="24" t="s">
+      <c r="A108" s="32"/>
+      <c r="B108" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="C108" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E108" s="40"/>
+      <c r="C108" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E108" s="33"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="9" t="s">
+      <c r="A109" s="45" t="s">
         <v>174</v>
       </c>
-      <c r="B109" s="25" t="s">
+      <c r="B109" s="24" t="s">
         <v>176</v>
       </c>
-      <c r="C109" s="8" t="s">
+      <c r="C109" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="D109" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E109" s="33" t="s">
+      <c r="D109" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E109" s="40" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+      <c r="A110" s="46" t="s">
         <v>179</v>
       </c>
-      <c r="B110" s="24" t="s">
+      <c r="B110" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="C110" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E110" s="32"/>
+      <c r="C110" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E110" s="41" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="39" t="s">
+      <c r="A111" s="47" t="s">
         <v>180</v>
       </c>
-      <c r="B111" s="25" t="s">
+      <c r="B111" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="C111" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D111" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E111" s="43"/>
+      <c r="C111" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E111" s="35" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="39"/>
-      <c r="B112" s="24" t="s">
+      <c r="A112" s="47"/>
+      <c r="B112" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="C112" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D112" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E112" s="43"/>
+      <c r="C112" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E112" s="35"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="40" t="s">
+      <c r="A113" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="B113" s="34" t="s">
+      <c r="B113" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="C113" s="8" t="s">
+      <c r="C113" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="D113" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E113" s="41"/>
+      <c r="D113" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E113" s="33" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="40"/>
-      <c r="B114" s="35" t="s">
+      <c r="A114" s="48"/>
+      <c r="B114" s="31" t="s">
         <v>186</v>
       </c>
-      <c r="C114" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E114" s="41"/>
+      <c r="C114" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E114" s="33"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="26" t="s">
+      <c r="A115" s="49" t="s">
         <v>188</v>
       </c>
-      <c r="B115" s="25" t="s">
+      <c r="B115" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="C115" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D115" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E115" s="26"/>
+      <c r="C115" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E115" s="11" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="40" t="s">
+      <c r="A116" s="48" t="s">
         <v>189</v>
       </c>
-      <c r="B116" s="35" t="s">
+      <c r="B116" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="C116" s="7" t="s">
+      <c r="C116" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D116" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E116" s="41"/>
+      <c r="D116" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E116" s="33" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" s="40"/>
-      <c r="B117" s="25" t="s">
+      <c r="A117" s="48"/>
+      <c r="B117" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="C117" s="8" t="s">
+      <c r="C117" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D117" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E117" s="41"/>
+      <c r="D117" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E117" s="33"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="40"/>
-      <c r="B118" s="35" t="s">
+      <c r="A118" s="48"/>
+      <c r="B118" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="C118" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D118" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E118" s="41"/>
+      <c r="C118" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E118" s="33"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="40"/>
-      <c r="B119" s="25" t="s">
+      <c r="A119" s="48"/>
+      <c r="B119" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="C119" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D119" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E119" s="41"/>
+      <c r="C119" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E119" s="33"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" s="40"/>
-      <c r="B120" s="35" t="s">
+      <c r="A120" s="48"/>
+      <c r="B120" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="C120" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D120" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E120" s="41"/>
+      <c r="C120" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E120" s="33"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" s="26" t="s">
+      <c r="A121" s="49" t="s">
         <v>195</v>
       </c>
-      <c r="B121" s="25" t="s">
+      <c r="B121" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="C121" s="8" t="s">
+      <c r="C121" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D121" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E121" s="26"/>
+      <c r="D121" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E121" s="11" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="37" t="s">
+      <c r="A122" s="50" t="s">
         <v>197</v>
       </c>
-      <c r="B122" s="35" t="s">
+      <c r="B122" s="31" t="s">
         <v>199</v>
       </c>
-      <c r="C122" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D122" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E122" s="32" t="s">
+      <c r="C122" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E122" s="41" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" s="38"/>
-      <c r="B123" s="25"/>
-      <c r="C123" s="8"/>
-      <c r="D123" s="6"/>
-      <c r="E123" s="33"/>
+      <c r="A123" s="51"/>
+      <c r="B123" s="24"/>
+      <c r="C123" s="7"/>
+      <c r="D123" s="5"/>
+      <c r="E123" s="40"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" s="37"/>
-      <c r="B124" s="35"/>
-      <c r="C124" s="7"/>
-      <c r="D124" s="6"/>
-      <c r="E124" s="32"/>
+      <c r="A124" s="50"/>
+      <c r="B124" s="31"/>
+      <c r="C124" s="6"/>
+      <c r="D124" s="5"/>
+      <c r="E124" s="41"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" s="39" t="s">
+      <c r="A125" s="47" t="s">
         <v>200</v>
       </c>
-      <c r="B125" s="25" t="s">
+      <c r="B125" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="C125" s="8" t="s">
+      <c r="C125" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="D125" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E125" s="39" t="s">
+      <c r="D125" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E125" s="35" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="39"/>
-      <c r="B126" s="35" t="s">
+      <c r="A126" s="47"/>
+      <c r="B126" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="C126" s="7" t="s">
+      <c r="C126" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="D126" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E126" s="39"/>
+      <c r="D126" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E126" s="35"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" s="39"/>
-      <c r="B127" s="25" t="s">
+      <c r="A127" s="47"/>
+      <c r="B127" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="C127" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D127" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E127" s="39"/>
+      <c r="C127" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D127" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E127" s="35"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" s="39"/>
-      <c r="B128" s="35" t="s">
+      <c r="A128" s="47"/>
+      <c r="B128" s="31" t="s">
         <v>205</v>
       </c>
-      <c r="C128" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D128" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E128" s="39"/>
+      <c r="C128" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D128" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E128" s="35"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" s="39"/>
-      <c r="B129" s="25" t="s">
+      <c r="A129" s="47"/>
+      <c r="B129" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="C129" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D129" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E129" s="39"/>
+      <c r="C129" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D129" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E129" s="35"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" s="39"/>
-      <c r="B130" s="35" t="s">
+      <c r="A130" s="47"/>
+      <c r="B130" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="C130" s="7" t="s">
+      <c r="C130" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="D130" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E130" s="39"/>
+      <c r="D130" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E130" s="35"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" s="36"/>
-      <c r="B131" s="25"/>
-      <c r="C131" s="8"/>
-      <c r="D131" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E131" s="33"/>
+      <c r="A131" s="50" t="s">
+        <v>211</v>
+      </c>
+      <c r="B131" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="C131" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D131" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E131" s="41" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" s="37" t="s">
-        <v>211</v>
-      </c>
-      <c r="B132" s="35" t="s">
-        <v>212</v>
-      </c>
-      <c r="C132" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D132" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E132" s="32" t="s">
-        <v>213</v>
-      </c>
+      <c r="A132" s="49"/>
+      <c r="B132" s="24"/>
+      <c r="C132" s="7"/>
+      <c r="D132" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E132" s="40"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" s="26"/>
-      <c r="B133" s="25"/>
-      <c r="C133" s="8"/>
-      <c r="D133" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E133" s="33"/>
+      <c r="A133" s="50"/>
+      <c r="B133" s="31"/>
+      <c r="C133" s="6"/>
+      <c r="D133" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E133" s="41"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" s="37"/>
-      <c r="B134" s="35"/>
+      <c r="A134" s="49"/>
+      <c r="B134" s="24"/>
       <c r="C134" s="7"/>
-      <c r="D134" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E134" s="32"/>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" s="26"/>
-      <c r="B135" s="25"/>
-      <c r="C135" s="8"/>
-      <c r="D135" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E135" s="33"/>
+      <c r="D134" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E134" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="42">

</xml_diff>

<commit_message>
Integrated several mods (fixes mostly)
</commit_message>
<xml_diff>
--- a/development/Integrated Mods.xlsx
+++ b/development/Integrated Mods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\S.T.A.L.K.E.R\Anomaly Mods\mods\Back-to-roots-wip\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD683483-6053-48E3-8291-05C9A9673308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56A5223-83A0-461D-8259-8029877BFA3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65B4BA79-B472-4E31-A68E-8412999619D4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="260">
   <si>
     <t>Filename</t>
   </si>
@@ -723,6 +723,99 @@
   </si>
   <si>
     <t>MissingnoBW</t>
+  </si>
+  <si>
+    <t>Pray For The Monolith To Heal</t>
+  </si>
+  <si>
+    <t>Kutee</t>
+  </si>
+  <si>
+    <t>pray_monolith.script</t>
+  </si>
+  <si>
+    <t>pray_ui.xml</t>
+  </si>
+  <si>
+    <t>configs/ui</t>
+  </si>
+  <si>
+    <t>Nagant 1887 Revolver</t>
+  </si>
+  <si>
+    <t>JMerc75</t>
+  </si>
+  <si>
+    <t>w_n1895.ltx</t>
+  </si>
+  <si>
+    <t>configs/items/weapons</t>
+  </si>
+  <si>
+    <t>st_wpn_n1887_j.xml</t>
+  </si>
+  <si>
+    <t>meshes/</t>
+  </si>
+  <si>
+    <t>(Bunch of meshes)</t>
+  </si>
+  <si>
+    <t>sounds/weapons/n1887_j</t>
+  </si>
+  <si>
+    <t>(Bunch of sounds)</t>
+  </si>
+  <si>
+    <t>(Bunch of textures)</t>
+  </si>
+  <si>
+    <t>Dark signal stand weapon audio</t>
+  </si>
+  <si>
+    <t>Shr¡ke</t>
+  </si>
+  <si>
+    <t>weapon_sounds.ltx</t>
+  </si>
+  <si>
+    <t>configs/items/weapons/sound_layers</t>
+  </si>
+  <si>
+    <t>wpn_ar_sounds.ltx</t>
+  </si>
+  <si>
+    <t>wpn_explosion_sounds.ltx</t>
+  </si>
+  <si>
+    <t>wpn_lmg_sounds.ltx</t>
+  </si>
+  <si>
+    <t>wpn_pistol_sounds.ltx</t>
+  </si>
+  <si>
+    <t>wpn_rifle_sounds.ltx</t>
+  </si>
+  <si>
+    <t>wpn_sd_sounds.ltx</t>
+  </si>
+  <si>
+    <t>wpn_sd_upgraded_sounds.ltx</t>
+  </si>
+  <si>
+    <t>wpn_shotgun_sounds.ltx</t>
+  </si>
+  <si>
+    <t>wpn_smg_sounds.ltx</t>
+  </si>
+  <si>
+    <t>wpn_sniper_sounds.ltx</t>
+  </si>
+  <si>
+    <t>sounds/material/bullet/collide/</t>
+  </si>
+  <si>
+    <t>sounds/weapons/</t>
   </si>
 </sst>
 </file>
@@ -945,7 +1038,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -1030,6 +1123,37 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1045,9 +1169,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1057,17 +1178,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1403,10 +1513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8700934C-DA8F-46A3-9CCC-A5B0203FB02B}">
-  <dimension ref="A1:E142"/>
+  <dimension ref="A1:E250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C137" sqref="C137"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D156" sqref="D156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,7 +1547,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="55" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -1449,12 +1559,12 @@
       <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="58" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="43"/>
+      <c r="A3" s="56"/>
       <c r="B3" s="15" t="s">
         <v>12</v>
       </c>
@@ -1464,7 +1574,7 @@
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="46"/>
+      <c r="E3" s="59"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1484,7 +1594,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="56" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="16" t="s">
@@ -1496,12 +1606,12 @@
       <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="59" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
+      <c r="A6" s="56"/>
       <c r="B6" s="14" t="s">
         <v>20</v>
       </c>
@@ -1511,10 +1621,10 @@
       <c r="D6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="46"/>
+      <c r="E6" s="59"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="15" t="s">
         <v>22</v>
       </c>
@@ -1524,10 +1634,10 @@
       <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="46"/>
+      <c r="E7" s="59"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
+      <c r="A8" s="56"/>
       <c r="B8" s="14" t="s">
         <v>23</v>
       </c>
@@ -1537,10 +1647,10 @@
       <c r="D8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="46"/>
+      <c r="E8" s="59"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
+      <c r="A9" s="56"/>
       <c r="B9" s="15" t="s">
         <v>24</v>
       </c>
@@ -1550,10 +1660,10 @@
       <c r="D9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="46"/>
+      <c r="E9" s="59"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="14" t="s">
         <v>25</v>
       </c>
@@ -1563,10 +1673,10 @@
       <c r="D10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="46"/>
+      <c r="E10" s="59"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
+      <c r="A11" s="56"/>
       <c r="B11" s="15" t="s">
         <v>26</v>
       </c>
@@ -1576,10 +1686,10 @@
       <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="46"/>
+      <c r="E11" s="59"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
+      <c r="A12" s="56"/>
       <c r="B12" s="14" t="s">
         <v>25</v>
       </c>
@@ -1589,10 +1699,10 @@
       <c r="D12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="59"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
+      <c r="A13" s="56"/>
       <c r="B13" s="15" t="s">
         <v>26</v>
       </c>
@@ -1602,10 +1712,10 @@
       <c r="D13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="46"/>
+      <c r="E13" s="59"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="57" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="17" t="s">
@@ -1617,10 +1727,10 @@
       <c r="D14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="46"/>
+      <c r="E14" s="59"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="57"/>
       <c r="B15" s="15" t="s">
         <v>31</v>
       </c>
@@ -1630,10 +1740,10 @@
       <c r="D15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="46"/>
+      <c r="E15" s="59"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
+      <c r="A16" s="57"/>
       <c r="B16" s="14" t="s">
         <v>32</v>
       </c>
@@ -1643,10 +1753,10 @@
       <c r="D16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="46"/>
+      <c r="E16" s="59"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
+      <c r="A17" s="57"/>
       <c r="B17" s="15" t="s">
         <v>33</v>
       </c>
@@ -1656,10 +1766,10 @@
       <c r="D17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="46"/>
+      <c r="E17" s="59"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="57"/>
       <c r="B18" s="14" t="s">
         <v>34</v>
       </c>
@@ -1669,10 +1779,10 @@
       <c r="D18" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="46"/>
+      <c r="E18" s="59"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="57"/>
       <c r="B19" s="15" t="s">
         <v>35</v>
       </c>
@@ -1682,10 +1792,10 @@
       <c r="D19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="46"/>
+      <c r="E19" s="59"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="57"/>
       <c r="B20" s="14" t="s">
         <v>36</v>
       </c>
@@ -1695,10 +1805,10 @@
       <c r="D20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="46"/>
+      <c r="E20" s="59"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
+      <c r="A21" s="57"/>
       <c r="B21" s="15" t="s">
         <v>37</v>
       </c>
@@ -1708,10 +1818,10 @@
       <c r="D21" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="46"/>
+      <c r="E21" s="59"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
+      <c r="A22" s="57"/>
       <c r="B22" s="14" t="s">
         <v>38</v>
       </c>
@@ -1721,10 +1831,10 @@
       <c r="D22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="46"/>
+      <c r="E22" s="59"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="57"/>
       <c r="B23" s="15" t="s">
         <v>39</v>
       </c>
@@ -1734,10 +1844,10 @@
       <c r="D23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="46"/>
+      <c r="E23" s="59"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
+      <c r="A24" s="57"/>
       <c r="B24" s="14" t="s">
         <v>40</v>
       </c>
@@ -1747,10 +1857,10 @@
       <c r="D24" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="46"/>
+      <c r="E24" s="59"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
+      <c r="A25" s="57"/>
       <c r="B25" s="15" t="s">
         <v>40</v>
       </c>
@@ -1760,7 +1870,7 @@
       <c r="D25" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="46"/>
+      <c r="E25" s="59"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
@@ -1780,7 +1890,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="57" t="s">
         <v>45</v>
       </c>
       <c r="B27" s="16" t="s">
@@ -1792,12 +1902,12 @@
       <c r="D27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="46" t="s">
+      <c r="E27" s="59" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
+      <c r="A28" s="57"/>
       <c r="B28" s="17" t="s">
         <v>19</v>
       </c>
@@ -1807,10 +1917,10 @@
       <c r="D28" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="46"/>
+      <c r="E28" s="59"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="44"/>
+      <c r="A29" s="57"/>
       <c r="B29" s="16" t="s">
         <v>19</v>
       </c>
@@ -1820,7 +1930,7 @@
       <c r="D29" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="46"/>
+      <c r="E29" s="59"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
@@ -1840,7 +1950,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="44" t="s">
+      <c r="A31" s="57" t="s">
         <v>53</v>
       </c>
       <c r="B31" s="15" t="s">
@@ -1852,12 +1962,12 @@
       <c r="D31" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="59" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="44"/>
+      <c r="A32" s="57"/>
       <c r="B32" s="14" t="s">
         <v>55</v>
       </c>
@@ -1867,56 +1977,56 @@
       <c r="D32" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="46"/>
+      <c r="E32" s="59"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="44"/>
+      <c r="A33" s="57"/>
       <c r="B33" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="48" t="s">
+      <c r="C33" s="60" t="s">
         <v>62</v>
       </c>
       <c r="D33" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="46"/>
+      <c r="E33" s="59"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="44"/>
+      <c r="A34" s="57"/>
       <c r="B34" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="48"/>
+      <c r="C34" s="60"/>
       <c r="D34" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="46"/>
+      <c r="E34" s="59"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="44"/>
+      <c r="A35" s="57"/>
       <c r="B35" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="48"/>
+      <c r="C35" s="60"/>
       <c r="D35" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E35" s="46"/>
+      <c r="E35" s="59"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="44"/>
+      <c r="A36" s="57"/>
       <c r="B36" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="48"/>
+      <c r="C36" s="60"/>
       <c r="D36" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="46"/>
+      <c r="E36" s="59"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="44"/>
+      <c r="A37" s="57"/>
       <c r="B37" s="15" t="s">
         <v>61</v>
       </c>
@@ -1926,10 +2036,10 @@
       <c r="D37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="46"/>
+      <c r="E37" s="59"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="44"/>
+      <c r="A38" s="57"/>
       <c r="B38" s="14" t="s">
         <v>63</v>
       </c>
@@ -1939,10 +2049,10 @@
       <c r="D38" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="46"/>
+      <c r="E38" s="59"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="44"/>
+      <c r="A39" s="57"/>
       <c r="B39" s="15" t="s">
         <v>64</v>
       </c>
@@ -1952,10 +2062,10 @@
       <c r="D39" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E39" s="46"/>
+      <c r="E39" s="59"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="44"/>
+      <c r="A40" s="57"/>
       <c r="B40" s="14" t="s">
         <v>65</v>
       </c>
@@ -1965,10 +2075,10 @@
       <c r="D40" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="46"/>
+      <c r="E40" s="59"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="44"/>
+      <c r="A41" s="57"/>
       <c r="B41" s="15" t="s">
         <v>66</v>
       </c>
@@ -1978,10 +2088,10 @@
       <c r="D41" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E41" s="46"/>
+      <c r="E41" s="59"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="44"/>
+      <c r="A42" s="57"/>
       <c r="B42" s="17" t="s">
         <v>19</v>
       </c>
@@ -1991,10 +2101,10 @@
       <c r="D42" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="46"/>
+      <c r="E42" s="59"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="44"/>
+      <c r="A43" s="57"/>
       <c r="B43" s="15" t="s">
         <v>68</v>
       </c>
@@ -2004,10 +2114,10 @@
       <c r="D43" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E43" s="46"/>
+      <c r="E43" s="59"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="43" t="s">
+      <c r="A44" s="56" t="s">
         <v>70</v>
       </c>
       <c r="B44" s="14" t="s">
@@ -2019,12 +2129,12 @@
       <c r="D44" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E44" s="47" t="s">
+      <c r="E44" s="54" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="43"/>
+      <c r="A45" s="56"/>
       <c r="B45" s="15" t="s">
         <v>72</v>
       </c>
@@ -2034,10 +2144,10 @@
       <c r="D45" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E45" s="47"/>
+      <c r="E45" s="54"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="43"/>
+      <c r="A46" s="56"/>
       <c r="B46" s="14" t="s">
         <v>73</v>
       </c>
@@ -2047,10 +2157,10 @@
       <c r="D46" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E46" s="47"/>
+      <c r="E46" s="54"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="43"/>
+      <c r="A47" s="56"/>
       <c r="B47" s="15" t="s">
         <v>74</v>
       </c>
@@ -2060,10 +2170,10 @@
       <c r="D47" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E47" s="47"/>
+      <c r="E47" s="54"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="43"/>
+      <c r="A48" s="56"/>
       <c r="B48" s="14" t="s">
         <v>75</v>
       </c>
@@ -2073,10 +2183,10 @@
       <c r="D48" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E48" s="47"/>
+      <c r="E48" s="54"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="43"/>
+      <c r="A49" s="56"/>
       <c r="B49" s="15" t="s">
         <v>76</v>
       </c>
@@ -2086,7 +2196,7 @@
       <c r="D49" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="47"/>
+      <c r="E49" s="54"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
@@ -2106,7 +2216,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="43" t="s">
+      <c r="A51" s="56" t="s">
         <v>79</v>
       </c>
       <c r="B51" s="15" t="s">
@@ -2118,12 +2228,12 @@
       <c r="D51" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E51" s="47" t="s">
+      <c r="E51" s="54" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="43"/>
+      <c r="A52" s="56"/>
       <c r="B52" s="14" t="s">
         <v>83</v>
       </c>
@@ -2133,10 +2243,10 @@
       <c r="D52" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E52" s="47"/>
+      <c r="E52" s="54"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="43"/>
+      <c r="A53" s="56"/>
       <c r="B53" s="15" t="s">
         <v>83</v>
       </c>
@@ -2146,10 +2256,10 @@
       <c r="D53" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E53" s="47"/>
+      <c r="E53" s="54"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="43"/>
+      <c r="A54" s="56"/>
       <c r="B54" s="14" t="s">
         <v>84</v>
       </c>
@@ -2159,10 +2269,10 @@
       <c r="D54" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E54" s="47"/>
+      <c r="E54" s="54"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="43"/>
+      <c r="A55" s="56"/>
       <c r="B55" s="15" t="s">
         <v>85</v>
       </c>
@@ -2172,10 +2282,10 @@
       <c r="D55" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E55" s="47"/>
+      <c r="E55" s="54"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="43"/>
+      <c r="A56" s="56"/>
       <c r="B56" s="14" t="s">
         <v>86</v>
       </c>
@@ -2185,10 +2295,10 @@
       <c r="D56" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E56" s="47"/>
+      <c r="E56" s="54"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="43"/>
+      <c r="A57" s="56"/>
       <c r="B57" s="15" t="s">
         <v>87</v>
       </c>
@@ -2198,10 +2308,10 @@
       <c r="D57" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E57" s="47"/>
+      <c r="E57" s="54"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="43"/>
+      <c r="A58" s="56"/>
       <c r="B58" s="14" t="s">
         <v>88</v>
       </c>
@@ -2211,10 +2321,10 @@
       <c r="D58" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E58" s="47"/>
+      <c r="E58" s="54"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="43"/>
+      <c r="A59" s="56"/>
       <c r="B59" s="15" t="s">
         <v>89</v>
       </c>
@@ -2224,10 +2334,10 @@
       <c r="D59" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E59" s="47"/>
+      <c r="E59" s="54"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="43"/>
+      <c r="A60" s="56"/>
       <c r="B60" s="14" t="s">
         <v>91</v>
       </c>
@@ -2237,7 +2347,7 @@
       <c r="D60" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E60" s="47"/>
+      <c r="E60" s="54"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
@@ -2257,7 +2367,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="43" t="s">
+      <c r="A62" s="56" t="s">
         <v>96</v>
       </c>
       <c r="B62" s="14" t="s">
@@ -2269,12 +2379,12 @@
       <c r="D62" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E62" s="47" t="s">
+      <c r="E62" s="54" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="43"/>
+      <c r="A63" s="56"/>
       <c r="B63" s="15" t="s">
         <v>98</v>
       </c>
@@ -2284,10 +2394,10 @@
       <c r="D63" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E63" s="47"/>
+      <c r="E63" s="54"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="43"/>
+      <c r="A64" s="56"/>
       <c r="B64" s="14" t="s">
         <v>99</v>
       </c>
@@ -2297,10 +2407,10 @@
       <c r="D64" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E64" s="47"/>
+      <c r="E64" s="54"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="43"/>
+      <c r="A65" s="56"/>
       <c r="B65" s="15" t="s">
         <v>100</v>
       </c>
@@ -2310,10 +2420,10 @@
       <c r="D65" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="47"/>
+      <c r="E65" s="54"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="43"/>
+      <c r="A66" s="56"/>
       <c r="B66" s="14" t="s">
         <v>101</v>
       </c>
@@ -2323,10 +2433,10 @@
       <c r="D66" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E66" s="47"/>
+      <c r="E66" s="54"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="43"/>
+      <c r="A67" s="56"/>
       <c r="B67" s="15" t="s">
         <v>102</v>
       </c>
@@ -2336,10 +2446,10 @@
       <c r="D67" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E67" s="47"/>
+      <c r="E67" s="54"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="43"/>
+      <c r="A68" s="56"/>
       <c r="B68" s="14" t="s">
         <v>103</v>
       </c>
@@ -2349,7 +2459,7 @@
       <c r="D68" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E68" s="47"/>
+      <c r="E68" s="54"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
@@ -2406,10 +2516,10 @@
       <c r="A72" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B72" s="49" t="s">
+      <c r="B72" s="61" t="s">
         <v>114</v>
       </c>
-      <c r="C72" s="48" t="s">
+      <c r="C72" s="60" t="s">
         <v>116</v>
       </c>
       <c r="D72" s="21" t="s">
@@ -2420,20 +2530,20 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="44" t="s">
+      <c r="A73" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="B73" s="49"/>
-      <c r="C73" s="48"/>
+      <c r="B73" s="61"/>
+      <c r="C73" s="60"/>
       <c r="D73" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E73" s="46" t="s">
+      <c r="E73" s="59" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="44"/>
+      <c r="A74" s="57"/>
       <c r="B74" s="29" t="s">
         <v>194</v>
       </c>
@@ -2443,10 +2553,10 @@
       <c r="D74" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E74" s="46"/>
+      <c r="E74" s="59"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="43" t="s">
+      <c r="A75" s="56" t="s">
         <v>112</v>
       </c>
       <c r="B75" s="22" t="s">
@@ -2458,12 +2568,12 @@
       <c r="D75" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E75" s="47" t="s">
+      <c r="E75" s="54" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="43"/>
+      <c r="A76" s="56"/>
       <c r="B76" s="15" t="s">
         <v>119</v>
       </c>
@@ -2473,10 +2583,10 @@
       <c r="D76" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E76" s="47"/>
+      <c r="E76" s="54"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="43"/>
+      <c r="A77" s="56"/>
       <c r="B77" s="14" t="s">
         <v>120</v>
       </c>
@@ -2486,10 +2596,10 @@
       <c r="D77" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E77" s="47"/>
+      <c r="E77" s="54"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="44" t="s">
+      <c r="A78" s="57" t="s">
         <v>121</v>
       </c>
       <c r="B78" s="15" t="s">
@@ -2501,12 +2611,12 @@
       <c r="D78" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E78" s="46" t="s">
+      <c r="E78" s="59" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="44"/>
+      <c r="A79" s="57"/>
       <c r="B79" s="14" t="s">
         <v>123</v>
       </c>
@@ -2516,10 +2626,10 @@
       <c r="D79" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E79" s="46"/>
+      <c r="E79" s="59"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="44"/>
+      <c r="A80" s="57"/>
       <c r="B80" s="15" t="s">
         <v>124</v>
       </c>
@@ -2529,10 +2639,10 @@
       <c r="D80" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E80" s="46"/>
+      <c r="E80" s="59"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="44"/>
+      <c r="A81" s="57"/>
       <c r="B81" s="14" t="s">
         <v>125</v>
       </c>
@@ -2542,7 +2652,7 @@
       <c r="D81" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E81" s="46"/>
+      <c r="E81" s="59"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="36" t="s">
@@ -2562,7 +2672,7 @@
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="44" t="s">
+      <c r="A83" s="57" t="s">
         <v>129</v>
       </c>
       <c r="B83" s="24" t="s">
@@ -2574,12 +2684,12 @@
       <c r="D83" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E83" s="46" t="s">
+      <c r="E83" s="59" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="44"/>
+      <c r="A84" s="57"/>
       <c r="B84" s="23" t="s">
         <v>132</v>
       </c>
@@ -2589,10 +2699,10 @@
       <c r="D84" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E84" s="46"/>
+      <c r="E84" s="59"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="43" t="s">
+      <c r="A85" s="56" t="s">
         <v>133</v>
       </c>
       <c r="B85" s="24" t="s">
@@ -2604,12 +2714,12 @@
       <c r="D85" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E85" s="47" t="s">
+      <c r="E85" s="54" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="43"/>
+      <c r="A86" s="56"/>
       <c r="B86" s="23" t="s">
         <v>135</v>
       </c>
@@ -2619,10 +2729,10 @@
       <c r="D86" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E86" s="47"/>
+      <c r="E86" s="54"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="43"/>
+      <c r="A87" s="56"/>
       <c r="B87" s="24" t="s">
         <v>136</v>
       </c>
@@ -2632,10 +2742,10 @@
       <c r="D87" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E87" s="47"/>
+      <c r="E87" s="54"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="43"/>
+      <c r="A88" s="56"/>
       <c r="B88" s="23" t="s">
         <v>137</v>
       </c>
@@ -2645,10 +2755,10 @@
       <c r="D88" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E88" s="47"/>
+      <c r="E88" s="54"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="43"/>
+      <c r="A89" s="56"/>
       <c r="B89" s="34" t="s">
         <v>19</v>
       </c>
@@ -2658,7 +2768,7 @@
       <c r="D89" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E89" s="47"/>
+      <c r="E89" s="54"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="37" t="s">
@@ -2712,7 +2822,7 @@
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="43" t="s">
+      <c r="A93" s="56" t="s">
         <v>148</v>
       </c>
       <c r="B93" s="24" t="s">
@@ -2724,12 +2834,12 @@
       <c r="D93" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E93" s="47" t="s">
+      <c r="E93" s="54" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="43"/>
+      <c r="A94" s="56"/>
       <c r="B94" s="23" t="s">
         <v>151</v>
       </c>
@@ -2739,10 +2849,10 @@
       <c r="D94" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E94" s="47"/>
+      <c r="E94" s="54"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="43"/>
+      <c r="A95" s="56"/>
       <c r="B95" s="24" t="s">
         <v>152</v>
       </c>
@@ -2752,10 +2862,10 @@
       <c r="D95" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E95" s="47"/>
+      <c r="E95" s="54"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="43"/>
+      <c r="A96" s="56"/>
       <c r="B96" s="23" t="s">
         <v>153</v>
       </c>
@@ -2765,10 +2875,10 @@
       <c r="D96" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E96" s="47"/>
+      <c r="E96" s="54"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="43"/>
+      <c r="A97" s="56"/>
       <c r="B97" s="24" t="s">
         <v>154</v>
       </c>
@@ -2778,10 +2888,10 @@
       <c r="D97" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E97" s="47"/>
+      <c r="E97" s="54"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="43"/>
+      <c r="A98" s="56"/>
       <c r="B98" s="23" t="s">
         <v>155</v>
       </c>
@@ -2791,10 +2901,10 @@
       <c r="D98" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E98" s="47"/>
+      <c r="E98" s="54"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="44" t="s">
+      <c r="A99" s="57" t="s">
         <v>156</v>
       </c>
       <c r="B99" s="24" t="s">
@@ -2806,12 +2916,12 @@
       <c r="D99" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E99" s="46" t="s">
+      <c r="E99" s="59" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="44"/>
+      <c r="A100" s="57"/>
       <c r="B100" s="23" t="s">
         <v>157</v>
       </c>
@@ -2821,10 +2931,10 @@
       <c r="D100" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E100" s="46"/>
+      <c r="E100" s="59"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="44"/>
+      <c r="A101" s="57"/>
       <c r="B101" s="24" t="s">
         <v>158</v>
       </c>
@@ -2834,10 +2944,10 @@
       <c r="D101" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E101" s="46"/>
+      <c r="E101" s="59"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="44"/>
+      <c r="A102" s="57"/>
       <c r="B102" s="23" t="s">
         <v>159</v>
       </c>
@@ -2847,10 +2957,10 @@
       <c r="D102" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E102" s="46"/>
+      <c r="E102" s="59"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="44"/>
+      <c r="A103" s="57"/>
       <c r="B103" s="24" t="s">
         <v>160</v>
       </c>
@@ -2860,10 +2970,10 @@
       <c r="D103" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E103" s="46"/>
+      <c r="E103" s="59"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="44"/>
+      <c r="A104" s="57"/>
       <c r="B104" s="35" t="s">
         <v>162</v>
       </c>
@@ -2873,10 +2983,10 @@
       <c r="D104" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E104" s="46"/>
+      <c r="E104" s="59"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="43" t="s">
+      <c r="A105" s="56" t="s">
         <v>169</v>
       </c>
       <c r="B105" s="24" t="s">
@@ -2888,12 +2998,12 @@
       <c r="D105" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E105" s="47" t="s">
+      <c r="E105" s="54" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="43"/>
+      <c r="A106" s="56"/>
       <c r="B106" s="23" t="s">
         <v>171</v>
       </c>
@@ -2903,10 +3013,10 @@
       <c r="D106" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E106" s="47"/>
+      <c r="E106" s="54"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="43"/>
+      <c r="A107" s="56"/>
       <c r="B107" s="24" t="s">
         <v>172</v>
       </c>
@@ -2916,10 +3026,10 @@
       <c r="D107" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E107" s="47"/>
+      <c r="E107" s="54"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="43"/>
+      <c r="A108" s="56"/>
       <c r="B108" s="23" t="s">
         <v>173</v>
       </c>
@@ -2929,7 +3039,7 @@
       <c r="D108" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E108" s="47"/>
+      <c r="E108" s="54"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="37" t="s">
@@ -2966,7 +3076,7 @@
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="50" t="s">
+      <c r="A111" s="62" t="s">
         <v>180</v>
       </c>
       <c r="B111" s="24" t="s">
@@ -2978,12 +3088,12 @@
       <c r="D111" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E111" s="46" t="s">
+      <c r="E111" s="59" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="50"/>
+      <c r="A112" s="62"/>
       <c r="B112" s="23" t="s">
         <v>182</v>
       </c>
@@ -2993,10 +3103,10 @@
       <c r="D112" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E112" s="46"/>
+      <c r="E112" s="59"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="51" t="s">
+      <c r="A113" s="53" t="s">
         <v>183</v>
       </c>
       <c r="B113" s="30" t="s">
@@ -3008,12 +3118,12 @@
       <c r="D113" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E113" s="47" t="s">
+      <c r="E113" s="54" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="51"/>
+      <c r="A114" s="53"/>
       <c r="B114" s="31" t="s">
         <v>186</v>
       </c>
@@ -3023,7 +3133,7 @@
       <c r="D114" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E114" s="47"/>
+      <c r="E114" s="54"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="39" t="s">
@@ -3043,7 +3153,7 @@
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="51" t="s">
+      <c r="A116" s="53" t="s">
         <v>189</v>
       </c>
       <c r="B116" s="31" t="s">
@@ -3055,12 +3165,12 @@
       <c r="D116" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E116" s="47" t="s">
+      <c r="E116" s="54" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" s="51"/>
+      <c r="A117" s="53"/>
       <c r="B117" s="24" t="s">
         <v>190</v>
       </c>
@@ -3070,10 +3180,10 @@
       <c r="D117" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E117" s="47"/>
+      <c r="E117" s="54"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="51"/>
+      <c r="A118" s="53"/>
       <c r="B118" s="31" t="s">
         <v>191</v>
       </c>
@@ -3083,10 +3193,10 @@
       <c r="D118" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E118" s="47"/>
+      <c r="E118" s="54"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="51"/>
+      <c r="A119" s="53"/>
       <c r="B119" s="24" t="s">
         <v>192</v>
       </c>
@@ -3096,10 +3206,10 @@
       <c r="D119" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E119" s="47"/>
+      <c r="E119" s="54"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" s="51"/>
+      <c r="A120" s="53"/>
       <c r="B120" s="31" t="s">
         <v>193</v>
       </c>
@@ -3109,7 +3219,7 @@
       <c r="D120" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E120" s="47"/>
+      <c r="E120" s="54"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="39" t="s">
@@ -3141,7 +3251,7 @@
       <c r="D122" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E122" s="52" t="s">
+      <c r="E122" s="42" t="s">
         <v>198</v>
       </c>
     </row>
@@ -3160,7 +3270,7 @@
       <c r="E124" s="33"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" s="50" t="s">
+      <c r="A125" s="62" t="s">
         <v>200</v>
       </c>
       <c r="B125" s="24" t="s">
@@ -3172,12 +3282,12 @@
       <c r="D125" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E125" s="46" t="s">
+      <c r="E125" s="59" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="50"/>
+      <c r="A126" s="62"/>
       <c r="B126" s="31" t="s">
         <v>203</v>
       </c>
@@ -3187,10 +3297,10 @@
       <c r="D126" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E126" s="46"/>
+      <c r="E126" s="59"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" s="50"/>
+      <c r="A127" s="62"/>
       <c r="B127" s="24" t="s">
         <v>204</v>
       </c>
@@ -3200,10 +3310,10 @@
       <c r="D127" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E127" s="46"/>
+      <c r="E127" s="59"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" s="50"/>
+      <c r="A128" s="62"/>
       <c r="B128" s="31" t="s">
         <v>205</v>
       </c>
@@ -3213,10 +3323,10 @@
       <c r="D128" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E128" s="46"/>
+      <c r="E128" s="59"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" s="50"/>
+      <c r="A129" s="62"/>
       <c r="B129" s="24" t="s">
         <v>206</v>
       </c>
@@ -3226,10 +3336,10 @@
       <c r="D129" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E129" s="46"/>
+      <c r="E129" s="59"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" s="50"/>
+      <c r="A130" s="62"/>
       <c r="B130" s="31" t="s">
         <v>207</v>
       </c>
@@ -3239,7 +3349,7 @@
       <c r="D130" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E130" s="46"/>
+      <c r="E130" s="59"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="40" t="s">
@@ -3259,7 +3369,7 @@
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" s="50" t="s">
+      <c r="A132" s="62" t="s">
         <v>217</v>
       </c>
       <c r="B132" s="31" t="s">
@@ -3271,12 +3381,12 @@
       <c r="D132" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="E132" s="46" t="s">
+      <c r="E132" s="59" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" s="50"/>
+      <c r="A133" s="62"/>
       <c r="B133" s="24" t="s">
         <v>218</v>
       </c>
@@ -3286,10 +3396,10 @@
       <c r="D133" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E133" s="46"/>
+      <c r="E133" s="59"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" s="50"/>
+      <c r="A134" s="62"/>
       <c r="B134" s="31" t="s">
         <v>220</v>
       </c>
@@ -3299,20 +3409,20 @@
       <c r="D134" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E134" s="46"/>
+      <c r="E134" s="59"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" s="50"/>
+      <c r="A135" s="62"/>
       <c r="B135" s="14" t="s">
         <v>221</v>
       </c>
       <c r="C135" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="D135" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="E135" s="46"/>
+      <c r="D135" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E135" s="59"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="40" t="s">
@@ -3327,12 +3437,12 @@
       <c r="D136" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E136" s="53" t="s">
+      <c r="E136" s="43" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" s="54" t="s">
+      <c r="A137" s="44" t="s">
         <v>227</v>
       </c>
       <c r="B137" s="14" t="s">
@@ -3341,60 +3451,950 @@
       <c r="C137" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D137" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="E137" s="54" t="s">
+      <c r="D137" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E137" s="44" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" s="40"/>
-      <c r="B138" s="31"/>
-      <c r="C138" s="6"/>
+      <c r="A138" s="49" t="s">
+        <v>229</v>
+      </c>
+      <c r="B138" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="C138" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="D138" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E138" s="53"/>
+      <c r="E138" s="50" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" s="54"/>
-      <c r="B139" s="14"/>
-      <c r="C139" s="7"/>
-      <c r="D139" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="E139" s="54"/>
+      <c r="A139" s="49"/>
+      <c r="B139" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="C139" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="D139" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E139" s="50"/>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" s="40"/>
-      <c r="B140" s="31"/>
-      <c r="C140" s="6"/>
+      <c r="A140" s="49"/>
+      <c r="B140" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="C140" s="6" t="s">
+        <v>201</v>
+      </c>
       <c r="D140" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E140" s="53"/>
+      <c r="E140" s="50"/>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" s="54"/>
-      <c r="B141" s="14"/>
-      <c r="C141" s="7"/>
-      <c r="D141" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="E141" s="54"/>
+      <c r="A141" s="49"/>
+      <c r="B141" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C141" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D141" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E141" s="50"/>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A142" s="40"/>
-      <c r="B142" s="31"/>
-      <c r="C142" s="6"/>
-      <c r="D142" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E142" s="53"/>
+      <c r="A142" s="51" t="s">
+        <v>234</v>
+      </c>
+      <c r="B142" s="35" t="s">
+        <v>236</v>
+      </c>
+      <c r="C142" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="D142" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E142" s="52" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="51"/>
+      <c r="B143" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="C143" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D143" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E143" s="52"/>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="51"/>
+      <c r="B144" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="C144" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E144" s="52"/>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="51"/>
+      <c r="B145" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="C145" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="D145" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E145" s="52"/>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="51"/>
+      <c r="B146" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="C146" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E146" s="52"/>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="B147" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="C147" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D147" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E147" s="54" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="53"/>
+      <c r="B148" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="C148" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E148" s="54"/>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="53"/>
+      <c r="B149" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="C149" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="D149" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E149" s="54"/>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="53"/>
+      <c r="B150" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="C150" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E150" s="54"/>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="53"/>
+      <c r="B151" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="C151" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="D151" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E151" s="54"/>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="53"/>
+      <c r="B152" s="31" t="s">
+        <v>252</v>
+      </c>
+      <c r="C152" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E152" s="54"/>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="53"/>
+      <c r="B153" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="C153" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="D153" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E153" s="54"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="53"/>
+      <c r="B154" s="31" t="s">
+        <v>254</v>
+      </c>
+      <c r="C154" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E154" s="54"/>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="53"/>
+      <c r="B155" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="C155" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="D155" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E155" s="54"/>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="53"/>
+      <c r="B156" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="C156" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E156" s="54"/>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="53"/>
+      <c r="B157" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C157" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="D157" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E157" s="54"/>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="53"/>
+      <c r="B158" s="35" t="s">
+        <v>162</v>
+      </c>
+      <c r="C158" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E158" s="54"/>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="53"/>
+      <c r="B159" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C159" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="D159" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E159" s="54"/>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="41"/>
+      <c r="B160" s="31"/>
+      <c r="C160" s="6"/>
+      <c r="D160" s="2"/>
+      <c r="E160" s="46"/>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="47"/>
+      <c r="B161" s="14"/>
+      <c r="C161" s="7"/>
+      <c r="D161" s="45"/>
+      <c r="E161" s="47"/>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="41"/>
+      <c r="B162" s="31"/>
+      <c r="C162" s="6"/>
+      <c r="D162" s="2"/>
+      <c r="E162" s="46"/>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="47"/>
+      <c r="B163" s="14"/>
+      <c r="C163" s="7"/>
+      <c r="D163" s="45"/>
+      <c r="E163" s="47"/>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="41"/>
+      <c r="B164" s="31"/>
+      <c r="C164" s="6"/>
+      <c r="D164" s="2"/>
+      <c r="E164" s="46"/>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="47"/>
+      <c r="B165" s="14"/>
+      <c r="C165" s="7"/>
+      <c r="D165" s="45"/>
+      <c r="E165" s="47"/>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="41"/>
+      <c r="B166" s="31"/>
+      <c r="C166" s="6"/>
+      <c r="D166" s="2"/>
+      <c r="E166" s="46"/>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="47"/>
+      <c r="B167" s="14"/>
+      <c r="C167" s="7"/>
+      <c r="D167" s="45"/>
+      <c r="E167" s="47"/>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="41"/>
+      <c r="B168" s="31"/>
+      <c r="C168" s="6"/>
+      <c r="D168" s="2"/>
+      <c r="E168" s="46"/>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="47"/>
+      <c r="B169" s="14"/>
+      <c r="C169" s="7"/>
+      <c r="D169" s="45"/>
+      <c r="E169" s="47"/>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="41"/>
+      <c r="B170" s="31"/>
+      <c r="C170" s="6"/>
+      <c r="D170" s="2"/>
+      <c r="E170" s="46"/>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="47"/>
+      <c r="B171" s="14"/>
+      <c r="C171" s="7"/>
+      <c r="D171" s="45"/>
+      <c r="E171" s="47"/>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="41"/>
+      <c r="B172" s="31"/>
+      <c r="C172" s="6"/>
+      <c r="D172" s="2"/>
+      <c r="E172" s="46"/>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="47"/>
+      <c r="B173" s="14"/>
+      <c r="C173" s="7"/>
+      <c r="D173" s="45"/>
+      <c r="E173" s="47"/>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="41"/>
+      <c r="B174" s="31"/>
+      <c r="C174" s="6"/>
+      <c r="D174" s="2"/>
+      <c r="E174" s="46"/>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="47"/>
+      <c r="B175" s="14"/>
+      <c r="C175" s="7"/>
+      <c r="D175" s="45"/>
+      <c r="E175" s="47"/>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="41"/>
+      <c r="B176" s="31"/>
+      <c r="C176" s="6"/>
+      <c r="D176" s="2"/>
+      <c r="E176" s="46"/>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="47"/>
+      <c r="B177" s="14"/>
+      <c r="C177" s="7"/>
+      <c r="D177" s="45"/>
+      <c r="E177" s="47"/>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="41"/>
+      <c r="B178" s="31"/>
+      <c r="C178" s="6"/>
+      <c r="D178" s="2"/>
+      <c r="E178" s="46"/>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="47"/>
+      <c r="B179" s="14"/>
+      <c r="C179" s="7"/>
+      <c r="D179" s="45"/>
+      <c r="E179" s="47"/>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="41"/>
+      <c r="B180" s="31"/>
+      <c r="C180" s="6"/>
+      <c r="D180" s="2"/>
+      <c r="E180" s="46"/>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="47"/>
+      <c r="B181" s="14"/>
+      <c r="C181" s="7"/>
+      <c r="D181" s="45"/>
+      <c r="E181" s="47"/>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="41"/>
+      <c r="B182" s="31"/>
+      <c r="C182" s="6"/>
+      <c r="D182" s="2"/>
+      <c r="E182" s="46"/>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="47"/>
+      <c r="B183" s="14"/>
+      <c r="C183" s="7"/>
+      <c r="D183" s="45"/>
+      <c r="E183" s="47"/>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="41"/>
+      <c r="B184" s="31"/>
+      <c r="C184" s="6"/>
+      <c r="D184" s="2"/>
+      <c r="E184" s="46"/>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="47"/>
+      <c r="B185" s="14"/>
+      <c r="C185" s="7"/>
+      <c r="D185" s="45"/>
+      <c r="E185" s="47"/>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="41"/>
+      <c r="B186" s="31"/>
+      <c r="C186" s="6"/>
+      <c r="D186" s="2"/>
+      <c r="E186" s="46"/>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="47"/>
+      <c r="B187" s="14"/>
+      <c r="C187" s="7"/>
+      <c r="D187" s="45"/>
+      <c r="E187" s="47"/>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="41"/>
+      <c r="B188" s="31"/>
+      <c r="C188" s="6"/>
+      <c r="D188" s="2"/>
+      <c r="E188" s="46"/>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="47"/>
+      <c r="B189" s="14"/>
+      <c r="C189" s="7"/>
+      <c r="D189" s="45"/>
+      <c r="E189" s="47"/>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="41"/>
+      <c r="B190" s="31"/>
+      <c r="C190" s="6"/>
+      <c r="D190" s="2"/>
+      <c r="E190" s="46"/>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="47"/>
+      <c r="B191" s="14"/>
+      <c r="C191" s="7"/>
+      <c r="D191" s="45"/>
+      <c r="E191" s="47"/>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="41"/>
+      <c r="B192" s="31"/>
+      <c r="C192" s="6"/>
+      <c r="D192" s="2"/>
+      <c r="E192" s="46"/>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="47"/>
+      <c r="B193" s="14"/>
+      <c r="C193" s="7"/>
+      <c r="D193" s="45"/>
+      <c r="E193" s="47"/>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="41"/>
+      <c r="B194" s="31"/>
+      <c r="C194" s="6"/>
+      <c r="D194" s="2"/>
+      <c r="E194" s="46"/>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="47"/>
+      <c r="B195" s="14"/>
+      <c r="C195" s="7"/>
+      <c r="D195" s="45"/>
+      <c r="E195" s="47"/>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="41"/>
+      <c r="B196" s="31"/>
+      <c r="C196" s="6"/>
+      <c r="D196" s="2"/>
+      <c r="E196" s="46"/>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="47"/>
+      <c r="B197" s="14"/>
+      <c r="C197" s="7"/>
+      <c r="D197" s="45"/>
+      <c r="E197" s="47"/>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="41"/>
+      <c r="B198" s="31"/>
+      <c r="C198" s="6"/>
+      <c r="D198" s="2"/>
+      <c r="E198" s="46"/>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="47"/>
+      <c r="B199" s="14"/>
+      <c r="C199" s="7"/>
+      <c r="D199" s="45"/>
+      <c r="E199" s="47"/>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="41"/>
+      <c r="B200" s="31"/>
+      <c r="C200" s="6"/>
+      <c r="D200" s="2"/>
+      <c r="E200" s="46"/>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="47"/>
+      <c r="B201" s="14"/>
+      <c r="C201" s="7"/>
+      <c r="D201" s="45"/>
+      <c r="E201" s="47"/>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="41"/>
+      <c r="B202" s="31"/>
+      <c r="C202" s="6"/>
+      <c r="D202" s="2"/>
+      <c r="E202" s="46"/>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="47"/>
+      <c r="B203" s="14"/>
+      <c r="C203" s="7"/>
+      <c r="D203" s="45"/>
+      <c r="E203" s="47"/>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="41"/>
+      <c r="B204" s="31"/>
+      <c r="C204" s="6"/>
+      <c r="D204" s="2"/>
+      <c r="E204" s="46"/>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="47"/>
+      <c r="B205" s="14"/>
+      <c r="C205" s="7"/>
+      <c r="D205" s="45"/>
+      <c r="E205" s="47"/>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="41"/>
+      <c r="B206" s="31"/>
+      <c r="C206" s="6"/>
+      <c r="D206" s="2"/>
+      <c r="E206" s="46"/>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="47"/>
+      <c r="B207" s="14"/>
+      <c r="C207" s="7"/>
+      <c r="D207" s="45"/>
+      <c r="E207" s="47"/>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="41"/>
+      <c r="B208" s="31"/>
+      <c r="C208" s="6"/>
+      <c r="D208" s="2"/>
+      <c r="E208" s="46"/>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="47"/>
+      <c r="B209" s="14"/>
+      <c r="C209" s="7"/>
+      <c r="D209" s="45"/>
+      <c r="E209" s="47"/>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="41"/>
+      <c r="B210" s="31"/>
+      <c r="C210" s="6"/>
+      <c r="D210" s="2"/>
+      <c r="E210" s="46"/>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="47"/>
+      <c r="B211" s="14"/>
+      <c r="C211" s="7"/>
+      <c r="D211" s="45"/>
+      <c r="E211" s="47"/>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" s="41"/>
+      <c r="B212" s="31"/>
+      <c r="C212" s="6"/>
+      <c r="D212" s="2"/>
+      <c r="E212" s="46"/>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="47"/>
+      <c r="B213" s="14"/>
+      <c r="C213" s="7"/>
+      <c r="D213" s="45"/>
+      <c r="E213" s="47"/>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="41"/>
+      <c r="B214" s="31"/>
+      <c r="C214" s="6"/>
+      <c r="D214" s="2"/>
+      <c r="E214" s="46"/>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="47"/>
+      <c r="B215" s="14"/>
+      <c r="C215" s="7"/>
+      <c r="D215" s="45"/>
+      <c r="E215" s="47"/>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="41"/>
+      <c r="B216" s="31"/>
+      <c r="C216" s="6"/>
+      <c r="D216" s="2"/>
+      <c r="E216" s="46"/>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="47"/>
+      <c r="B217" s="14"/>
+      <c r="C217" s="7"/>
+      <c r="D217" s="45"/>
+      <c r="E217" s="47"/>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="41"/>
+      <c r="B218" s="31"/>
+      <c r="C218" s="6"/>
+      <c r="D218" s="2"/>
+      <c r="E218" s="46"/>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="47"/>
+      <c r="B219" s="14"/>
+      <c r="C219" s="7"/>
+      <c r="D219" s="45"/>
+      <c r="E219" s="47"/>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="41"/>
+      <c r="B220" s="31"/>
+      <c r="C220" s="6"/>
+      <c r="D220" s="2"/>
+      <c r="E220" s="46"/>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="47"/>
+      <c r="B221" s="14"/>
+      <c r="C221" s="7"/>
+      <c r="D221" s="45"/>
+      <c r="E221" s="47"/>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="41"/>
+      <c r="B222" s="31"/>
+      <c r="C222" s="6"/>
+      <c r="D222" s="2"/>
+      <c r="E222" s="46"/>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="47"/>
+      <c r="B223" s="14"/>
+      <c r="C223" s="7"/>
+      <c r="D223" s="45"/>
+      <c r="E223" s="47"/>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="41"/>
+      <c r="B224" s="31"/>
+      <c r="C224" s="6"/>
+      <c r="D224" s="2"/>
+      <c r="E224" s="46"/>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="47"/>
+      <c r="B225" s="14"/>
+      <c r="C225" s="7"/>
+      <c r="D225" s="45"/>
+      <c r="E225" s="47"/>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" s="41"/>
+      <c r="B226" s="31"/>
+      <c r="C226" s="6"/>
+      <c r="D226" s="2"/>
+      <c r="E226" s="46"/>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="47"/>
+      <c r="B227" s="14"/>
+      <c r="C227" s="7"/>
+      <c r="D227" s="45"/>
+      <c r="E227" s="47"/>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="41"/>
+      <c r="B228" s="31"/>
+      <c r="C228" s="6"/>
+      <c r="D228" s="2"/>
+      <c r="E228" s="46"/>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="47"/>
+      <c r="B229" s="14"/>
+      <c r="C229" s="7"/>
+      <c r="D229" s="45"/>
+      <c r="E229" s="47"/>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="41"/>
+      <c r="B230" s="31"/>
+      <c r="C230" s="6"/>
+      <c r="D230" s="2"/>
+      <c r="E230" s="46"/>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="47"/>
+      <c r="B231" s="14"/>
+      <c r="C231" s="7"/>
+      <c r="D231" s="45"/>
+      <c r="E231" s="47"/>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="41"/>
+      <c r="B232" s="31"/>
+      <c r="C232" s="6"/>
+      <c r="D232" s="2"/>
+      <c r="E232" s="46"/>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="47"/>
+      <c r="B233" s="14"/>
+      <c r="C233" s="7"/>
+      <c r="D233" s="45"/>
+      <c r="E233" s="47"/>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" s="41"/>
+      <c r="B234" s="31"/>
+      <c r="C234" s="6"/>
+      <c r="D234" s="2"/>
+      <c r="E234" s="46"/>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" s="47"/>
+      <c r="B235" s="14"/>
+      <c r="C235" s="7"/>
+      <c r="D235" s="45"/>
+      <c r="E235" s="47"/>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" s="41"/>
+      <c r="B236" s="31"/>
+      <c r="C236" s="6"/>
+      <c r="D236" s="2"/>
+      <c r="E236" s="46"/>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" s="47"/>
+      <c r="B237" s="14"/>
+      <c r="C237" s="7"/>
+      <c r="D237" s="45"/>
+      <c r="E237" s="47"/>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" s="41"/>
+      <c r="B238" s="31"/>
+      <c r="C238" s="6"/>
+      <c r="D238" s="2"/>
+      <c r="E238" s="46"/>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" s="47"/>
+      <c r="B239" s="14"/>
+      <c r="C239" s="7"/>
+      <c r="D239" s="45"/>
+      <c r="E239" s="47"/>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" s="41"/>
+      <c r="B240" s="31"/>
+      <c r="C240" s="6"/>
+      <c r="D240" s="2"/>
+      <c r="E240" s="46"/>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" s="47"/>
+      <c r="B241" s="14"/>
+      <c r="C241" s="7"/>
+      <c r="D241" s="45"/>
+      <c r="E241" s="47"/>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" s="41"/>
+      <c r="B242" s="31"/>
+      <c r="C242" s="6"/>
+      <c r="D242" s="2"/>
+      <c r="E242" s="46"/>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" s="47"/>
+      <c r="B243" s="14"/>
+      <c r="C243" s="7"/>
+      <c r="D243" s="45"/>
+      <c r="E243" s="47"/>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" s="41"/>
+      <c r="B244" s="31"/>
+      <c r="C244" s="6"/>
+      <c r="D244" s="2"/>
+      <c r="E244" s="46"/>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" s="47"/>
+      <c r="B245" s="14"/>
+      <c r="C245" s="7"/>
+      <c r="D245" s="45"/>
+      <c r="E245" s="47"/>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A246" s="41"/>
+      <c r="B246" s="31"/>
+      <c r="C246" s="6"/>
+      <c r="D246" s="2"/>
+      <c r="E246" s="46"/>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A247" s="47"/>
+      <c r="B247" s="14"/>
+      <c r="C247" s="7"/>
+      <c r="D247" s="45"/>
+      <c r="E247" s="47"/>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A248" s="41"/>
+      <c r="B248" s="31"/>
+      <c r="C248" s="6"/>
+      <c r="D248" s="2"/>
+      <c r="E248" s="46"/>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A249" s="47"/>
+      <c r="B249" s="14"/>
+      <c r="C249" s="7"/>
+      <c r="D249" s="45"/>
+      <c r="E249" s="47"/>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A250" s="41"/>
+      <c r="B250" s="31"/>
+      <c r="C250" s="6"/>
+      <c r="D250" s="2"/>
+      <c r="E250" s="46"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
+  <mergeCells count="50">
     <mergeCell ref="A132:A135"/>
     <mergeCell ref="E132:E135"/>
     <mergeCell ref="A125:A130"/>
@@ -3439,6 +4439,12 @@
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="A31:A43"/>
+    <mergeCell ref="A138:A141"/>
+    <mergeCell ref="E138:E141"/>
+    <mergeCell ref="A142:A146"/>
+    <mergeCell ref="E142:E146"/>
+    <mergeCell ref="A147:A159"/>
+    <mergeCell ref="E147:E159"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{D01E85B4-1DB0-475A-87DE-364916E7DA22}"/>

</xml_diff>